<commit_message>
Aggiornamento per allineamento env/svia
</commit_message>
<xml_diff>
--- a/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
+++ b/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openshift\SoftwareAllineamenti\src\main\resources\excelutils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D03EF63-7712-47E6-AC16-8B785C9169B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD3CEBF-7914-43DC-8555-242F312FA979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
+    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="15990" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Versioni EJB" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="140">
   <si>
     <t>isp-ib-om</t>
   </si>
@@ -366,97 +366,97 @@
     <t>VERSIONE SVIS/SVIA</t>
   </si>
   <si>
-    <t>1.8.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.5.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.7.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.6.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.48.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.24.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.10.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.12.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.9.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.14.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.11.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>0.30.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.19.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>Mettere l'Ignore nella classi di test per ridurre i tempi di build</t>
-  </si>
-  <si>
-    <t>1.39.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.20.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.15.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.16.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.51.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.22.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.70.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.27.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.40.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.47.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.201.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.136.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.30.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.120.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.38.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.13.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.69.0-env-svis-SNAPSHOT</t>
+    <t>1.8.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.5.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.7.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.6.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.48.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.24.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.10.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.12.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.9.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.14.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.11.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>0.30.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.19.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.13.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.39.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.20.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.15.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.17.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.52.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.22.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.70.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.16.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.27.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.40.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.47.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.201.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.136.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.30.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.120.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.38.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.69.0-env-svia-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1006,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>4</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" t="s">
         <v>12</v>
@@ -1026,7 +1026,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" t="s">
         <v>13</v>
@@ -1035,7 +1035,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" t="s">
         <v>14</v>
@@ -1044,7 +1044,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" t="s">
         <v>15</v>
@@ -1052,11 +1052,8 @@
       <c r="C21" t="s">
         <v>116</v>
       </c>
-      <c r="D21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" t="s">
         <v>16</v>
@@ -1065,7 +1062,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>17</v>
@@ -1074,7 +1071,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" t="s">
         <v>18</v>
@@ -1083,7 +1080,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" t="s">
         <v>19</v>
@@ -1092,7 +1089,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" t="s">
         <v>20</v>
@@ -1101,7 +1098,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" t="s">
         <v>21</v>
@@ -1110,7 +1107,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
         <v>22</v>
@@ -1119,7 +1116,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
         <v>23</v>
@@ -1128,7 +1125,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" t="s">
         <v>24</v>
@@ -1137,7 +1134,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>25</v>
@@ -1146,7 +1143,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
         <v>26</v>
@@ -1179,7 +1176,7 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,7 +1238,7 @@
         <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1505,7 +1502,7 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1567,7 +1564,7 @@
         <v>65</v>
       </c>
       <c r="C79" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1576,7 +1573,7 @@
         <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1594,7 +1591,7 @@
         <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1637,7 +1634,7 @@
         <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1654,7 +1651,7 @@
         <v>72</v>
       </c>
       <c r="C89" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1689,7 +1686,7 @@
         <v>75</v>
       </c>
       <c r="C93" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1698,7 +1695,7 @@
         <v>76</v>
       </c>
       <c r="C94" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -1707,7 +1704,7 @@
         <v>77</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1751,7 +1748,7 @@
         <v>81</v>
       </c>
       <c r="C100" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -1793,11 +1790,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD315DD5-8851-4C46-8B35-757CD3C08EC5}">
-  <dimension ref="A1:D511"/>
+  <dimension ref="A1:D510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E386" sqref="E386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1849,7 +1846,7 @@
       </c>
       <c r="C5" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="6" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1866,7 +1863,7 @@
       </c>
       <c r="C7" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="8" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1897,7 +1894,7 @@
       </c>
       <c r="C11" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="12" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1914,7 +1911,7 @@
       </c>
       <c r="C13" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="14" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1938,7 +1935,7 @@
       </c>
       <c r="C16" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="17" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1948,7 +1945,7 @@
       </c>
       <c r="C17" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="18" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -1965,7 +1962,7 @@
       </c>
       <c r="C19" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="20" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1975,7 +1972,7 @@
       </c>
       <c r="C20" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="21" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -1992,7 +1989,7 @@
       </c>
       <c r="C22" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="23" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2002,7 +1999,7 @@
       </c>
       <c r="C23" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="24" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2026,7 +2023,7 @@
       </c>
       <c r="C26" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="27" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2036,7 +2033,7 @@
       </c>
       <c r="C27" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="28" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2046,7 +2043,7 @@
       </c>
       <c r="C28" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="29" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2056,7 +2053,7 @@
       </c>
       <c r="C29" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="30" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2080,7 +2077,7 @@
       </c>
       <c r="C32" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="33" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2090,7 +2087,7 @@
       </c>
       <c r="C33" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="34" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2100,7 +2097,7 @@
       </c>
       <c r="C34" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="35" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2110,7 +2107,7 @@
       </c>
       <c r="C35" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="36" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2120,7 +2117,7 @@
       </c>
       <c r="C36" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="37" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2137,7 +2134,7 @@
       </c>
       <c r="C38" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="39" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2147,7 +2144,7 @@
       </c>
       <c r="C39" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="40" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2157,7 +2154,7 @@
       </c>
       <c r="C40" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="41" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2167,7 +2164,7 @@
       </c>
       <c r="C41" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="42" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2184,7 +2181,7 @@
       </c>
       <c r="C43" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="44" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2194,7 +2191,7 @@
       </c>
       <c r="C44" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="45" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2204,7 +2201,7 @@
       </c>
       <c r="C45" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="46" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2221,7 +2218,7 @@
       </c>
       <c r="C47" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2231,7 +2228,7 @@
       </c>
       <c r="C48" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="49" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2241,7 +2238,7 @@
       </c>
       <c r="C49" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="50" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2258,7 +2255,7 @@
       </c>
       <c r="C51" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="52" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2268,7 +2265,7 @@
       </c>
       <c r="C52" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="53" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2278,7 +2275,7 @@
       </c>
       <c r="C53" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="54" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2295,7 +2292,7 @@
       </c>
       <c r="C55" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="56" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2305,7 +2302,7 @@
       </c>
       <c r="C56" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="57" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2322,7 +2319,7 @@
       </c>
       <c r="C58" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="59" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2332,7 +2329,7 @@
       </c>
       <c r="C59" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="60" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2342,7 +2339,7 @@
       </c>
       <c r="C60" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="61" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2352,7 +2349,7 @@
       </c>
       <c r="C61" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="62" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2362,7 +2359,7 @@
       </c>
       <c r="C62" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="63" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2387,7 +2384,7 @@
       </c>
       <c r="C65" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="66" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2397,7 +2394,7 @@
       </c>
       <c r="C66" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="67" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2407,7 +2404,7 @@
       </c>
       <c r="C67" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="68" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2424,7 +2421,7 @@
       </c>
       <c r="C69" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="70" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2434,7 +2431,7 @@
       </c>
       <c r="C70" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="71" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2451,7 +2448,7 @@
       </c>
       <c r="C72" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="73" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2461,7 +2458,7 @@
       </c>
       <c r="C73" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="74" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2478,7 +2475,7 @@
       </c>
       <c r="C75" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="76" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2488,7 +2485,7 @@
       </c>
       <c r="C76" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="77" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2505,7 +2502,7 @@
       </c>
       <c r="C78" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="79" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2515,7 +2512,7 @@
       </c>
       <c r="C79" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="80" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2532,7 +2529,7 @@
       </c>
       <c r="C81" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="82" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2542,7 +2539,7 @@
       </c>
       <c r="C82" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="83" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2559,7 +2556,7 @@
       </c>
       <c r="C84" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="85" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2569,7 +2566,7 @@
       </c>
       <c r="C85" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="86" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2586,7 +2583,7 @@
       </c>
       <c r="C87" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="88" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2596,7 +2593,7 @@
       </c>
       <c r="C88" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="89" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2613,7 +2610,7 @@
       </c>
       <c r="C90" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="91" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2623,7 +2620,7 @@
       </c>
       <c r="C91" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="92" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2640,7 +2637,7 @@
       </c>
       <c r="C93" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="94" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2650,7 +2647,7 @@
       </c>
       <c r="C94" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="95" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2675,7 +2672,7 @@
       </c>
       <c r="C97" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="98" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2685,7 +2682,7 @@
       </c>
       <c r="C98" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="99" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2695,7 +2692,7 @@
       </c>
       <c r="C99" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="100" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2705,7 +2702,7 @@
       </c>
       <c r="C100" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="101" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2722,7 +2719,7 @@
       </c>
       <c r="C102" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="103" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2732,7 +2729,7 @@
       </c>
       <c r="C103" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="104" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2742,7 +2739,7 @@
       </c>
       <c r="C104" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="105" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2752,7 +2749,7 @@
       </c>
       <c r="C105" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="106" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2769,7 +2766,7 @@
       </c>
       <c r="C107" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="108" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2779,7 +2776,7 @@
       </c>
       <c r="C108" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="109" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2789,7 +2786,7 @@
       </c>
       <c r="C109" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="110" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2799,7 +2796,7 @@
       </c>
       <c r="C110" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="111" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2809,7 +2806,7 @@
       </c>
       <c r="C111" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="112" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2819,7 +2816,7 @@
       </c>
       <c r="C112" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="113" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2836,7 +2833,7 @@
       </c>
       <c r="C114" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="115" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2846,7 +2843,7 @@
       </c>
       <c r="C115" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="116" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2856,7 +2853,7 @@
       </c>
       <c r="C116" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="117" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2866,7 +2863,7 @@
       </c>
       <c r="C117" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="118" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2876,7 +2873,7 @@
       </c>
       <c r="C118" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="119" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2900,7 +2897,7 @@
       </c>
       <c r="C121" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="122" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2910,7 +2907,7 @@
       </c>
       <c r="C122" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="123" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2920,7 +2917,7 @@
       </c>
       <c r="C123" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="124" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2930,7 +2927,7 @@
       </c>
       <c r="C124" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="125" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2940,7 +2937,7 @@
       </c>
       <c r="C125" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="126" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2957,7 +2954,7 @@
       </c>
       <c r="C127" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="128" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2967,7 +2964,7 @@
       </c>
       <c r="C128" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2985,7 +2982,7 @@
       </c>
       <c r="C130" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="131" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2995,7 +2992,7 @@
       </c>
       <c r="C131" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="132" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3012,7 +3009,7 @@
       </c>
       <c r="C133" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="134" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3022,7 +3019,7 @@
       </c>
       <c r="C134" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="135" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3039,7 +3036,7 @@
       </c>
       <c r="C136" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="137" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3049,7 +3046,7 @@
       </c>
       <c r="C137" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="138" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3059,7 +3056,7 @@
       </c>
       <c r="C138" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="139" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3077,7 +3074,7 @@
       </c>
       <c r="C140" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="141" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3102,7 +3099,7 @@
       </c>
       <c r="C143" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="144" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3112,7 +3109,7 @@
       </c>
       <c r="C144" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="145" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3122,7 +3119,7 @@
       </c>
       <c r="C145" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="146" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3139,7 +3136,7 @@
       </c>
       <c r="C147" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="148" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3149,7 +3146,7 @@
       </c>
       <c r="C148" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="149" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3159,7 +3156,7 @@
       </c>
       <c r="C149" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="150" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3169,7 +3166,7 @@
       </c>
       <c r="C150" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="151" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3193,7 +3190,7 @@
       </c>
       <c r="C153" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="154" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3203,7 +3200,7 @@
       </c>
       <c r="C154" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="155" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3213,7 +3210,7 @@
       </c>
       <c r="C155" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="156" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3223,7 +3220,7 @@
       </c>
       <c r="C156" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="157" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3240,7 +3237,7 @@
       </c>
       <c r="C158" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="159" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3247,7 @@
       </c>
       <c r="C159" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="160" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3260,7 +3257,7 @@
       </c>
       <c r="C160" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="161" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3277,7 +3274,7 @@
       </c>
       <c r="C162" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="163" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3287,7 +3284,7 @@
       </c>
       <c r="C163" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="164" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3297,7 +3294,7 @@
       </c>
       <c r="C164" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="165" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3307,7 +3304,7 @@
       </c>
       <c r="C165" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="166" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3324,7 +3321,7 @@
       </c>
       <c r="C167" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="168" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3334,7 +3331,7 @@
       </c>
       <c r="C168" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="169" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3344,7 +3341,7 @@
       </c>
       <c r="C169" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="170" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3361,7 +3358,7 @@
       </c>
       <c r="C171" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="172" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3371,7 +3368,7 @@
       </c>
       <c r="C172" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="173" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3395,7 +3392,7 @@
       </c>
       <c r="C175" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="176" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3405,7 +3402,7 @@
       </c>
       <c r="C176" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="177" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3415,7 +3412,7 @@
       </c>
       <c r="C177" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="178" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3425,7 +3422,7 @@
       </c>
       <c r="C178" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="179" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3435,7 +3432,7 @@
       </c>
       <c r="C179" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="180" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3459,7 +3456,7 @@
       </c>
       <c r="C182" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="183" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3469,7 +3466,7 @@
       </c>
       <c r="C183" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="184" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3479,7 +3476,7 @@
       </c>
       <c r="C184" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="185" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3489,7 +3486,7 @@
       </c>
       <c r="C185" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="186" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3499,7 +3496,7 @@
       </c>
       <c r="C186" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="187" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3523,7 +3520,7 @@
       </c>
       <c r="C189" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="190" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3533,7 +3530,7 @@
       </c>
       <c r="C190" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="191" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3543,7 +3540,7 @@
       </c>
       <c r="C191" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="192" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3553,7 +3550,7 @@
       </c>
       <c r="C192" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="193" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3563,7 +3560,7 @@
       </c>
       <c r="C193" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="194" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3580,7 +3577,7 @@
       </c>
       <c r="C195" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="196" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3590,7 +3587,7 @@
       </c>
       <c r="C196" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="197" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3600,7 +3597,7 @@
       </c>
       <c r="C197" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="198" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3617,7 +3614,7 @@
       </c>
       <c r="C199" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="200" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3627,7 +3624,7 @@
       </c>
       <c r="C200" t="str">
         <f>'Versioni EJB'!C33</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="201" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3637,7 +3634,7 @@
       </c>
       <c r="C201" t="str">
         <f>'Versioni EJB'!C25</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="202" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3647,7 +3644,7 @@
       </c>
       <c r="C202" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="203" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3657,7 +3654,7 @@
       </c>
       <c r="C203" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="204" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3667,7 +3664,7 @@
       </c>
       <c r="C204" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="205" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3677,7 +3674,7 @@
       </c>
       <c r="C205" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="206" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3687,7 +3684,7 @@
       </c>
       <c r="C206" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="207" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3697,7 +3694,7 @@
       </c>
       <c r="C207" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="208" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3707,7 +3704,7 @@
       </c>
       <c r="C208" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="209" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3724,7 +3721,7 @@
       </c>
       <c r="C210" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="211" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3734,7 +3731,7 @@
       </c>
       <c r="C211" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="212" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3744,7 +3741,7 @@
       </c>
       <c r="C212" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="213" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3761,7 +3758,7 @@
       </c>
       <c r="C214" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="215" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3771,7 +3768,7 @@
       </c>
       <c r="C215" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="216" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3781,7 +3778,7 @@
       </c>
       <c r="C216" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="217" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3791,7 +3788,7 @@
       </c>
       <c r="C217" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="218" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3801,7 +3798,7 @@
       </c>
       <c r="C218" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="219" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3811,7 +3808,7 @@
       </c>
       <c r="C219" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="220" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3821,7 +3818,7 @@
       </c>
       <c r="C220" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="221" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3831,7 +3828,7 @@
       </c>
       <c r="C221" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="222" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3848,7 +3845,7 @@
       </c>
       <c r="C223" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="224" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3858,7 +3855,7 @@
       </c>
       <c r="C224" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="225" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3868,7 +3865,7 @@
       </c>
       <c r="C225" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="226" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3878,7 +3875,7 @@
       </c>
       <c r="C226" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="227" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3888,7 +3885,7 @@
       </c>
       <c r="C227" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="228" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3898,7 +3895,7 @@
       </c>
       <c r="C228" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="229" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3908,7 +3905,7 @@
       </c>
       <c r="C229" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="230" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3918,7 +3915,7 @@
       </c>
       <c r="C230" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="231" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3928,7 +3925,7 @@
       </c>
       <c r="C231" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="232" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3952,7 +3949,7 @@
       </c>
       <c r="C234" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="235" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3962,7 +3959,7 @@
       </c>
       <c r="C235" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="236" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3972,7 +3969,7 @@
       </c>
       <c r="C236" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="237" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3982,7 +3979,7 @@
       </c>
       <c r="C237" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="238" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3992,7 +3989,7 @@
       </c>
       <c r="C238" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="239" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4002,7 +3999,7 @@
       </c>
       <c r="C239" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="240" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4012,7 +4009,7 @@
       </c>
       <c r="C240" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="241" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4022,7 +4019,7 @@
       </c>
       <c r="C241" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="242" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4032,7 +4029,7 @@
       </c>
       <c r="C242" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="243" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4049,7 +4046,7 @@
       </c>
       <c r="C244" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="245" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4059,7 +4056,7 @@
       </c>
       <c r="C245" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="246" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4069,7 +4066,7 @@
       </c>
       <c r="C246" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="247" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4079,7 +4076,7 @@
       </c>
       <c r="C247" t="str">
         <f>'Versioni EJB'!C19</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="248" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4089,7 +4086,7 @@
       </c>
       <c r="C248" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="249" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4099,7 +4096,7 @@
       </c>
       <c r="C249" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="250" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4109,7 +4106,7 @@
       </c>
       <c r="C250" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="251" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4119,7 +4116,7 @@
       </c>
       <c r="C251" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="252" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4129,7 +4126,7 @@
       </c>
       <c r="C252" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="253" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4139,7 +4136,7 @@
       </c>
       <c r="C253" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="254" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4149,7 +4146,7 @@
       </c>
       <c r="C254" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="255" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4159,7 +4156,7 @@
       </c>
       <c r="C255" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="256" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4176,7 +4173,7 @@
       </c>
       <c r="C257" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="258" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4186,7 +4183,7 @@
       </c>
       <c r="C258" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="259" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4196,7 +4193,7 @@
       </c>
       <c r="C259" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="260" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4206,7 +4203,7 @@
       </c>
       <c r="C260" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="261" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4216,7 +4213,7 @@
       </c>
       <c r="C261" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="262" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4226,7 +4223,7 @@
       </c>
       <c r="C262" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="263" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4236,7 +4233,7 @@
       </c>
       <c r="C263" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="264" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4253,7 +4250,7 @@
       </c>
       <c r="C265" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="266" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4263,7 +4260,7 @@
       </c>
       <c r="C266" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="267" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4273,7 +4270,7 @@
       </c>
       <c r="C267" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="268" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4283,7 +4280,7 @@
       </c>
       <c r="C268" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="269" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4293,7 +4290,7 @@
       </c>
       <c r="C269" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="270" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4303,7 +4300,7 @@
       </c>
       <c r="C270" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="271" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4320,7 +4317,7 @@
       </c>
       <c r="C272" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="273" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4330,7 +4327,7 @@
       </c>
       <c r="C273" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="274" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4340,7 +4337,7 @@
       </c>
       <c r="C274" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="275" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4350,7 +4347,7 @@
       </c>
       <c r="C275" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="276" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4360,7 +4357,7 @@
       </c>
       <c r="C276" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="277" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4370,7 +4367,7 @@
       </c>
       <c r="C277" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="278" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4387,7 +4384,7 @@
       </c>
       <c r="C279" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="280" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4397,7 +4394,7 @@
       </c>
       <c r="C280" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="281" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4407,7 +4404,7 @@
       </c>
       <c r="C281" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="282" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4417,7 +4414,7 @@
       </c>
       <c r="C282" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="283" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4427,7 +4424,7 @@
       </c>
       <c r="C283" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="284" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4437,7 +4434,7 @@
       </c>
       <c r="C284" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="285" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4447,7 +4444,7 @@
       </c>
       <c r="C285" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="286" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4457,7 +4454,7 @@
       </c>
       <c r="C286" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="287" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4467,7 +4464,7 @@
       </c>
       <c r="C287" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="288" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4484,7 +4481,7 @@
       </c>
       <c r="C289" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="290" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4494,7 +4491,7 @@
       </c>
       <c r="C290" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="291" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4504,7 +4501,7 @@
       </c>
       <c r="C291" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="292" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4514,7 +4511,7 @@
       </c>
       <c r="C292" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="293" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4524,7 +4521,7 @@
       </c>
       <c r="C293" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="294" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4534,7 +4531,7 @@
       </c>
       <c r="C294" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="295" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4544,7 +4541,7 @@
       </c>
       <c r="C295" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="296" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4554,7 +4551,7 @@
       </c>
       <c r="C296" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="297" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4571,7 +4568,7 @@
       </c>
       <c r="C298" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="299" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4581,7 +4578,7 @@
       </c>
       <c r="C299" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="300" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4591,7 +4588,7 @@
       </c>
       <c r="C300" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="301" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4601,7 +4598,7 @@
       </c>
       <c r="C301" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="302" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4625,7 +4622,7 @@
       </c>
       <c r="C304" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="305" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4635,7 +4632,7 @@
       </c>
       <c r="C305" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="306" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4645,7 +4642,7 @@
       </c>
       <c r="C306" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="307" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4655,7 +4652,7 @@
       </c>
       <c r="C307" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="308" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4665,7 +4662,7 @@
       </c>
       <c r="C308" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="309" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4675,7 +4672,7 @@
       </c>
       <c r="C309" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="310" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4685,7 +4682,7 @@
       </c>
       <c r="C310" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="311" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4695,7 +4692,7 @@
       </c>
       <c r="C311" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="312" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4712,7 +4709,7 @@
       </c>
       <c r="C313" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="314" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4722,7 +4719,7 @@
       </c>
       <c r="C314" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="315" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4732,7 +4729,7 @@
       </c>
       <c r="C315" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="316" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4742,7 +4739,7 @@
       </c>
       <c r="C316" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="317" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4752,7 +4749,7 @@
       </c>
       <c r="C317" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="318" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4762,7 +4759,7 @@
       </c>
       <c r="C318" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="319" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4772,7 +4769,7 @@
       </c>
       <c r="C319" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="320" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4782,7 +4779,7 @@
       </c>
       <c r="C320" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="321" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4792,7 +4789,7 @@
       </c>
       <c r="C321" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="322" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4802,7 +4799,7 @@
       </c>
       <c r="C322" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="323" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4812,7 +4809,7 @@
       </c>
       <c r="C323" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="324" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4829,7 +4826,7 @@
       </c>
       <c r="C325" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="326" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4839,7 +4836,7 @@
       </c>
       <c r="C326" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="327" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4849,7 +4846,7 @@
       </c>
       <c r="C327" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="328" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4859,7 +4856,7 @@
       </c>
       <c r="C328" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="329" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4869,7 +4866,7 @@
       </c>
       <c r="C329" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="330" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4879,7 +4876,7 @@
       </c>
       <c r="C330" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svis-SNAPSHOT</v>
+        <v>1.70.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="331" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4896,7 +4893,7 @@
       </c>
       <c r="C332" t="str">
         <f>'Versioni EJB'!C61</f>
-        <v>1.51.0-env-svis-SNAPSHOT</v>
+        <v>1.52.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="333" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4906,7 +4903,7 @@
       </c>
       <c r="C333" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svis-SNAPSHOT</v>
+        <v>1.70.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="334" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4916,7 +4913,7 @@
       </c>
       <c r="C334" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="335" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4926,7 +4923,7 @@
       </c>
       <c r="C335" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="336" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4936,7 +4933,7 @@
       </c>
       <c r="C336" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="337" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4946,7 +4943,7 @@
       </c>
       <c r="C337" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="338" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4956,7 +4953,7 @@
       </c>
       <c r="C338" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="339" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4966,7 +4963,7 @@
       </c>
       <c r="C339" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="340" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4990,7 +4987,7 @@
       </c>
       <c r="C342" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="343" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5000,7 +4997,7 @@
       </c>
       <c r="C343" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="344" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5010,7 +5007,7 @@
       </c>
       <c r="C344" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="345" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5020,7 +5017,7 @@
       </c>
       <c r="C345" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="346" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5037,7 +5034,7 @@
       </c>
       <c r="C347" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="348" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5047,7 +5044,7 @@
       </c>
       <c r="C348" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="349" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5057,7 +5054,7 @@
       </c>
       <c r="C349" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="350" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5067,7 +5064,7 @@
       </c>
       <c r="C350" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="351" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5084,7 +5081,7 @@
       </c>
       <c r="C352" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="353" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5094,7 +5091,7 @@
       </c>
       <c r="C353" t="str">
         <f>'Versioni EJB'!C33</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="354" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5104,7 +5101,7 @@
       </c>
       <c r="C354" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="355" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5114,7 +5111,7 @@
       </c>
       <c r="C355" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="356" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5124,7 +5121,7 @@
       </c>
       <c r="C356" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="357" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5141,7 +5138,7 @@
       </c>
       <c r="C358" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="359" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5151,7 +5148,7 @@
       </c>
       <c r="C359" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="360" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5161,7 +5158,7 @@
       </c>
       <c r="C360" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="361" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5171,7 +5168,7 @@
       </c>
       <c r="C361" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="362" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5188,7 +5185,7 @@
       </c>
       <c r="C363" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="364" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5198,7 +5195,7 @@
       </c>
       <c r="C364" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="365" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5208,7 +5205,7 @@
       </c>
       <c r="C365" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="366" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5218,7 +5215,7 @@
       </c>
       <c r="C366" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="367" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5228,7 +5225,7 @@
       </c>
       <c r="C367" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="368" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5245,7 +5242,7 @@
       </c>
       <c r="C369" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="370" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5255,7 +5252,7 @@
       </c>
       <c r="C370" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="371" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5265,7 +5262,7 @@
       </c>
       <c r="C371" t="str">
         <f>'Versioni EJB'!C61</f>
-        <v>1.51.0-env-svis-SNAPSHOT</v>
+        <v>1.52.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="372" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5275,7 +5272,7 @@
       </c>
       <c r="C372" t="str">
         <f>'Versioni EJB'!C44</f>
-        <v>1.39.0-env-svis-SNAPSHOT</v>
+        <v>1.39.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="373" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5285,7 +5282,7 @@
       </c>
       <c r="C373" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svis-SNAPSHOT</v>
+        <v>1.70.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="374" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5295,7 +5292,7 @@
       </c>
       <c r="C374" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="375" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5305,7 +5302,7 @@
       </c>
       <c r="C375" t="str">
         <f>'Versioni EJB'!C66</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="376" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5315,7 +5312,7 @@
       </c>
       <c r="C376" t="str">
         <f>'Versioni EJB'!C69</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="377" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5325,7 +5322,7 @@
       </c>
       <c r="C377" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="378" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5335,7 +5332,7 @@
       </c>
       <c r="C378" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="379" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5345,7 +5342,7 @@
       </c>
       <c r="C379" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="380" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5355,7 +5352,7 @@
       </c>
       <c r="C380" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="381" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5372,7 +5369,7 @@
       </c>
       <c r="C382" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="383" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5382,7 +5379,7 @@
       </c>
       <c r="C383" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="384" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5392,7 +5389,7 @@
       </c>
       <c r="C384" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="385" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5402,7 +5399,7 @@
       </c>
       <c r="C385" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="386" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5426,7 +5423,7 @@
       </c>
       <c r="C388" t="str">
         <f>'Versioni EJB'!C5</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="389" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5436,7 +5433,7 @@
       </c>
       <c r="C389" t="str">
         <f>'Versioni EJB'!C43</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="390" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5446,7 +5443,7 @@
       </c>
       <c r="C390" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="391" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5456,7 +5453,7 @@
       </c>
       <c r="C391" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="392" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5466,7 +5463,7 @@
       </c>
       <c r="C392" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="393" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5476,7 +5473,7 @@
       </c>
       <c r="C393" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="394" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5486,7 +5483,7 @@
       </c>
       <c r="C394" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="395" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5518,7 +5515,7 @@
       </c>
       <c r="C398" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="399" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5528,7 +5525,7 @@
       </c>
       <c r="C399" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="400" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5538,7 +5535,7 @@
       </c>
       <c r="C400" t="str">
         <f>'Versioni EJB'!C85</f>
-        <v>1.19.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="401" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5548,7 +5545,7 @@
       </c>
       <c r="C401" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="402" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5558,7 +5555,7 @@
       </c>
       <c r="C402" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="403" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5568,7 +5565,7 @@
       </c>
       <c r="C403" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="404" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5578,7 +5575,7 @@
       </c>
       <c r="C404" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="405" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5588,7 +5585,7 @@
       </c>
       <c r="C405" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="406" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5598,7 +5595,7 @@
       </c>
       <c r="C406" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="407" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5608,7 +5605,7 @@
       </c>
       <c r="C407" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="408" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5618,7 +5615,7 @@
       </c>
       <c r="C408" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="409" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5642,7 +5639,7 @@
       </c>
       <c r="C411" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="412" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5652,7 +5649,7 @@
       </c>
       <c r="C412" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svis-SNAPSHOT</v>
+        <v>1.201.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="413" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5662,7 +5659,7 @@
       </c>
       <c r="C413" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="414" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5672,7 +5669,7 @@
       </c>
       <c r="C414" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="415" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5682,7 +5679,7 @@
       </c>
       <c r="C415" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="416" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5692,7 +5689,7 @@
       </c>
       <c r="C416" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="417" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5716,7 +5713,7 @@
       </c>
       <c r="C419" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="420" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5726,7 +5723,7 @@
       </c>
       <c r="C420" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="421" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5736,7 +5733,7 @@
       </c>
       <c r="C421" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.136.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="422" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5746,7 +5743,7 @@
       </c>
       <c r="C422" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="423" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5756,7 +5753,7 @@
       </c>
       <c r="C423" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="424" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5766,7 +5763,7 @@
       </c>
       <c r="C424" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="425" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5783,7 +5780,7 @@
       </c>
       <c r="C426" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="427" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5793,7 +5790,7 @@
       </c>
       <c r="C427" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svis-SNAPSHOT</v>
+        <v>1.201.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="428" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5803,7 +5800,7 @@
       </c>
       <c r="C428" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="429" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5813,7 +5810,7 @@
       </c>
       <c r="C429" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="430" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5823,7 +5820,7 @@
       </c>
       <c r="C430" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="431" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5833,7 +5830,7 @@
       </c>
       <c r="C431" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="432" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5843,7 +5840,7 @@
       </c>
       <c r="C432" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="433" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5860,7 +5857,7 @@
       </c>
       <c r="C434" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.136.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="435" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5870,7 +5867,7 @@
       </c>
       <c r="C435" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="436" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5880,7 +5877,7 @@
       </c>
       <c r="C436" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="437" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5890,7 +5887,7 @@
       </c>
       <c r="C437" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="438" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5900,7 +5897,7 @@
       </c>
       <c r="C438" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="439" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5917,7 +5914,7 @@
       </c>
       <c r="C440" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svis-SNAPSHOT</v>
+        <v>1.201.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="441" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5927,7 +5924,7 @@
       </c>
       <c r="C441" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="442" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5937,7 +5934,7 @@
       </c>
       <c r="C442" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="443" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5947,7 +5944,7 @@
       </c>
       <c r="C443" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="444" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5957,7 +5954,7 @@
       </c>
       <c r="C444" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="445" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5967,7 +5964,7 @@
       </c>
       <c r="C445" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="446" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5977,7 +5974,7 @@
       </c>
       <c r="C446" t="str">
         <f>'Versioni EJB'!C19</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="447" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5987,7 +5984,7 @@
       </c>
       <c r="C447" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="448" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5997,7 +5994,7 @@
       </c>
       <c r="C448" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="449" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6007,7 +6004,7 @@
       </c>
       <c r="C449" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="450" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6017,7 +6014,7 @@
       </c>
       <c r="C450" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="451" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6027,7 +6024,7 @@
       </c>
       <c r="C451" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="452" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6037,7 +6034,7 @@
       </c>
       <c r="C452" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="453" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6047,7 +6044,7 @@
       </c>
       <c r="C453" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="454" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6057,7 +6054,7 @@
       </c>
       <c r="C454" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="455" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6074,7 +6071,7 @@
       </c>
       <c r="C456" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="457" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6084,7 +6081,7 @@
       </c>
       <c r="C457" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="458" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6094,7 +6091,7 @@
       </c>
       <c r="C458" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="459" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6104,7 +6101,7 @@
       </c>
       <c r="C459" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="460" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6114,7 +6111,7 @@
       </c>
       <c r="C460" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="461" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6124,7 +6121,7 @@
       </c>
       <c r="C461" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="462" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6134,7 +6131,7 @@
       </c>
       <c r="C462" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.136.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="463" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6151,7 +6148,7 @@
       </c>
       <c r="C464" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.136.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="465" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6161,7 +6158,7 @@
       </c>
       <c r="C465" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.48.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="466" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6171,7 +6168,7 @@
       </c>
       <c r="C466" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="467" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6181,7 +6178,7 @@
       </c>
       <c r="C467" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="468" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6191,7 +6188,7 @@
       </c>
       <c r="C468" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="469" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6215,7 +6212,7 @@
       </c>
       <c r="C471" t="str">
         <f>'Versioni EJB'!C80</f>
-        <v>1.40.0-env-svis-SNAPSHOT</v>
+        <v>1.40.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="472" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6225,7 +6222,7 @@
       </c>
       <c r="C472" t="str">
         <f>'Versioni EJB'!C79</f>
-        <v>1.27.0-env-svis-SNAPSHOT</v>
+        <v>1.27.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="473" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6235,7 +6232,7 @@
       </c>
       <c r="C473" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="474" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6245,7 +6242,7 @@
       </c>
       <c r="C474" t="str">
         <f>'Versioni EJB'!C59</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="475" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6255,7 +6252,7 @@
       </c>
       <c r="C475" t="str">
         <f>'Versioni EJB'!C77</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="476" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6265,7 +6262,7 @@
       </c>
       <c r="C476" t="str">
         <f>'Versioni EJB'!C25</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="477" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6275,7 +6272,7 @@
       </c>
       <c r="C477" t="str">
         <f>'Versioni EJB'!C57</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="478" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6285,7 +6282,7 @@
       </c>
       <c r="C478" t="str">
         <f>'Versioni EJB'!C96</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="479" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6295,7 +6292,7 @@
       </c>
       <c r="C479" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="480" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6305,7 +6302,7 @@
       </c>
       <c r="C480" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="481" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6315,7 +6312,7 @@
       </c>
       <c r="C481" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="482" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6325,7 +6322,7 @@
       </c>
       <c r="C482" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="483" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6335,7 +6332,7 @@
       </c>
       <c r="C483" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="484" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6352,7 +6349,7 @@
       </c>
       <c r="C485" t="str">
         <f>'Versioni EJB'!C94</f>
-        <v>1.120.0-env-svis-SNAPSHOT</v>
+        <v>1.120.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="486" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6362,7 +6359,7 @@
       </c>
       <c r="C486" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svis-SNAPSHOT</v>
+        <v>1.201.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="487" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6372,7 +6369,7 @@
       </c>
       <c r="C487" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="488" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6382,7 +6379,7 @@
       </c>
       <c r="C488" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="489" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6392,7 +6389,7 @@
       </c>
       <c r="C489" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="490" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6402,7 +6399,7 @@
       </c>
       <c r="C490" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.6.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="491" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6412,7 +6409,7 @@
       </c>
       <c r="C491" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="492" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6429,7 +6426,7 @@
       </c>
       <c r="C493" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="494" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6439,7 +6436,7 @@
       </c>
       <c r="C494" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svis-SNAPSHOT</v>
+        <v>1.24.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="495" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6449,7 +6446,7 @@
       </c>
       <c r="C495" t="str">
         <f>'Versioni EJB'!C94</f>
-        <v>1.120.0-env-svis-SNAPSHOT</v>
+        <v>1.120.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="496" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6459,7 +6456,7 @@
       </c>
       <c r="C496" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="497" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6476,127 +6473,126 @@
       <c r="B498" s="4"/>
       <c r="C498" s="4"/>
     </row>
-    <row r="499" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B499" t="str">
         <f>'Versioni EJB'!B87</f>
         <v>comunicazioni-ejb</v>
       </c>
       <c r="C499" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="500" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.201.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B500" t="str">
         <f>'Versioni EJB'!B99</f>
         <v>pulsantiera-ejb</v>
       </c>
       <c r="C500" t="str">
         <f>'Versioni EJB'!C99</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="501" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.14.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B501" t="str">
         <f>'Versioni EJB'!B59</f>
         <v>matchingidbpfm-ejb</v>
       </c>
       <c r="C501" t="str">
         <f>'Versioni EJB'!C59</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="502" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.8.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B502" t="str">
         <f>'Versioni EJB'!B57</f>
         <v>bustine-ejb</v>
       </c>
       <c r="C502" t="str">
         <f>'Versioni EJB'!C57</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="503" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.7.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B503" t="str">
         <f>'Versioni EJB'!B34</f>
         <v>prestiti-ejb</v>
       </c>
       <c r="C503" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="504" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.9.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B504" t="str">
         <f>'Versioni EJB'!B96</f>
         <v>proposte-ejb</v>
       </c>
       <c r="C504" t="str">
         <f>'Versioni EJB'!C96</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="505" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.6.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B505" t="str">
         <f>'Versioni EJB'!B64</f>
         <v>bonifico-ejb</v>
       </c>
       <c r="C505" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="506" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.22.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B506" t="str">
         <f>'Versioni EJB'!B42</f>
         <v>pfm-ejb</v>
       </c>
       <c r="C506" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="507" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.10.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B507" t="str">
         <f>'Versioni EJB'!B18</f>
         <v>agenda-ejb</v>
       </c>
       <c r="C507" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="508" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.8.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B508" t="str">
         <f>'Versioni EJB'!B73</f>
         <v>carte-ejb</v>
       </c>
       <c r="C508" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="509" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.22.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B509" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
       <c r="C509" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="510" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.5.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B510" t="str">
         <f>'Versioni EJB'!B35</f>
         <v>saldo-ejb</v>
       </c>
       <c r="C510" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
-      </c>
-    </row>
-    <row r="511" spans="1:3" collapsed="1" x14ac:dyDescent="0.3"/>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B16:C17">
     <sortCondition ref="B16"/>

</xml_diff>

<commit_message>
Aggiornamento per allineamento env/svis
</commit_message>
<xml_diff>
--- a/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
+++ b/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openshift\SoftwareAllineamenti\src\main\resources\excelutils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD3CEBF-7914-43DC-8555-242F312FA979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A096AE88-5982-4359-94C5-3738FC22158C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="15990" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Versioni EJB" sheetId="1" r:id="rId1"/>
@@ -366,97 +366,97 @@
     <t>VERSIONE SVIS/SVIA</t>
   </si>
   <si>
-    <t>1.8.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.5.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.7.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.6.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.48.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.24.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.10.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.12.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.9.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.14.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.11.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>0.30.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.19.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.13.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.39.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.20.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.15.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.17.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.52.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.22.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.70.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.16.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.27.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.40.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.47.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.201.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.136.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.30.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.120.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.38.0-env-svia-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.69.0-env-svia-SNAPSHOT</t>
+    <t>1.10.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.5.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.7.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.8.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.6.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.48.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.29.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.12.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.9.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.20.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.11.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>0.30.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.19.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.14.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.39.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.15.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.17.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.52.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.22.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.70.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.16.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.27.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.40.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.47.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.202.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.136.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.120.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.38.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.30.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.13.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.69.0-env-svis-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
@@ -936,7 +936,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -945,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -971,7 +971,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +980,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -997,7 +997,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1014,7 +1014,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1023,7 +1023,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,7 +1032,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1041,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1059,7 +1059,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1095,7 +1095,7 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1122,7 +1122,7 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1149,7 +1149,7 @@
         <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1158,7 +1158,7 @@
         <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1211,7 +1211,7 @@
         <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1220,7 +1220,7 @@
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1229,7 +1229,7 @@
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1238,7 +1238,7 @@
         <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1247,7 +1247,7 @@
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1309,7 +1309,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,7 +1326,7 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1343,7 +1343,7 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1378,7 +1378,7 @@
         <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1387,7 +1387,7 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1396,7 +1396,7 @@
         <v>49</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
         <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1422,7 +1422,7 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1431,7 +1431,7 @@
         <v>52</v>
       </c>
       <c r="C64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1440,7 +1440,7 @@
         <v>53</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,7 +1458,7 @@
         <v>55</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,7 +1467,7 @@
         <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1502,7 +1502,7 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1511,7 +1511,7 @@
         <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1520,7 +1520,7 @@
         <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,7 +1564,7 @@
         <v>65</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1573,7 +1573,7 @@
         <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1591,7 +1591,7 @@
         <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1600,7 +1600,7 @@
         <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
         <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1634,7 +1634,7 @@
         <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1651,7 +1651,7 @@
         <v>72</v>
       </c>
       <c r="C89" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1686,7 +1686,7 @@
         <v>75</v>
       </c>
       <c r="C93" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1695,7 +1695,7 @@
         <v>76</v>
       </c>
       <c r="C94" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,7 +1704,7 @@
         <v>77</v>
       </c>
       <c r="C95" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1713,7 +1713,7 @@
         <v>78</v>
       </c>
       <c r="C96" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -1730,7 +1730,7 @@
         <v>79</v>
       </c>
       <c r="C98" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -1739,7 +1739,7 @@
         <v>80</v>
       </c>
       <c r="C99" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -1748,7 +1748,7 @@
         <v>81</v>
       </c>
       <c r="C100" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -1794,7 +1794,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E386" sqref="E386"/>
+      <selection pane="bottomLeft" activeCell="A388" sqref="A388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="C5" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="6" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="C7" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="8" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="C11" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="12" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="C13" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="14" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="C16" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="17" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="C17" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="18" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="C19" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svia-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="20" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="C20" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="21" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="C22" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="23" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="C23" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="24" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="C26" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="27" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="C27" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="28" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2043,7 +2043,7 @@
       </c>
       <c r="C28" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="29" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="C29" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="30" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="C32" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="33" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="C33" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="34" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="C34" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="35" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="C35" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="36" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="C36" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="37" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="C38" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="39" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="C39" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="40" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="C40" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="41" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="C41" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="42" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C43" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="44" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="C44" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="45" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C45" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="46" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="C47" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="C48" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="49" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C49" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="50" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="C51" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="52" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C52" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="53" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="C53" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="54" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="C55" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="56" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="C56" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="57" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="C58" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="59" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="C59" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="60" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="C60" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="61" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="C61" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="62" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="C62" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="63" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="C65" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="66" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="C66" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="67" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="C67" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="68" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="C69" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="70" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="C70" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="71" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="C72" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="73" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="C73" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="74" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2475,7 +2475,7 @@
       </c>
       <c r="C75" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="76" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="C76" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="77" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="C78" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="79" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="C79" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="80" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="C81" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="82" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="C82" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="83" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="C84" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="85" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="C85" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="86" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="C87" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="88" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="C88" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="89" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="C90" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="91" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="C91" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="92" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2637,7 +2637,7 @@
       </c>
       <c r="C93" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="94" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2647,7 +2647,7 @@
       </c>
       <c r="C94" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="95" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="C97" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="98" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="C98" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="99" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="C99" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="100" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="C100" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="101" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="C102" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="103" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="C103" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="104" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="C104" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="105" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="C105" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="106" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C107" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="108" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="C108" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="109" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="C109" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="110" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="C110" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="111" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2806,7 +2806,7 @@
       </c>
       <c r="C111" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="112" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="C112" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="113" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="C114" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="115" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="C115" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="116" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="C116" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="117" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="C117" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="118" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="C118" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="119" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="C121" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="122" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2907,7 +2907,7 @@
       </c>
       <c r="C122" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="123" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2917,7 +2917,7 @@
       </c>
       <c r="C123" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="124" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="C124" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="125" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="C125" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="126" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="C127" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="128" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2964,7 +2964,7 @@
       </c>
       <c r="C128" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="C130" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="131" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="C131" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="132" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3009,7 +3009,7 @@
       </c>
       <c r="C133" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="134" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="C134" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="135" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="C136" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="137" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3046,7 +3046,7 @@
       </c>
       <c r="C137" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="138" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="C138" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="139" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3074,7 +3074,7 @@
       </c>
       <c r="C140" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="141" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="C143" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="144" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="C144" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="145" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="C145" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="146" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3136,7 +3136,7 @@
       </c>
       <c r="C147" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="148" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="C148" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="149" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="C149" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="150" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="C150" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="151" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="C153" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="154" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="C154" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="155" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="C155" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="156" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3220,7 +3220,7 @@
       </c>
       <c r="C156" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="157" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="C158" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="159" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="C159" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="160" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3257,7 +3257,7 @@
       </c>
       <c r="C160" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="161" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="C162" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="163" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3284,7 +3284,7 @@
       </c>
       <c r="C163" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="164" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="C164" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="165" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="C165" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="166" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="C167" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="168" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="C168" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="169" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="C169" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="170" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3358,7 +3358,7 @@
       </c>
       <c r="C171" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="172" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="C172" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="173" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3392,7 +3392,7 @@
       </c>
       <c r="C175" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="176" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="C176" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="177" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3412,7 +3412,7 @@
       </c>
       <c r="C177" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="178" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="C178" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svia-SNAPSHOT</v>
+        <v>1.12.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="179" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="C179" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="180" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="C182" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="183" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="C183" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="184" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="C184" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="185" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="C185" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="186" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="C186" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="187" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="C189" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="190" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="C190" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="191" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C191" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="192" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="C192" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="193" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3560,7 +3560,7 @@
       </c>
       <c r="C193" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="194" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="C195" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="196" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3587,7 +3587,7 @@
       </c>
       <c r="C196" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="197" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="C197" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="198" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="C199" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="200" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3624,7 +3624,7 @@
       </c>
       <c r="C200" t="str">
         <f>'Versioni EJB'!C33</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="201" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3634,7 +3634,7 @@
       </c>
       <c r="C201" t="str">
         <f>'Versioni EJB'!C25</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="202" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3644,7 +3644,7 @@
       </c>
       <c r="C202" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="203" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="C203" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="204" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="C204" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="205" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="C205" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="206" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="C206" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="207" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3694,7 +3694,7 @@
       </c>
       <c r="C207" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="208" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C208" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="209" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="C210" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="211" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="C211" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="212" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="C212" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="213" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="C214" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="215" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="C215" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="216" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3778,7 +3778,7 @@
       </c>
       <c r="C216" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="217" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="C217" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="218" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="C218" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="219" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="C219" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="220" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="C220" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="221" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="C221" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="222" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3845,7 +3845,7 @@
       </c>
       <c r="C223" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="224" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3855,7 +3855,7 @@
       </c>
       <c r="C224" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="225" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="C225" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="226" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="C226" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="227" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="C227" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="228" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="C228" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="229" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="C229" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="230" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="C230" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="231" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="C231" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="232" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="C234" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="235" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="C235" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="236" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="C236" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="237" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="C237" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="238" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3989,7 +3989,7 @@
       </c>
       <c r="C238" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="239" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="C239" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="240" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4009,7 +4009,7 @@
       </c>
       <c r="C240" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="241" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C241" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="242" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4029,7 +4029,7 @@
       </c>
       <c r="C242" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="243" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="C244" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="245" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="C245" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="246" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="C246" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="247" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4076,7 +4076,7 @@
       </c>
       <c r="C247" t="str">
         <f>'Versioni EJB'!C19</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="248" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="C248" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="249" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C249" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svia-SNAPSHOT</v>
+        <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="250" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="C250" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="251" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="C251" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="252" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="C252" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="253" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="C253" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="254" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4146,7 +4146,7 @@
       </c>
       <c r="C254" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="255" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="C255" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="256" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="C257" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="258" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="C258" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="259" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="C259" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="260" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="C260" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="261" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C261" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="262" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="C262" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="263" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="C263" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="264" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="C265" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="266" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4260,7 +4260,7 @@
       </c>
       <c r="C266" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="267" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="C267" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="268" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="C268" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="269" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4290,7 +4290,7 @@
       </c>
       <c r="C269" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="270" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="C270" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="271" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4317,7 +4317,7 @@
       </c>
       <c r="C272" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="273" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="C273" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="274" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="C274" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="275" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="C275" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="276" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4357,7 +4357,7 @@
       </c>
       <c r="C276" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="277" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="C277" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="278" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4384,7 +4384,7 @@
       </c>
       <c r="C279" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="280" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="C280" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="281" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4404,7 +4404,7 @@
       </c>
       <c r="C281" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="282" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4414,7 +4414,7 @@
       </c>
       <c r="C282" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="283" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4424,7 +4424,7 @@
       </c>
       <c r="C283" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="284" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="C284" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="285" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="C285" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="286" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="C286" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="287" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="C287" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="288" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="C289" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="290" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4491,7 +4491,7 @@
       </c>
       <c r="C290" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="291" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4501,7 +4501,7 @@
       </c>
       <c r="C291" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="292" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4511,7 +4511,7 @@
       </c>
       <c r="C292" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="293" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="C293" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="294" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4531,7 +4531,7 @@
       </c>
       <c r="C294" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="295" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="C295" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="296" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="C296" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="297" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="C298" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="299" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="C299" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="300" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4588,7 +4588,7 @@
       </c>
       <c r="C300" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="301" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="C301" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svia-SNAPSHOT</v>
+        <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="302" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4622,7 +4622,7 @@
       </c>
       <c r="C304" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="305" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="C305" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="306" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4642,7 +4642,7 @@
       </c>
       <c r="C306" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="307" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="C307" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="308" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4662,7 +4662,7 @@
       </c>
       <c r="C308" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="309" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="C309" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="310" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4682,7 +4682,7 @@
       </c>
       <c r="C310" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="311" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="C311" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="312" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="C313" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="314" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4719,7 +4719,7 @@
       </c>
       <c r="C314" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="315" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="C315" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svia-SNAPSHOT</v>
+        <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="316" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4739,7 +4739,7 @@
       </c>
       <c r="C316" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="317" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4749,7 +4749,7 @@
       </c>
       <c r="C317" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="318" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4759,7 +4759,7 @@
       </c>
       <c r="C318" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="319" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="C319" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="320" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4779,7 +4779,7 @@
       </c>
       <c r="C320" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="321" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="C321" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="322" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C322" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="323" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="C323" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="324" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="C325" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="326" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="C326" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="327" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="C327" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="328" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="C328" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="329" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4866,7 +4866,7 @@
       </c>
       <c r="C329" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="330" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4876,7 +4876,7 @@
       </c>
       <c r="C330" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svia-SNAPSHOT</v>
+        <v>1.70.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="331" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="C332" t="str">
         <f>'Versioni EJB'!C61</f>
-        <v>1.52.0-env-svia-SNAPSHOT</v>
+        <v>1.52.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="333" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4903,7 +4903,7 @@
       </c>
       <c r="C333" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svia-SNAPSHOT</v>
+        <v>1.70.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="334" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="C334" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="335" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4923,7 +4923,7 @@
       </c>
       <c r="C335" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="336" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="C336" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="337" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="C337" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="338" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="C338" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="339" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C339" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="340" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4987,7 +4987,7 @@
       </c>
       <c r="C342" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="343" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="C343" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="344" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5007,7 +5007,7 @@
       </c>
       <c r="C344" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svia-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="345" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="C345" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="346" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5034,7 +5034,7 @@
       </c>
       <c r="C347" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="348" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5044,7 +5044,7 @@
       </c>
       <c r="C348" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="349" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="C349" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="350" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5064,7 +5064,7 @@
       </c>
       <c r="C350" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="351" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="C352" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="353" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5091,7 +5091,7 @@
       </c>
       <c r="C353" t="str">
         <f>'Versioni EJB'!C33</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="354" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="C354" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="355" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="C355" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="356" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5121,7 +5121,7 @@
       </c>
       <c r="C356" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="357" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C358" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="359" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="C359" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="360" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="C360" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="361" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="C361" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svia-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="362" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5185,7 +5185,7 @@
       </c>
       <c r="C363" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="364" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="C364" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="365" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5205,7 +5205,7 @@
       </c>
       <c r="C365" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="366" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5215,7 +5215,7 @@
       </c>
       <c r="C366" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.16.0-env-svia-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="367" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5225,7 +5225,7 @@
       </c>
       <c r="C367" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="368" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="C369" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="370" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5252,7 +5252,7 @@
       </c>
       <c r="C370" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="371" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5262,7 +5262,7 @@
       </c>
       <c r="C371" t="str">
         <f>'Versioni EJB'!C61</f>
-        <v>1.52.0-env-svia-SNAPSHOT</v>
+        <v>1.52.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="372" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="C372" t="str">
         <f>'Versioni EJB'!C44</f>
-        <v>1.39.0-env-svia-SNAPSHOT</v>
+        <v>1.39.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="373" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5282,7 +5282,7 @@
       </c>
       <c r="C373" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svia-SNAPSHOT</v>
+        <v>1.70.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="374" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5292,7 +5292,7 @@
       </c>
       <c r="C374" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.16.0-env-svia-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="375" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="C375" t="str">
         <f>'Versioni EJB'!C66</f>
-        <v>1.11.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="376" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5312,7 +5312,7 @@
       </c>
       <c r="C376" t="str">
         <f>'Versioni EJB'!C69</f>
-        <v>1.12.0-env-svia-SNAPSHOT</v>
+        <v>1.12.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="377" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="C377" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="378" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5332,7 +5332,7 @@
       </c>
       <c r="C378" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="379" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5342,7 +5342,7 @@
       </c>
       <c r="C379" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="380" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5352,7 +5352,7 @@
       </c>
       <c r="C380" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="381" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5369,7 +5369,7 @@
       </c>
       <c r="C382" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="383" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5379,7 +5379,7 @@
       </c>
       <c r="C383" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="384" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="C384" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="385" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5399,7 +5399,7 @@
       </c>
       <c r="C385" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="386" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="C388" t="str">
         <f>'Versioni EJB'!C5</f>
-        <v>1.7.0-env-svia-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="389" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5433,7 +5433,7 @@
       </c>
       <c r="C389" t="str">
         <f>'Versioni EJB'!C43</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="390" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5443,7 +5443,7 @@
       </c>
       <c r="C390" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="391" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="C391" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="392" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5463,7 +5463,7 @@
       </c>
       <c r="C392" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="393" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="C393" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="394" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5483,7 +5483,7 @@
       </c>
       <c r="C394" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="395" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5515,7 +5515,7 @@
       </c>
       <c r="C398" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="399" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5525,7 +5525,7 @@
       </c>
       <c r="C399" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svia-SNAPSHOT</v>
+        <v>1.12.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="400" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5535,7 +5535,7 @@
       </c>
       <c r="C400" t="str">
         <f>'Versioni EJB'!C85</f>
-        <v>1.19.0-env-svia-SNAPSHOT</v>
+        <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="401" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="C401" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="402" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5555,7 +5555,7 @@
       </c>
       <c r="C402" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svia-SNAPSHOT</v>
+        <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="403" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5565,7 +5565,7 @@
       </c>
       <c r="C403" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="404" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="C404" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="405" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5585,7 +5585,7 @@
       </c>
       <c r="C405" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="406" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5595,7 +5595,7 @@
       </c>
       <c r="C406" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="407" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="C407" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="408" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5615,7 +5615,7 @@
       </c>
       <c r="C408" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="409" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5639,7 +5639,7 @@
       </c>
       <c r="C411" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="412" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5649,7 +5649,7 @@
       </c>
       <c r="C412" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svia-SNAPSHOT</v>
+        <v>1.202.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="413" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5659,7 +5659,7 @@
       </c>
       <c r="C413" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="414" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="C414" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="415" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5679,7 +5679,7 @@
       </c>
       <c r="C415" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="416" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="C416" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="417" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C419" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="420" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5723,7 +5723,7 @@
       </c>
       <c r="C420" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="421" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5733,7 +5733,7 @@
       </c>
       <c r="C421" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svia-SNAPSHOT</v>
+        <v>1.136.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="422" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5743,7 +5743,7 @@
       </c>
       <c r="C422" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="423" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5753,7 +5753,7 @@
       </c>
       <c r="C423" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="424" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="C424" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="425" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5780,7 +5780,7 @@
       </c>
       <c r="C426" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="427" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5790,7 +5790,7 @@
       </c>
       <c r="C427" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svia-SNAPSHOT</v>
+        <v>1.202.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="428" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5800,7 +5800,7 @@
       </c>
       <c r="C428" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="429" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5810,7 +5810,7 @@
       </c>
       <c r="C429" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="430" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5820,7 +5820,7 @@
       </c>
       <c r="C430" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="431" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5830,7 +5830,7 @@
       </c>
       <c r="C431" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="432" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5840,7 +5840,7 @@
       </c>
       <c r="C432" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="433" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5857,7 +5857,7 @@
       </c>
       <c r="C434" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svia-SNAPSHOT</v>
+        <v>1.136.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="435" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5867,7 +5867,7 @@
       </c>
       <c r="C435" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="436" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5877,7 +5877,7 @@
       </c>
       <c r="C436" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="437" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5887,7 +5887,7 @@
       </c>
       <c r="C437" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="438" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5897,7 +5897,7 @@
       </c>
       <c r="C438" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="439" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5914,7 +5914,7 @@
       </c>
       <c r="C440" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svia-SNAPSHOT</v>
+        <v>1.202.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="441" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5924,7 +5924,7 @@
       </c>
       <c r="C441" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="442" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="C442" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="443" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5944,7 +5944,7 @@
       </c>
       <c r="C443" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="444" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="C444" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="445" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5964,7 +5964,7 @@
       </c>
       <c r="C445" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svia-SNAPSHOT</v>
+        <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="446" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5974,7 +5974,7 @@
       </c>
       <c r="C446" t="str">
         <f>'Versioni EJB'!C19</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="447" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5984,7 +5984,7 @@
       </c>
       <c r="C447" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="448" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5994,7 +5994,7 @@
       </c>
       <c r="C448" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="449" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="C449" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="450" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="C450" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="451" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6024,7 +6024,7 @@
       </c>
       <c r="C451" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="452" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6034,7 +6034,7 @@
       </c>
       <c r="C452" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="453" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6044,7 +6044,7 @@
       </c>
       <c r="C453" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="454" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6054,7 +6054,7 @@
       </c>
       <c r="C454" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="455" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6071,7 +6071,7 @@
       </c>
       <c r="C456" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="457" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="C457" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="458" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6091,7 +6091,7 @@
       </c>
       <c r="C458" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.14.0-env-svia-SNAPSHOT</v>
+        <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="459" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6101,7 +6101,7 @@
       </c>
       <c r="C459" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="460" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6111,7 +6111,7 @@
       </c>
       <c r="C460" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="461" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="C461" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="462" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6131,7 +6131,7 @@
       </c>
       <c r="C462" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svia-SNAPSHOT</v>
+        <v>1.136.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="463" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6148,7 +6148,7 @@
       </c>
       <c r="C464" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svia-SNAPSHOT</v>
+        <v>1.136.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="465" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="C465" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svia-SNAPSHOT</v>
+        <v>1.48.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="466" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6168,7 +6168,7 @@
       </c>
       <c r="C466" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="467" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6178,7 +6178,7 @@
       </c>
       <c r="C467" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="468" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="C468" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="469" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="C471" t="str">
         <f>'Versioni EJB'!C80</f>
-        <v>1.40.0-env-svia-SNAPSHOT</v>
+        <v>1.40.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="472" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6222,7 +6222,7 @@
       </c>
       <c r="C472" t="str">
         <f>'Versioni EJB'!C79</f>
-        <v>1.27.0-env-svia-SNAPSHOT</v>
+        <v>1.27.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="473" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6232,7 +6232,7 @@
       </c>
       <c r="C473" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.11.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="474" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6242,7 +6242,7 @@
       </c>
       <c r="C474" t="str">
         <f>'Versioni EJB'!C59</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="475" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="C475" t="str">
         <f>'Versioni EJB'!C77</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="476" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6262,7 +6262,7 @@
       </c>
       <c r="C476" t="str">
         <f>'Versioni EJB'!C25</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="477" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6272,7 +6272,7 @@
       </c>
       <c r="C477" t="str">
         <f>'Versioni EJB'!C57</f>
-        <v>1.7.0-env-svia-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="478" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="C478" t="str">
         <f>'Versioni EJB'!C96</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="479" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6292,7 +6292,7 @@
       </c>
       <c r="C479" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="480" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="C480" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="481" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6312,7 +6312,7 @@
       </c>
       <c r="C481" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="482" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="C482" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="483" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="C483" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="484" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="C485" t="str">
         <f>'Versioni EJB'!C94</f>
-        <v>1.120.0-env-svia-SNAPSHOT</v>
+        <v>1.120.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="486" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6359,7 +6359,7 @@
       </c>
       <c r="C486" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svia-SNAPSHOT</v>
+        <v>1.202.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="487" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6369,7 +6369,7 @@
       </c>
       <c r="C487" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="488" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6379,7 +6379,7 @@
       </c>
       <c r="C488" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svia-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="489" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6389,7 +6389,7 @@
       </c>
       <c r="C489" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="490" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6399,7 +6399,7 @@
       </c>
       <c r="C490" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="491" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6409,7 +6409,7 @@
       </c>
       <c r="C491" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="492" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="C493" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="494" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6436,7 +6436,7 @@
       </c>
       <c r="C494" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.24.0-env-svia-SNAPSHOT</v>
+        <v>1.29.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="495" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="C495" t="str">
         <f>'Versioni EJB'!C94</f>
-        <v>1.120.0-env-svia-SNAPSHOT</v>
+        <v>1.120.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="496" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6456,7 +6456,7 @@
       </c>
       <c r="C496" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="497" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6480,7 +6480,7 @@
       </c>
       <c r="C499" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.201.0-env-svia-SNAPSHOT</v>
+        <v>1.202.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="500" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6490,7 +6490,7 @@
       </c>
       <c r="C500" t="str">
         <f>'Versioni EJB'!C99</f>
-        <v>1.14.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="501" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="C501" t="str">
         <f>'Versioni EJB'!C59</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="502" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6510,7 +6510,7 @@
       </c>
       <c r="C502" t="str">
         <f>'Versioni EJB'!C57</f>
-        <v>1.7.0-env-svia-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="503" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6520,7 +6520,7 @@
       </c>
       <c r="C503" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.9.0-env-svia-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="504" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6530,7 +6530,7 @@
       </c>
       <c r="C504" t="str">
         <f>'Versioni EJB'!C96</f>
-        <v>1.6.0-env-svia-SNAPSHOT</v>
+        <v>1.6.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="505" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6540,7 +6540,7 @@
       </c>
       <c r="C505" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="506" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6550,7 +6550,7 @@
       </c>
       <c r="C506" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.10.0-env-svia-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="507" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6560,7 +6560,7 @@
       </c>
       <c r="C507" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svia-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="508" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6570,7 +6570,7 @@
       </c>
       <c r="C508" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svia-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="509" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6580,7 +6580,7 @@
       </c>
       <c r="C509" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svia-SNAPSHOT</v>
+        <v>1.5.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="510" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="C510" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.13.0-env-svia-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
   </sheetData>
@@ -6598,11 +6598,6 @@
     <sortCondition ref="B16"/>
   </sortState>
   <mergeCells count="18">
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A497:C497"/>
     <mergeCell ref="A469:C469"/>
     <mergeCell ref="A151:C151"/>
@@ -6616,6 +6611,11 @@
     <mergeCell ref="A187:C187"/>
     <mergeCell ref="A180:C180"/>
     <mergeCell ref="A173:C173"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Allinemento settimanale di env/svis
</commit_message>
<xml_diff>
--- a/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
+++ b/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openshift\SoftwareAllineamenti\src\main\resources\excelutils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A096AE88-5982-4359-94C5-3738FC22158C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33021A85-5A9B-47BD-B3EC-171286295890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="142">
   <si>
     <t>isp-ib-om</t>
   </si>
@@ -369,42 +369,24 @@
     <t>1.10.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.5.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.7.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
     <t>1.8.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.6.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.48.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.29.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.12.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
     <t>1.9.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.20.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.11.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>0.30.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.19.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.14.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
@@ -417,9 +399,6 @@
     <t>1.17.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.52.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.22.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
@@ -429,34 +408,61 @@
     <t>1.16.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.27.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.40.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.47.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.202.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.136.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.120.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.38.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.30.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>1.13.0-env-svis-SNAPSHOT</t>
   </si>
   <si>
-    <t>1.69.0-env-svis-SNAPSHOT</t>
+    <t>1.50.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.34.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.26.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>0.33.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.18.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.42.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.21.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.53.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.23.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.71.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.25.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.28.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.41.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.205.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.138.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.31.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.122.0-env-svis-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.49.0-env-svis-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -853,7 +859,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
@@ -909,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -918,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -927,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -936,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -945,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -962,7 +968,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -971,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -997,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1014,7 +1020,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1023,7 +1029,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1041,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1050,7 +1056,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1059,7 +1065,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1068,7 +1074,7 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1077,7 +1083,7 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1086,7 +1092,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1095,7 +1101,7 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1104,7 +1110,7 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1113,7 +1119,7 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1122,7 +1128,7 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1131,7 +1137,7 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1140,7 +1146,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1149,7 +1155,7 @@
         <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1158,7 +1164,7 @@
         <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1167,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,7 +1182,7 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1185,7 +1191,7 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,7 +1200,7 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1211,7 +1217,7 @@
         <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1220,7 +1226,7 @@
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1229,7 +1235,7 @@
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1238,7 +1244,7 @@
         <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1247,7 +1253,7 @@
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,7 +1262,7 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1273,7 +1279,7 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1291,7 +1297,7 @@
         <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1300,7 +1306,7 @@
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1309,7 +1315,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,7 +1332,7 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1343,7 +1349,7 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1360,7 +1366,7 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1378,7 +1384,7 @@
         <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1387,7 +1393,7 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1396,7 +1402,7 @@
         <v>49</v>
       </c>
       <c r="C60" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1405,7 +1411,7 @@
         <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1422,7 +1428,7 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1431,7 +1437,7 @@
         <v>52</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1440,7 +1446,7 @@
         <v>53</v>
       </c>
       <c r="C65" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1449,7 +1455,7 @@
         <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,7 +1464,7 @@
         <v>55</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,7 +1473,7 @@
         <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1476,7 +1482,7 @@
         <v>57</v>
       </c>
       <c r="C69" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1485,7 +1491,7 @@
         <v>58</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1502,7 +1508,7 @@
         <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1511,7 +1517,7 @@
         <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1520,7 +1526,7 @@
         <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1529,7 +1535,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1546,7 +1552,7 @@
         <v>63</v>
       </c>
       <c r="C77" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1555,7 +1561,7 @@
         <v>64</v>
       </c>
       <c r="C78" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,7 +1570,7 @@
         <v>65</v>
       </c>
       <c r="C79" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1573,7 +1579,7 @@
         <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1582,7 +1588,7 @@
         <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1591,7 +1597,7 @@
         <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1600,7 +1606,7 @@
         <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1617,7 +1623,7 @@
         <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1634,7 +1640,7 @@
         <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1651,7 +1657,7 @@
         <v>72</v>
       </c>
       <c r="C89" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1668,7 +1674,7 @@
         <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1677,7 +1683,7 @@
         <v>74</v>
       </c>
       <c r="C92" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -1686,7 +1692,7 @@
         <v>75</v>
       </c>
       <c r="C93" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1695,7 +1701,7 @@
         <v>76</v>
       </c>
       <c r="C94" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,7 +1710,7 @@
         <v>77</v>
       </c>
       <c r="C95" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1713,7 +1719,7 @@
         <v>78</v>
       </c>
       <c r="C96" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -1730,7 +1736,7 @@
         <v>79</v>
       </c>
       <c r="C98" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -1739,7 +1745,7 @@
         <v>80</v>
       </c>
       <c r="C99" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -1748,7 +1754,7 @@
         <v>81</v>
       </c>
       <c r="C100" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -1765,7 +1771,7 @@
         <v>82</v>
       </c>
       <c r="C102" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1793,8 +1799,8 @@
   <dimension ref="A1:D510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A388" sqref="A388"/>
+      <pane ySplit="1" topLeftCell="A469" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1935,7 +1941,7 @@
       </c>
       <c r="C16" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="17" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1962,7 +1968,7 @@
       </c>
       <c r="C19" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="20" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1989,7 +1995,7 @@
       </c>
       <c r="C22" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="23" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2033,7 +2039,7 @@
       </c>
       <c r="C27" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="28" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2043,7 +2049,7 @@
       </c>
       <c r="C28" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="29" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2059,7 @@
       </c>
       <c r="C29" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="30" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2087,7 +2093,7 @@
       </c>
       <c r="C33" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="34" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2097,7 +2103,7 @@
       </c>
       <c r="C34" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="35" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2107,7 +2113,7 @@
       </c>
       <c r="C35" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="36" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2117,7 +2123,7 @@
       </c>
       <c r="C36" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="37" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2144,7 +2150,7 @@
       </c>
       <c r="C39" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="40" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2154,7 +2160,7 @@
       </c>
       <c r="C40" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="41" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2164,7 +2170,7 @@
       </c>
       <c r="C41" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="42" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2191,7 +2197,7 @@
       </c>
       <c r="C44" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="45" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2201,7 +2207,7 @@
       </c>
       <c r="C45" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="46" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2228,7 +2234,7 @@
       </c>
       <c r="C48" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="49" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2238,7 +2244,7 @@
       </c>
       <c r="C49" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="50" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2265,7 +2271,7 @@
       </c>
       <c r="C52" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="53" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2275,7 +2281,7 @@
       </c>
       <c r="C53" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="54" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2308,7 @@
       </c>
       <c r="C56" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="57" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2319,7 +2325,7 @@
       </c>
       <c r="C58" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="59" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2339,7 +2345,7 @@
       </c>
       <c r="C60" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="61" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2349,7 +2355,7 @@
       </c>
       <c r="C61" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="62" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2365,7 @@
       </c>
       <c r="C62" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="63" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2384,7 +2390,7 @@
       </c>
       <c r="C65" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="66" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2394,7 +2400,7 @@
       </c>
       <c r="C66" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="67" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2404,7 +2410,7 @@
       </c>
       <c r="C67" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="68" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2431,7 +2437,7 @@
       </c>
       <c r="C70" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="71" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2458,7 +2464,7 @@
       </c>
       <c r="C73" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="74" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2485,7 +2491,7 @@
       </c>
       <c r="C76" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="77" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2512,7 +2518,7 @@
       </c>
       <c r="C79" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="80" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2529,7 +2535,7 @@
       </c>
       <c r="C81" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="82" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2566,7 +2572,7 @@
       </c>
       <c r="C85" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="86" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2593,7 +2599,7 @@
       </c>
       <c r="C88" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="89" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2620,7 +2626,7 @@
       </c>
       <c r="C91" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="92" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2647,7 +2653,7 @@
       </c>
       <c r="C94" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="95" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2672,7 +2678,7 @@
       </c>
       <c r="C97" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="98" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2682,7 +2688,7 @@
       </c>
       <c r="C98" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="99" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2692,7 +2698,7 @@
       </c>
       <c r="C99" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="100" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2719,7 +2725,7 @@
       </c>
       <c r="C102" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="103" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2739,7 +2745,7 @@
       </c>
       <c r="C104" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="105" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2749,7 +2755,7 @@
       </c>
       <c r="C105" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="106" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2766,7 +2772,7 @@
       </c>
       <c r="C107" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="108" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2776,7 +2782,7 @@
       </c>
       <c r="C108" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="109" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2796,7 +2802,7 @@
       </c>
       <c r="C110" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="111" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2806,7 +2812,7 @@
       </c>
       <c r="C111" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="112" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2816,7 +2822,7 @@
       </c>
       <c r="C112" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="113" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2833,7 +2839,7 @@
       </c>
       <c r="C114" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="115" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2843,7 +2849,7 @@
       </c>
       <c r="C115" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="116" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2853,7 +2859,7 @@
       </c>
       <c r="C116" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="117" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2873,7 +2879,7 @@
       </c>
       <c r="C118" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="119" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2907,7 +2913,7 @@
       </c>
       <c r="C122" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="123" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2917,7 +2923,7 @@
       </c>
       <c r="C123" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="124" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2927,7 +2933,7 @@
       </c>
       <c r="C124" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="125" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2937,7 +2943,7 @@
       </c>
       <c r="C125" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="126" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2964,7 +2970,7 @@
       </c>
       <c r="C128" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2982,7 +2988,7 @@
       </c>
       <c r="C130" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="131" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2992,7 +2998,7 @@
       </c>
       <c r="C131" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="132" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3009,7 +3015,7 @@
       </c>
       <c r="C133" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="134" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3019,7 +3025,7 @@
       </c>
       <c r="C134" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="135" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3036,7 +3042,7 @@
       </c>
       <c r="C136" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="137" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3056,7 +3062,7 @@
       </c>
       <c r="C138" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="139" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3074,7 +3080,7 @@
       </c>
       <c r="C140" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="141" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3099,7 +3105,7 @@
       </c>
       <c r="C143" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="144" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3109,7 +3115,7 @@
       </c>
       <c r="C144" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="145" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3136,7 +3142,7 @@
       </c>
       <c r="C147" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="148" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3146,7 +3152,7 @@
       </c>
       <c r="C148" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="149" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3156,7 +3162,7 @@
       </c>
       <c r="C149" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="150" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3200,7 +3206,7 @@
       </c>
       <c r="C154" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="155" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3210,7 +3216,7 @@
       </c>
       <c r="C155" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="156" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3220,7 +3226,7 @@
       </c>
       <c r="C156" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="157" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3237,7 +3243,7 @@
       </c>
       <c r="C158" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="159" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3247,7 +3253,7 @@
       </c>
       <c r="C159" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="160" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3274,7 +3280,7 @@
       </c>
       <c r="C162" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="163" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3294,7 +3300,7 @@
       </c>
       <c r="C164" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="165" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3304,7 +3310,7 @@
       </c>
       <c r="C165" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="166" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3331,7 +3337,7 @@
       </c>
       <c r="C168" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="169" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3341,7 +3347,7 @@
       </c>
       <c r="C169" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="170" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3358,7 +3364,7 @@
       </c>
       <c r="C171" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="172" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3402,7 +3408,7 @@
       </c>
       <c r="C176" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="177" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3412,7 +3418,7 @@
       </c>
       <c r="C177" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="178" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3428,7 @@
       </c>
       <c r="C178" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="179" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3432,7 +3438,7 @@
       </c>
       <c r="C179" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="180" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3456,7 +3462,7 @@
       </c>
       <c r="C182" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="183" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3466,7 +3472,7 @@
       </c>
       <c r="C183" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="184" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3486,7 +3492,7 @@
       </c>
       <c r="C185" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="186" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3496,7 +3502,7 @@
       </c>
       <c r="C186" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="187" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3530,7 +3536,7 @@
       </c>
       <c r="C190" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="191" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3540,7 +3546,7 @@
       </c>
       <c r="C191" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="192" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3550,7 +3556,7 @@
       </c>
       <c r="C192" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="193" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3560,7 +3566,7 @@
       </c>
       <c r="C193" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="194" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3577,7 +3583,7 @@
       </c>
       <c r="C195" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="196" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3587,7 +3593,7 @@
       </c>
       <c r="C196" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="197" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3597,7 +3603,7 @@
       </c>
       <c r="C197" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="198" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3614,7 +3620,7 @@
       </c>
       <c r="C199" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="200" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3624,7 +3630,7 @@
       </c>
       <c r="C200" t="str">
         <f>'Versioni EJB'!C33</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="201" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3634,7 +3640,7 @@
       </c>
       <c r="C201" t="str">
         <f>'Versioni EJB'!C25</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="202" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3644,7 +3650,7 @@
       </c>
       <c r="C202" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="203" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3654,7 +3660,7 @@
       </c>
       <c r="C203" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="204" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3664,7 +3670,7 @@
       </c>
       <c r="C204" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="205" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3674,7 +3680,7 @@
       </c>
       <c r="C205" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="206" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3684,7 +3690,7 @@
       </c>
       <c r="C206" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="207" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3694,7 +3700,7 @@
       </c>
       <c r="C207" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="208" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3721,7 +3727,7 @@
       </c>
       <c r="C210" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="211" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3731,7 +3737,7 @@
       </c>
       <c r="C211" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="212" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3741,7 +3747,7 @@
       </c>
       <c r="C212" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="213" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3758,7 +3764,7 @@
       </c>
       <c r="C214" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="215" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3768,7 +3774,7 @@
       </c>
       <c r="C215" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="216" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3788,7 +3794,7 @@
       </c>
       <c r="C217" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="218" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3798,7 +3804,7 @@
       </c>
       <c r="C218" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="219" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3808,7 +3814,7 @@
       </c>
       <c r="C219" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="220" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3818,7 +3824,7 @@
       </c>
       <c r="C220" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="221" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3828,7 +3834,7 @@
       </c>
       <c r="C221" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="222" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3845,7 +3851,7 @@
       </c>
       <c r="C223" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="224" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3855,7 +3861,7 @@
       </c>
       <c r="C224" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="225" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3865,7 +3871,7 @@
       </c>
       <c r="C225" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="226" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3875,7 +3881,7 @@
       </c>
       <c r="C226" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="227" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3885,7 +3891,7 @@
       </c>
       <c r="C227" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="228" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3895,7 +3901,7 @@
       </c>
       <c r="C228" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="229" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3915,7 +3921,7 @@
       </c>
       <c r="C230" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="231" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3925,7 +3931,7 @@
       </c>
       <c r="C231" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="232" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3959,7 +3965,7 @@
       </c>
       <c r="C235" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="236" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3969,7 +3975,7 @@
       </c>
       <c r="C236" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="237" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3979,7 +3985,7 @@
       </c>
       <c r="C237" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="238" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3989,7 +3995,7 @@
       </c>
       <c r="C238" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="239" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3999,7 +4005,7 @@
       </c>
       <c r="C239" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="240" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4009,7 +4015,7 @@
       </c>
       <c r="C240" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="241" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4019,7 +4025,7 @@
       </c>
       <c r="C241" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="242" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4029,7 +4035,7 @@
       </c>
       <c r="C242" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="243" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4056,7 +4062,7 @@
       </c>
       <c r="C245" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="246" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4066,7 +4072,7 @@
       </c>
       <c r="C246" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="247" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4076,7 +4082,7 @@
       </c>
       <c r="C247" t="str">
         <f>'Versioni EJB'!C19</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="248" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4086,7 +4092,7 @@
       </c>
       <c r="C248" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="249" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4096,7 +4102,7 @@
       </c>
       <c r="C249" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="250" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4106,7 +4112,7 @@
       </c>
       <c r="C250" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="251" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4116,7 +4122,7 @@
       </c>
       <c r="C251" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="252" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4126,7 +4132,7 @@
       </c>
       <c r="C252" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="253" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4136,7 +4142,7 @@
       </c>
       <c r="C253" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="254" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4146,7 +4152,7 @@
       </c>
       <c r="C254" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="255" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4156,7 +4162,7 @@
       </c>
       <c r="C255" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="256" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4173,7 +4179,7 @@
       </c>
       <c r="C257" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="258" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4183,7 +4189,7 @@
       </c>
       <c r="C258" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="259" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4203,7 +4209,7 @@
       </c>
       <c r="C260" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="261" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4213,7 +4219,7 @@
       </c>
       <c r="C261" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="262" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4223,7 +4229,7 @@
       </c>
       <c r="C262" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="263" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4233,7 +4239,7 @@
       </c>
       <c r="C263" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="264" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4250,7 +4256,7 @@
       </c>
       <c r="C265" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="266" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4260,7 +4266,7 @@
       </c>
       <c r="C266" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="267" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4270,7 +4276,7 @@
       </c>
       <c r="C267" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="268" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4290,7 +4296,7 @@
       </c>
       <c r="C269" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="270" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4300,7 +4306,7 @@
       </c>
       <c r="C270" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="271" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4317,7 +4323,7 @@
       </c>
       <c r="C272" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="273" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4327,7 +4333,7 @@
       </c>
       <c r="C273" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="274" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4337,7 +4343,7 @@
       </c>
       <c r="C274" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="275" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4357,7 +4363,7 @@
       </c>
       <c r="C276" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="277" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4367,7 +4373,7 @@
       </c>
       <c r="C277" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="278" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4394,7 +4400,7 @@
       </c>
       <c r="C280" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="281" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4404,7 +4410,7 @@
       </c>
       <c r="C281" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="282" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4414,7 +4420,7 @@
       </c>
       <c r="C282" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="283" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4424,7 +4430,7 @@
       </c>
       <c r="C283" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="284" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4434,7 +4440,7 @@
       </c>
       <c r="C284" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="285" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4444,7 +4450,7 @@
       </c>
       <c r="C285" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="286" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4454,7 +4460,7 @@
       </c>
       <c r="C286" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="287" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4464,7 +4470,7 @@
       </c>
       <c r="C287" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="288" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4481,7 +4487,7 @@
       </c>
       <c r="C289" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="290" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4491,7 +4497,7 @@
       </c>
       <c r="C290" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="291" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4501,7 +4507,7 @@
       </c>
       <c r="C291" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="292" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4511,7 +4517,7 @@
       </c>
       <c r="C292" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="293" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4531,7 +4537,7 @@
       </c>
       <c r="C294" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="295" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4541,7 +4547,7 @@
       </c>
       <c r="C295" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="296" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4551,7 +4557,7 @@
       </c>
       <c r="C296" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="297" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4568,7 +4574,7 @@
       </c>
       <c r="C298" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="299" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4588,7 +4594,7 @@
       </c>
       <c r="C300" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="301" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4598,7 +4604,7 @@
       </c>
       <c r="C301" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="302" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4632,7 +4638,7 @@
       </c>
       <c r="C305" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="306" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4642,7 +4648,7 @@
       </c>
       <c r="C306" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="307" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4652,7 +4658,7 @@
       </c>
       <c r="C307" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="308" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4662,7 +4668,7 @@
       </c>
       <c r="C308" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="309" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4672,7 +4678,7 @@
       </c>
       <c r="C309" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="310" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4682,7 +4688,7 @@
       </c>
       <c r="C310" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="311" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4692,7 +4698,7 @@
       </c>
       <c r="C311" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="312" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4709,7 +4715,7 @@
       </c>
       <c r="C313" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="314" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4719,7 +4725,7 @@
       </c>
       <c r="C314" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="315" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4729,7 +4735,7 @@
       </c>
       <c r="C315" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.20.0-env-svis-SNAPSHOT</v>
+        <v>1.26.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="316" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4739,7 +4745,7 @@
       </c>
       <c r="C316" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="317" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4749,7 +4755,7 @@
       </c>
       <c r="C317" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="318" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4759,7 +4765,7 @@
       </c>
       <c r="C318" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="319" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4769,7 +4775,7 @@
       </c>
       <c r="C319" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="320" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4779,7 +4785,7 @@
       </c>
       <c r="C320" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="321" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4789,7 +4795,7 @@
       </c>
       <c r="C321" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="322" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4799,7 +4805,7 @@
       </c>
       <c r="C322" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="323" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4809,7 +4815,7 @@
       </c>
       <c r="C323" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="324" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4826,7 +4832,7 @@
       </c>
       <c r="C325" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="326" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4836,7 +4842,7 @@
       </c>
       <c r="C326" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="327" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4846,7 +4852,7 @@
       </c>
       <c r="C327" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="328" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4866,7 +4872,7 @@
       </c>
       <c r="C329" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="330" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4876,7 +4882,7 @@
       </c>
       <c r="C330" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svis-SNAPSHOT</v>
+        <v>1.71.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="331" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4893,7 +4899,7 @@
       </c>
       <c r="C332" t="str">
         <f>'Versioni EJB'!C61</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.53.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="333" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4903,7 +4909,7 @@
       </c>
       <c r="C333" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svis-SNAPSHOT</v>
+        <v>1.71.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="334" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4913,7 +4919,7 @@
       </c>
       <c r="C334" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="335" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4923,7 +4929,7 @@
       </c>
       <c r="C335" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="336" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4933,7 +4939,7 @@
       </c>
       <c r="C336" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="337" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4943,7 +4949,7 @@
       </c>
       <c r="C337" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="338" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4953,7 +4959,7 @@
       </c>
       <c r="C338" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="339" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4997,7 +5003,7 @@
       </c>
       <c r="C343" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="344" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5007,7 +5013,7 @@
       </c>
       <c r="C344" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="345" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5017,7 +5023,7 @@
       </c>
       <c r="C345" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="346" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5044,7 +5050,7 @@
       </c>
       <c r="C348" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="349" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5054,7 +5060,7 @@
       </c>
       <c r="C349" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="350" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5064,7 +5070,7 @@
       </c>
       <c r="C350" t="str">
         <f>'Versioni EJB'!C8</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="351" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5081,7 +5087,7 @@
       </c>
       <c r="C352" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="353" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5091,7 +5097,7 @@
       </c>
       <c r="C353" t="str">
         <f>'Versioni EJB'!C33</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="354" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5101,7 +5107,7 @@
       </c>
       <c r="C354" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="355" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5121,7 +5127,7 @@
       </c>
       <c r="C356" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="357" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5138,7 +5144,7 @@
       </c>
       <c r="C358" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="359" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5148,7 +5154,7 @@
       </c>
       <c r="C359" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="360" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5168,7 +5174,7 @@
       </c>
       <c r="C361" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="362" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5185,7 +5191,7 @@
       </c>
       <c r="C363" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="364" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5205,7 +5211,7 @@
       </c>
       <c r="C365" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="366" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5215,7 +5221,7 @@
       </c>
       <c r="C366" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="367" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5225,7 +5231,7 @@
       </c>
       <c r="C367" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="368" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5242,7 +5248,7 @@
       </c>
       <c r="C369" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="370" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5262,7 +5268,7 @@
       </c>
       <c r="C371" t="str">
         <f>'Versioni EJB'!C61</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.53.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="372" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5272,7 +5278,7 @@
       </c>
       <c r="C372" t="str">
         <f>'Versioni EJB'!C44</f>
-        <v>1.39.0-env-svis-SNAPSHOT</v>
+        <v>1.42.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="373" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5282,7 +5288,7 @@
       </c>
       <c r="C373" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.70.0-env-svis-SNAPSHOT</v>
+        <v>1.71.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="374" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5292,7 +5298,7 @@
       </c>
       <c r="C374" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="375" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5302,7 +5308,7 @@
       </c>
       <c r="C375" t="str">
         <f>'Versioni EJB'!C66</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="376" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5312,7 +5318,7 @@
       </c>
       <c r="C376" t="str">
         <f>'Versioni EJB'!C69</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="377" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5322,7 +5328,7 @@
       </c>
       <c r="C377" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="378" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5332,7 +5338,7 @@
       </c>
       <c r="C378" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="379" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5342,7 +5348,7 @@
       </c>
       <c r="C379" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="380" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5352,7 +5358,7 @@
       </c>
       <c r="C380" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="381" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5369,7 +5375,7 @@
       </c>
       <c r="C382" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="383" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5389,7 +5395,7 @@
       </c>
       <c r="C384" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="385" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5399,7 +5405,7 @@
       </c>
       <c r="C385" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="386" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5423,7 +5429,7 @@
       </c>
       <c r="C388" t="str">
         <f>'Versioni EJB'!C5</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="389" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5433,7 +5439,7 @@
       </c>
       <c r="C389" t="str">
         <f>'Versioni EJB'!C43</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="390" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5443,7 +5449,7 @@
       </c>
       <c r="C390" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="391" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5453,7 +5459,7 @@
       </c>
       <c r="C391" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="392" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5463,7 +5469,7 @@
       </c>
       <c r="C392" t="str">
         <f>'Versioni EJB'!C56</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="393" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5473,7 +5479,7 @@
       </c>
       <c r="C393" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="394" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5515,7 +5521,7 @@
       </c>
       <c r="C398" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="399" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5525,7 +5531,7 @@
       </c>
       <c r="C399" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="400" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5535,7 +5541,7 @@
       </c>
       <c r="C400" t="str">
         <f>'Versioni EJB'!C85</f>
-        <v>1.20.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="401" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5545,7 +5551,7 @@
       </c>
       <c r="C401" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="402" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5555,7 +5561,7 @@
       </c>
       <c r="C402" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.20.0-env-svis-SNAPSHOT</v>
+        <v>1.26.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="403" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5565,7 +5571,7 @@
       </c>
       <c r="C403" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="404" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5575,7 +5581,7 @@
       </c>
       <c r="C404" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="405" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5585,7 +5591,7 @@
       </c>
       <c r="C405" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="406" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5595,7 +5601,7 @@
       </c>
       <c r="C406" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="407" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5605,7 +5611,7 @@
       </c>
       <c r="C407" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="408" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5639,7 +5645,7 @@
       </c>
       <c r="C411" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="412" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5649,7 +5655,7 @@
       </c>
       <c r="C412" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.202.0-env-svis-SNAPSHOT</v>
+        <v>1.205.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="413" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5659,7 +5665,7 @@
       </c>
       <c r="C413" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="414" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5679,7 +5685,7 @@
       </c>
       <c r="C415" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="416" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5689,7 +5695,7 @@
       </c>
       <c r="C416" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="417" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5723,7 +5729,7 @@
       </c>
       <c r="C420" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="421" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5733,7 +5739,7 @@
       </c>
       <c r="C421" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.138.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="422" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5743,7 +5749,7 @@
       </c>
       <c r="C422" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="423" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5753,7 +5759,7 @@
       </c>
       <c r="C423" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="424" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5763,7 +5769,7 @@
       </c>
       <c r="C424" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="425" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5780,7 +5786,7 @@
       </c>
       <c r="C426" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="427" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5790,7 +5796,7 @@
       </c>
       <c r="C427" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.202.0-env-svis-SNAPSHOT</v>
+        <v>1.205.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="428" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5800,7 +5806,7 @@
       </c>
       <c r="C428" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="429" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5810,7 +5816,7 @@
       </c>
       <c r="C429" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="430" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5820,7 +5826,7 @@
       </c>
       <c r="C430" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="431" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5830,7 +5836,7 @@
       </c>
       <c r="C431" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="432" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5857,7 +5863,7 @@
       </c>
       <c r="C434" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.138.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="435" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5867,7 +5873,7 @@
       </c>
       <c r="C435" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="436" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5877,7 +5883,7 @@
       </c>
       <c r="C436" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="437" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5887,7 +5893,7 @@
       </c>
       <c r="C437" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="438" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -5914,7 +5920,7 @@
       </c>
       <c r="C440" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.202.0-env-svis-SNAPSHOT</v>
+        <v>1.205.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="441" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5924,7 +5930,7 @@
       </c>
       <c r="C441" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="442" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5934,7 +5940,7 @@
       </c>
       <c r="C442" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="443" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5944,7 +5950,7 @@
       </c>
       <c r="C443" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="444" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5954,7 +5960,7 @@
       </c>
       <c r="C444" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="445" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5964,7 +5970,7 @@
       </c>
       <c r="C445" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.20.0-env-svis-SNAPSHOT</v>
+        <v>1.26.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="446" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5974,7 +5980,7 @@
       </c>
       <c r="C446" t="str">
         <f>'Versioni EJB'!C19</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="447" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5984,7 +5990,7 @@
       </c>
       <c r="C447" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="448" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5994,7 +6000,7 @@
       </c>
       <c r="C448" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="449" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6004,7 +6010,7 @@
       </c>
       <c r="C449" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="450" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6014,7 +6020,7 @@
       </c>
       <c r="C450" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="451" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6024,7 +6030,7 @@
       </c>
       <c r="C451" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="452" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6034,7 +6040,7 @@
       </c>
       <c r="C452" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="453" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6044,7 +6050,7 @@
       </c>
       <c r="C453" t="str">
         <f>'Versioni EJB'!C52</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="454" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6054,7 +6060,7 @@
       </c>
       <c r="C454" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="455" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6071,7 +6077,7 @@
       </c>
       <c r="C456" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="457" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6081,7 +6087,7 @@
       </c>
       <c r="C457" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="458" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6091,7 +6097,7 @@
       </c>
       <c r="C458" t="str">
         <f>'Versioni EJB'!C24</f>
-        <v>1.20.0-env-svis-SNAPSHOT</v>
+        <v>1.26.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="459" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6101,7 +6107,7 @@
       </c>
       <c r="C459" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="460" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6121,7 +6127,7 @@
       </c>
       <c r="C461" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="462" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6131,7 +6137,7 @@
       </c>
       <c r="C462" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.138.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="463" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6148,7 +6154,7 @@
       </c>
       <c r="C464" t="str">
         <f>'Versioni EJB'!C89</f>
-        <v>1.136.0-env-svis-SNAPSHOT</v>
+        <v>1.138.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="465" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6158,7 +6164,7 @@
       </c>
       <c r="C465" t="str">
         <f>'Versioni EJB'!C12</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.50.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="466" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6168,7 +6174,7 @@
       </c>
       <c r="C466" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="467" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6178,7 +6184,7 @@
       </c>
       <c r="C467" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="468" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6188,7 +6194,7 @@
       </c>
       <c r="C468" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="469" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6212,7 +6218,7 @@
       </c>
       <c r="C471" t="str">
         <f>'Versioni EJB'!C80</f>
-        <v>1.40.0-env-svis-SNAPSHOT</v>
+        <v>1.41.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="472" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6222,7 +6228,7 @@
       </c>
       <c r="C472" t="str">
         <f>'Versioni EJB'!C79</f>
-        <v>1.27.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="473" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6232,7 +6238,7 @@
       </c>
       <c r="C473" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="474" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6242,7 +6248,7 @@
       </c>
       <c r="C474" t="str">
         <f>'Versioni EJB'!C59</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="475" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6252,7 +6258,7 @@
       </c>
       <c r="C475" t="str">
         <f>'Versioni EJB'!C77</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="476" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6262,7 +6268,7 @@
       </c>
       <c r="C476" t="str">
         <f>'Versioni EJB'!C25</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="477" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6272,7 +6278,7 @@
       </c>
       <c r="C477" t="str">
         <f>'Versioni EJB'!C57</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="478" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6282,7 +6288,7 @@
       </c>
       <c r="C478" t="str">
         <f>'Versioni EJB'!C96</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="479" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6292,7 +6298,7 @@
       </c>
       <c r="C479" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="480" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6302,7 +6308,7 @@
       </c>
       <c r="C480" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="481" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6312,7 +6318,7 @@
       </c>
       <c r="C481" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="482" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6322,7 +6328,7 @@
       </c>
       <c r="C482" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="483" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6349,7 +6355,7 @@
       </c>
       <c r="C485" t="str">
         <f>'Versioni EJB'!C94</f>
-        <v>1.120.0-env-svis-SNAPSHOT</v>
+        <v>1.122.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="486" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6359,7 +6365,7 @@
       </c>
       <c r="C486" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.202.0-env-svis-SNAPSHOT</v>
+        <v>1.205.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="487" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6369,7 +6375,7 @@
       </c>
       <c r="C487" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="488" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6379,7 +6385,7 @@
       </c>
       <c r="C488" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.15.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="489" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6389,7 +6395,7 @@
       </c>
       <c r="C489" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="490" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6399,7 +6405,7 @@
       </c>
       <c r="C490" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="491" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6409,7 +6415,7 @@
       </c>
       <c r="C491" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="492" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6426,7 +6432,7 @@
       </c>
       <c r="C493" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="494" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6436,7 +6442,7 @@
       </c>
       <c r="C494" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.34.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="495" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6446,7 +6452,7 @@
       </c>
       <c r="C495" t="str">
         <f>'Versioni EJB'!C94</f>
-        <v>1.120.0-env-svis-SNAPSHOT</v>
+        <v>1.122.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="496" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6456,7 +6462,7 @@
       </c>
       <c r="C496" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="497" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6480,7 +6486,7 @@
       </c>
       <c r="C499" t="str">
         <f>'Versioni EJB'!C87</f>
-        <v>1.202.0-env-svis-SNAPSHOT</v>
+        <v>1.205.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="500" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6490,7 +6496,7 @@
       </c>
       <c r="C500" t="str">
         <f>'Versioni EJB'!C99</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="501" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6500,7 +6506,7 @@
       </c>
       <c r="C501" t="str">
         <f>'Versioni EJB'!C59</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="502" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6510,7 +6516,7 @@
       </c>
       <c r="C502" t="str">
         <f>'Versioni EJB'!C57</f>
-        <v>1.7.0-env-svis-SNAPSHOT</v>
+        <v>1.8.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="503" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6520,7 +6526,7 @@
       </c>
       <c r="C503" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="504" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6530,7 +6536,7 @@
       </c>
       <c r="C504" t="str">
         <f>'Versioni EJB'!C96</f>
-        <v>1.6.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="505" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6540,7 +6546,7 @@
       </c>
       <c r="C505" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="506" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6550,7 +6556,7 @@
       </c>
       <c r="C506" t="str">
         <f>'Versioni EJB'!C42</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="507" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6560,7 +6566,7 @@
       </c>
       <c r="C507" t="str">
         <f>'Versioni EJB'!C18</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="508" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6570,7 +6576,7 @@
       </c>
       <c r="C508" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.22.0-env-svis-SNAPSHOT</v>
+        <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="509" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6580,7 +6586,7 @@
       </c>
       <c r="C509" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.7.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
     <row r="510" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6590,7 +6596,7 @@
       </c>
       <c r="C510" t="str">
         <f>'Versioni EJB'!C35</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
   </sheetData>
@@ -6598,6 +6604,11 @@
     <sortCondition ref="B16"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="A497:C497"/>
     <mergeCell ref="A469:C469"/>
     <mergeCell ref="A151:C151"/>
@@ -6611,11 +6622,6 @@
     <mergeCell ref="A187:C187"/>
     <mergeCell ref="A180:C180"/>
     <mergeCell ref="A173:C173"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiornamento file supporto per allineamento di env/svia
</commit_message>
<xml_diff>
--- a/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
+++ b/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openshift\SoftwareAllineamenti\src\main\resources\excelutils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BD7ADD-C4E4-4B01-AEC2-98D39D406622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9579BD6-5D00-4F77-9486-6910ABDA9F01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="15990" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{ED1ED9CF-A468-4C7A-9A72-2CE304B78EA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Versioni EJB" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="147">
   <si>
     <t>isp-ib-om</t>
   </si>
@@ -366,60 +366,6 @@
     <t>VERSIONE SVIS/SVIA</t>
   </si>
   <si>
-    <t>1.10.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.8.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.48.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.12.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.9.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.11.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.14.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.15.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.17.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.16.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.13.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.18.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.21.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.23.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.71.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.25.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.28.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.49.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>wishlist-ejb</t>
   </si>
   <si>
@@ -435,58 +381,103 @@
     <t>catalogo-prodotti-ejb</t>
   </si>
   <si>
-    <t>1.4.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.5.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.52.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.20.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>0.34.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
     <t>Blocco 19</t>
   </si>
   <si>
-    <t>1.43.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.19.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.55.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.72.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.29.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.30.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.206.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.140.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.33.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.123.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.40.0-env-svis-SNAPSHOT</t>
-  </si>
-  <si>
-    <t>1.51.0-env-svis-SNAPSHOT</t>
+    <t>1.14.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.9.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.11.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.4.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.12.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.10.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.5.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.54.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.13.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.16.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.33.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.18.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.22.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.17.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>0.34.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.23.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.19.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.43.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.55.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.28.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.15.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.72.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.21.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.30.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.8.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.49.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.206.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.140.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.34.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.124.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.40.0-env-svia-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>1.51.0-env-svia-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -884,7 +875,7 @@
   <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -931,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -940,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -949,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,16 +949,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -976,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -985,16 +976,16 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1011,7 +1002,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1020,7 +1011,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1029,7 +1020,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1046,7 +1037,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1072,7 +1063,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1081,7 +1072,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1090,7 +1081,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1099,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1108,7 +1099,7 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1117,7 +1108,7 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1126,7 +1117,7 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1141,10 +1132,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1153,7 +1144,7 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1162,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1179,7 +1170,7 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1188,7 +1179,7 @@
         <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1197,16 +1188,16 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1215,7 +1206,7 @@
         <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1224,7 +1215,7 @@
         <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1233,7 +1224,7 @@
         <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1242,7 +1233,7 @@
         <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1260,7 +1251,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1269,7 +1260,7 @@
         <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1278,7 +1269,7 @@
         <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1295,7 +1286,7 @@
         <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1304,7 +1295,7 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1313,7 +1304,7 @@
         <v>36</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1322,7 +1313,7 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1331,7 +1322,7 @@
         <v>37</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1340,7 +1331,7 @@
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1349,7 +1340,7 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,7 +1357,7 @@
         <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1375,7 +1366,7 @@
         <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1384,7 +1375,7 @@
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1393,7 +1384,7 @@
         <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1410,7 +1401,7 @@
         <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1427,7 +1418,7 @@
         <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1444,7 +1435,7 @@
         <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1453,7 +1444,7 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1462,7 +1453,7 @@
         <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1471,7 +1462,7 @@
         <v>53</v>
       </c>
       <c r="C65" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1480,7 +1471,7 @@
         <v>47</v>
       </c>
       <c r="C66" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1489,7 +1480,7 @@
         <v>48</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1498,7 +1489,7 @@
         <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1507,7 +1498,7 @@
         <v>50</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1524,7 +1515,7 @@
         <v>52</v>
       </c>
       <c r="C71" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1533,7 +1524,7 @@
         <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1542,7 +1533,7 @@
         <v>56</v>
       </c>
       <c r="C73" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1551,7 +1542,7 @@
         <v>57</v>
       </c>
       <c r="C74" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1560,7 +1551,7 @@
         <v>58</v>
       </c>
       <c r="C75" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1577,7 +1568,7 @@
         <v>59</v>
       </c>
       <c r="C77" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1586,7 +1577,7 @@
         <v>60</v>
       </c>
       <c r="C78" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1595,7 +1586,7 @@
         <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1604,7 +1595,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1621,7 +1612,7 @@
         <v>63</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1630,16 +1621,16 @@
         <v>64</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C84" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1648,7 +1639,7 @@
         <v>65</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1657,7 +1648,7 @@
         <v>66</v>
       </c>
       <c r="C86" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1666,7 +1657,7 @@
         <v>67</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1675,7 +1666,7 @@
         <v>68</v>
       </c>
       <c r="C88" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -1684,7 +1675,7 @@
         <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1701,7 +1692,7 @@
         <v>70</v>
       </c>
       <c r="C91" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1718,7 +1709,7 @@
         <v>71</v>
       </c>
       <c r="C93" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1735,7 +1726,7 @@
         <v>72</v>
       </c>
       <c r="C95" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,7 +1743,7 @@
         <v>73</v>
       </c>
       <c r="C97" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -1770,7 +1761,7 @@
         <v>75</v>
       </c>
       <c r="C99" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -1779,7 +1770,7 @@
         <v>76</v>
       </c>
       <c r="C100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -1788,7 +1779,7 @@
         <v>77</v>
       </c>
       <c r="C101" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -1797,7 +1788,7 @@
         <v>78</v>
       </c>
       <c r="C102" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -1814,7 +1805,7 @@
         <v>79</v>
       </c>
       <c r="C104" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -1823,7 +1814,7 @@
         <v>80</v>
       </c>
       <c r="C105" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -1832,7 +1823,7 @@
         <v>81</v>
       </c>
       <c r="C106" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -1849,7 +1840,7 @@
         <v>82</v>
       </c>
       <c r="C108" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1878,8 +1869,8 @@
   <dimension ref="A1:D525"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B514" sqref="B514"/>
+      <pane ySplit="1" topLeftCell="A478" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C362" sqref="C362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1931,7 +1922,7 @@
       </c>
       <c r="C5" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="6" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1948,7 +1939,7 @@
       </c>
       <c r="C7" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="8" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1967,7 +1958,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1980,7 +1971,7 @@
       </c>
       <c r="C11" s="7" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="12" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -1997,7 +1988,7 @@
       </c>
       <c r="C13" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="14" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
@@ -2014,12 +2005,12 @@
       </c>
       <c r="C15" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="16" spans="1:4" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2032,7 +2023,7 @@
       </c>
       <c r="C17" s="7" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="18" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2056,7 +2047,7 @@
       </c>
       <c r="C20" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="21" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2066,7 +2057,7 @@
       </c>
       <c r="C21" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="22" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2083,7 +2074,7 @@
       </c>
       <c r="C23" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="24" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2093,7 +2084,7 @@
       </c>
       <c r="C24" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="25" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2110,7 +2101,7 @@
       </c>
       <c r="C26" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="27" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2120,7 +2111,7 @@
       </c>
       <c r="C27" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="28" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2144,7 +2135,7 @@
       </c>
       <c r="C30" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="31" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2154,7 +2145,7 @@
       </c>
       <c r="C31" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="32" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2164,7 +2155,7 @@
       </c>
       <c r="C32" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="33" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2174,7 +2165,7 @@
       </c>
       <c r="C33" t="str">
         <f>'Versioni EJB'!C10</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="34" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2198,7 +2189,7 @@
       </c>
       <c r="C36" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="37" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2208,7 +2199,7 @@
       </c>
       <c r="C37" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="38" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2218,7 +2209,7 @@
       </c>
       <c r="C38" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="39" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2228,7 +2219,7 @@
       </c>
       <c r="C39" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="40" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2238,7 +2229,7 @@
       </c>
       <c r="C40" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="41" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2255,7 +2246,7 @@
       </c>
       <c r="C42" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="43" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2265,7 +2256,7 @@
       </c>
       <c r="C43" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="44" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2275,7 +2266,7 @@
       </c>
       <c r="C44" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="45" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2285,7 +2276,7 @@
       </c>
       <c r="C45" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="46" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2293,7 @@
       </c>
       <c r="C47" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2312,7 +2303,7 @@
       </c>
       <c r="C48" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="49" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2322,7 +2313,7 @@
       </c>
       <c r="C49" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="50" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2339,7 +2330,7 @@
       </c>
       <c r="C51" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="52" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2349,7 +2340,7 @@
       </c>
       <c r="C52" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="53" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2359,7 +2350,7 @@
       </c>
       <c r="C53" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="54" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2376,7 +2367,7 @@
       </c>
       <c r="C55" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="56" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2386,7 +2377,7 @@
       </c>
       <c r="C56" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="57" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2396,7 +2387,7 @@
       </c>
       <c r="C57" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="58" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2413,7 +2404,7 @@
       </c>
       <c r="C59" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="60" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2423,7 +2414,7 @@
       </c>
       <c r="C60" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="61" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2440,7 +2431,7 @@
       </c>
       <c r="C62" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="63" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2450,7 +2441,7 @@
       </c>
       <c r="C63" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="64" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2467,7 +2458,7 @@
       </c>
       <c r="C65" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="66" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2477,7 +2468,7 @@
       </c>
       <c r="C66" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="67" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2487,7 +2478,7 @@
       </c>
       <c r="C67" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="68" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2497,7 +2488,7 @@
       </c>
       <c r="C68" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="69" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2507,7 +2498,7 @@
       </c>
       <c r="C69" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="70" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2532,7 +2523,7 @@
       </c>
       <c r="C72" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="73" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2542,7 +2533,7 @@
       </c>
       <c r="C73" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="74" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2552,12 +2543,12 @@
       </c>
       <c r="C74" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="75" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2569,7 +2560,7 @@
       </c>
       <c r="C76" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="77" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2579,7 +2570,7 @@
       </c>
       <c r="C77" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="78" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2596,7 +2587,7 @@
       </c>
       <c r="C79" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="80" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2606,7 +2597,7 @@
       </c>
       <c r="C80" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="81" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2623,7 +2614,7 @@
       </c>
       <c r="C82" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="83" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2633,7 +2624,7 @@
       </c>
       <c r="C83" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="84" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2657,7 +2648,7 @@
       </c>
       <c r="C86" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="87" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2667,7 +2658,7 @@
       </c>
       <c r="C87" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="88" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2684,7 +2675,7 @@
       </c>
       <c r="C89" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="90" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2694,7 +2685,7 @@
       </c>
       <c r="C90" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="91" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2711,7 +2702,7 @@
       </c>
       <c r="C92" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="93" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2721,12 +2712,12 @@
       </c>
       <c r="C93" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="94" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2738,7 +2729,7 @@
       </c>
       <c r="C95" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="96" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2748,7 +2739,7 @@
       </c>
       <c r="C96" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="97" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2765,7 +2756,7 @@
       </c>
       <c r="C98" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="99" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2766,7 @@
       </c>
       <c r="C99" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="100" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2792,7 +2783,7 @@
       </c>
       <c r="C101" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="102" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2802,7 +2793,7 @@
       </c>
       <c r="C102" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="103" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2819,7 +2810,7 @@
       </c>
       <c r="C104" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="105" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2829,7 +2820,7 @@
       </c>
       <c r="C105" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="106" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2846,7 +2837,7 @@
       </c>
       <c r="C107" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="108" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2856,7 +2847,7 @@
       </c>
       <c r="C108" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="109" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2881,7 +2872,7 @@
       </c>
       <c r="C111" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="112" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2891,7 +2882,7 @@
       </c>
       <c r="C112" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="113" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2901,7 +2892,7 @@
       </c>
       <c r="C113" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="114" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2911,7 +2902,7 @@
       </c>
       <c r="C114" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="115" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2928,7 +2919,7 @@
       </c>
       <c r="C116" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="117" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2938,7 +2929,7 @@
       </c>
       <c r="C117" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="118" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2948,7 +2939,7 @@
       </c>
       <c r="C118" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="119" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2958,7 +2949,7 @@
       </c>
       <c r="C119" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="120" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -2975,7 +2966,7 @@
       </c>
       <c r="C121" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="122" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2985,7 +2976,7 @@
       </c>
       <c r="C122" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="123" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2995,7 +2986,7 @@
       </c>
       <c r="C123" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="124" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3005,7 +2996,7 @@
       </c>
       <c r="C124" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="125" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3015,7 +3006,7 @@
       </c>
       <c r="C125" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="126" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3025,7 +3016,7 @@
       </c>
       <c r="C126" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="127" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3042,7 +3033,7 @@
       </c>
       <c r="C128" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3052,7 +3043,7 @@
       </c>
       <c r="C129" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="130" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3062,7 +3053,7 @@
       </c>
       <c r="C130" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="131" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3072,7 +3063,7 @@
       </c>
       <c r="C131" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="132" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3082,7 +3073,7 @@
       </c>
       <c r="C132" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="133" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3106,7 +3097,7 @@
       </c>
       <c r="C135" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="136" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3116,7 +3107,7 @@
       </c>
       <c r="C136" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="137" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3126,7 +3117,7 @@
       </c>
       <c r="C137" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="138" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3136,7 +3127,7 @@
       </c>
       <c r="C138" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="139" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3146,7 +3137,7 @@
       </c>
       <c r="C139" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="140" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3163,7 +3154,7 @@
       </c>
       <c r="C141" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="142" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3173,7 +3164,7 @@
       </c>
       <c r="C142" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="143" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3191,7 +3182,7 @@
       </c>
       <c r="C144" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="145" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3201,7 +3192,7 @@
       </c>
       <c r="C145" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="146" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3218,7 +3209,7 @@
       </c>
       <c r="C147" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="148" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3228,7 +3219,7 @@
       </c>
       <c r="C148" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="149" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3245,7 +3236,7 @@
       </c>
       <c r="C150" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="151" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3255,7 +3246,7 @@
       </c>
       <c r="C151" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="152" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3265,7 +3256,7 @@
       </c>
       <c r="C152" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="153" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3275,7 +3266,7 @@
       </c>
       <c r="C153" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="154" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3285,7 +3276,7 @@
       </c>
       <c r="C154" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="155" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3295,7 +3286,7 @@
       </c>
       <c r="C155" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="156" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3312,7 +3303,7 @@
       </c>
       <c r="C157" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="158" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3322,7 +3313,7 @@
       </c>
       <c r="C158" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="159" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3332,7 +3323,7 @@
       </c>
       <c r="C159" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="160" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3350,7 +3341,7 @@
       </c>
       <c r="C161" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="162" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3375,7 +3366,7 @@
       </c>
       <c r="C164" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="165" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3385,7 +3376,7 @@
       </c>
       <c r="C165" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="166" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3395,7 +3386,7 @@
       </c>
       <c r="C166" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="167" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3412,7 +3403,7 @@
       </c>
       <c r="C168" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="169" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3413,7 @@
       </c>
       <c r="C169" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="170" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3432,7 +3423,7 @@
       </c>
       <c r="C170" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="171" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3442,7 +3433,7 @@
       </c>
       <c r="C171" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="172" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3466,7 +3457,7 @@
       </c>
       <c r="C174" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="175" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3476,7 +3467,7 @@
       </c>
       <c r="C175" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="176" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3486,7 +3477,7 @@
       </c>
       <c r="C176" t="str">
         <f>'Versioni EJB'!C46</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="177" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3496,7 +3487,7 @@
       </c>
       <c r="C177" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="178" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3513,7 +3504,7 @@
       </c>
       <c r="C179" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="180" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3523,7 +3514,7 @@
       </c>
       <c r="C180" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="181" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3533,7 +3524,7 @@
       </c>
       <c r="C181" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="182" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3543,7 +3534,7 @@
       </c>
       <c r="C182" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="183" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3560,7 +3551,7 @@
       </c>
       <c r="C184" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="185" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3570,7 +3561,7 @@
       </c>
       <c r="C185" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="186" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3580,7 +3571,7 @@
       </c>
       <c r="C186" t="str">
         <f>'Versioni EJB'!C46</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="187" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3597,7 +3588,7 @@
       </c>
       <c r="C188" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="189" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3607,7 +3598,7 @@
       </c>
       <c r="C189" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="190" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3631,7 +3622,7 @@
       </c>
       <c r="C192" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="193" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3641,7 +3632,7 @@
       </c>
       <c r="C193" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="194" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3651,7 +3642,7 @@
       </c>
       <c r="C194" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="195" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3661,7 +3652,7 @@
       </c>
       <c r="C195" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="196" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3671,7 +3662,7 @@
       </c>
       <c r="C196" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="197" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3695,7 +3686,7 @@
       </c>
       <c r="C199" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="200" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3705,7 +3696,7 @@
       </c>
       <c r="C200" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="201" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3715,7 +3706,7 @@
       </c>
       <c r="C201" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="202" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3725,7 +3716,7 @@
       </c>
       <c r="C202" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="203" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3735,7 +3726,7 @@
       </c>
       <c r="C203" t="str">
         <f>'Versioni EJB'!C46</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="204" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3759,7 +3750,7 @@
       </c>
       <c r="C206" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="207" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3769,7 +3760,7 @@
       </c>
       <c r="C207" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="208" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3779,7 +3770,7 @@
       </c>
       <c r="C208" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="209" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3789,7 +3780,7 @@
       </c>
       <c r="C209" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="210" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3799,7 +3790,7 @@
       </c>
       <c r="C210" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="211" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3816,7 +3807,7 @@
       </c>
       <c r="C212" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="213" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3826,7 +3817,7 @@
       </c>
       <c r="C213" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="214" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3836,7 +3827,7 @@
       </c>
       <c r="C214" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="215" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3846,7 +3837,7 @@
       </c>
       <c r="C215" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="216" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3856,7 +3847,7 @@
       </c>
       <c r="C216" t="str">
         <f>'Versioni EJB'!C47</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="217" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3866,7 +3857,7 @@
       </c>
       <c r="C217" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="218" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3876,7 +3867,7 @@
       </c>
       <c r="C218" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="219" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3886,7 +3877,7 @@
       </c>
       <c r="C219" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="220" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3896,7 +3887,7 @@
       </c>
       <c r="C220" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="221" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3913,7 +3904,7 @@
       </c>
       <c r="C222" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="223" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3923,7 +3914,7 @@
       </c>
       <c r="C223" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="224" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3933,7 +3924,7 @@
       </c>
       <c r="C224" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="225" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -3950,7 +3941,7 @@
       </c>
       <c r="C226" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="227" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3960,7 +3951,7 @@
       </c>
       <c r="C227" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="228" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3970,7 +3961,7 @@
       </c>
       <c r="C228" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="229" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3980,7 +3971,7 @@
       </c>
       <c r="C229" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="230" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3990,7 +3981,7 @@
       </c>
       <c r="C230" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="231" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4000,7 +3991,7 @@
       </c>
       <c r="C231" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="232" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4010,7 +4001,7 @@
       </c>
       <c r="C232" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="233" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4027,7 +4018,7 @@
       </c>
       <c r="C234" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="235" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4037,7 +4028,7 @@
       </c>
       <c r="C235" t="str">
         <f>'Versioni EJB'!C39</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="236" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4047,7 +4038,7 @@
       </c>
       <c r="C236" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="237" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4057,7 +4048,7 @@
       </c>
       <c r="C237" t="str">
         <f>'Versioni EJB'!C47</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="238" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4067,7 +4058,7 @@
       </c>
       <c r="C238" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="239" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4077,7 +4068,7 @@
       </c>
       <c r="C239" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="240" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4087,7 +4078,7 @@
       </c>
       <c r="C240" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="241" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4097,7 +4088,7 @@
       </c>
       <c r="C241" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="242" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4107,7 +4098,7 @@
       </c>
       <c r="C242" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="243" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4117,7 +4108,7 @@
       </c>
       <c r="C243" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="244" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4134,7 +4125,7 @@
       </c>
       <c r="C245" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="246" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4144,7 +4135,7 @@
       </c>
       <c r="C246" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="247" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4154,7 +4145,7 @@
       </c>
       <c r="C247" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="248" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4171,7 +4162,7 @@
       </c>
       <c r="C249" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="250" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4181,7 +4172,7 @@
       </c>
       <c r="C250" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="251" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4191,7 +4182,7 @@
       </c>
       <c r="C251" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="252" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4201,7 +4192,7 @@
       </c>
       <c r="C252" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="253" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4211,7 +4202,7 @@
       </c>
       <c r="C253" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="254" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4221,7 +4212,7 @@
       </c>
       <c r="C254" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="255" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4231,7 +4222,7 @@
       </c>
       <c r="C255" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="256" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4241,7 +4232,7 @@
       </c>
       <c r="C256" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="257" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4258,7 +4249,7 @@
       </c>
       <c r="C258" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="259" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4268,7 +4259,7 @@
       </c>
       <c r="C259" t="str">
         <f>'Versioni EJB'!C47</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="260" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4278,7 +4269,7 @@
       </c>
       <c r="C260" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="261" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4288,7 +4279,7 @@
       </c>
       <c r="C261" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="262" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4298,7 +4289,7 @@
       </c>
       <c r="C262" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="263" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4308,7 +4299,7 @@
       </c>
       <c r="C263" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="264" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4318,7 +4309,7 @@
       </c>
       <c r="C264" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="265" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4328,7 +4319,7 @@
       </c>
       <c r="C265" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="266" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4338,7 +4329,7 @@
       </c>
       <c r="C266" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="267" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4362,7 +4353,7 @@
       </c>
       <c r="C269" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="270" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4372,7 +4363,7 @@
       </c>
       <c r="C270" t="str">
         <f>'Versioni EJB'!C22</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="271" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4382,7 +4373,7 @@
       </c>
       <c r="C271" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="272" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4392,7 +4383,7 @@
       </c>
       <c r="C272" t="str">
         <f>'Versioni EJB'!C21</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="273" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4402,7 +4393,7 @@
       </c>
       <c r="C273" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="274" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4412,7 +4403,7 @@
       </c>
       <c r="C274" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.19.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="275" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4422,7 +4413,7 @@
       </c>
       <c r="C275" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="276" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4432,7 +4423,7 @@
       </c>
       <c r="C276" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="277" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4442,7 +4433,7 @@
       </c>
       <c r="C277" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="278" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4452,7 +4443,7 @@
       </c>
       <c r="C278" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="279" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4462,7 +4453,7 @@
       </c>
       <c r="C279" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="280" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4472,7 +4463,7 @@
       </c>
       <c r="C280" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="281" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4489,7 +4480,7 @@
       </c>
       <c r="C282" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="283" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4499,7 +4490,7 @@
       </c>
       <c r="C283" t="str">
         <f>'Versioni EJB'!C62</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="284" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4509,7 +4500,7 @@
       </c>
       <c r="C284" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="285" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4519,7 +4510,7 @@
       </c>
       <c r="C285" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="286" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4529,7 +4520,7 @@
       </c>
       <c r="C286" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="287" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4539,7 +4530,7 @@
       </c>
       <c r="C287" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="288" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4556,7 +4547,7 @@
       </c>
       <c r="C289" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="290" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4566,7 +4557,7 @@
       </c>
       <c r="C290" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="291" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4576,7 +4567,7 @@
       </c>
       <c r="C291" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="292" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4586,7 +4577,7 @@
       </c>
       <c r="C292" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="293" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4596,7 +4587,7 @@
       </c>
       <c r="C293" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="294" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4606,7 +4597,7 @@
       </c>
       <c r="C294" t="str">
         <f>'Versioni EJB'!C62</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="295" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4616,7 +4607,7 @@
       </c>
       <c r="C295" t="str">
         <f>'Versioni EJB'!C47</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="296" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4626,7 +4617,7 @@
       </c>
       <c r="C296" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="297" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4636,7 +4627,7 @@
       </c>
       <c r="C297" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="298" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4653,7 +4644,7 @@
       </c>
       <c r="C299" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="300" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4663,7 +4654,7 @@
       </c>
       <c r="C300" t="str">
         <f>'Versioni EJB'!C62</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="301" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4673,7 +4664,7 @@
       </c>
       <c r="C301" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="302" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4683,7 +4674,7 @@
       </c>
       <c r="C302" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="303" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4693,7 +4684,7 @@
       </c>
       <c r="C303" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="304" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4703,7 +4694,7 @@
       </c>
       <c r="C304" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="305" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4713,7 +4704,7 @@
       </c>
       <c r="C305" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="306" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4723,7 +4714,7 @@
       </c>
       <c r="C306" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="307" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4740,7 +4731,7 @@
       </c>
       <c r="C308" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="309" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4750,7 +4741,7 @@
       </c>
       <c r="C309" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="310" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4760,7 +4751,7 @@
       </c>
       <c r="C310" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="311" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4770,7 +4761,7 @@
       </c>
       <c r="C311" t="str">
         <f>'Versioni EJB'!C68</f>
-        <v>1.19.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="312" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4794,7 +4785,7 @@
       </c>
       <c r="C314" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="315" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4804,7 +4795,7 @@
       </c>
       <c r="C315" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="316" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4814,7 +4805,7 @@
       </c>
       <c r="C316" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="317" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4824,7 +4815,7 @@
       </c>
       <c r="C317" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="318" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4834,7 +4825,7 @@
       </c>
       <c r="C318" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="319" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4844,7 +4835,7 @@
       </c>
       <c r="C319" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="320" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4854,7 +4845,7 @@
       </c>
       <c r="C320" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="321" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4864,7 +4855,7 @@
       </c>
       <c r="C321" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="322" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4881,7 +4872,7 @@
       </c>
       <c r="C323" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="324" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4891,7 +4882,7 @@
       </c>
       <c r="C324" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="325" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4901,7 +4892,7 @@
       </c>
       <c r="C325" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.28.0-env-svis-SNAPSHOT</v>
+        <v>1.33.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="326" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4911,7 +4902,7 @@
       </c>
       <c r="C326" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="327" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4921,7 +4912,7 @@
       </c>
       <c r="C327" t="str">
         <f>'Versioni EJB'!C38</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="328" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4931,7 +4922,7 @@
       </c>
       <c r="C328" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="329" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4941,7 +4932,7 @@
       </c>
       <c r="C329" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="330" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4951,7 +4942,7 @@
       </c>
       <c r="C330" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="331" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4961,7 +4952,7 @@
       </c>
       <c r="C331" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="332" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4971,7 +4962,7 @@
       </c>
       <c r="C332" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="333" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4981,7 +4972,7 @@
       </c>
       <c r="C333" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="334" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -4998,7 +4989,7 @@
       </c>
       <c r="C335" t="str">
         <f>'Versioni EJB'!C46</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="336" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5008,7 +4999,7 @@
       </c>
       <c r="C336" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="337" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5018,7 +5009,7 @@
       </c>
       <c r="C337" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="338" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5028,7 +5019,7 @@
       </c>
       <c r="C338" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="339" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5038,7 +5029,7 @@
       </c>
       <c r="C339" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="340" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5048,7 +5039,7 @@
       </c>
       <c r="C340" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.72.0-env-svis-SNAPSHOT</v>
+        <v>1.72.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="341" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5065,7 +5056,7 @@
       </c>
       <c r="C342" t="str">
         <f>'Versioni EJB'!C69</f>
-        <v>1.55.0-env-svis-SNAPSHOT</v>
+        <v>1.55.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="343" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5075,7 +5066,7 @@
       </c>
       <c r="C343" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.72.0-env-svis-SNAPSHOT</v>
+        <v>1.72.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="344" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5085,7 +5076,7 @@
       </c>
       <c r="C344" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="345" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5095,7 +5086,7 @@
       </c>
       <c r="C345" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="346" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5105,7 +5096,7 @@
       </c>
       <c r="C346" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="347" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5115,7 +5106,7 @@
       </c>
       <c r="C347" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="348" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5125,7 +5116,7 @@
       </c>
       <c r="C348" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="349" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5135,7 +5126,7 @@
       </c>
       <c r="C349" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="350" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5159,7 +5150,7 @@
       </c>
       <c r="C352" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="353" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5169,7 +5160,7 @@
       </c>
       <c r="C353" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="354" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5179,7 +5170,7 @@
       </c>
       <c r="C354" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="355" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5189,7 +5180,7 @@
       </c>
       <c r="C355" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="356" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5206,7 +5197,7 @@
       </c>
       <c r="C357" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="358" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5216,7 +5207,7 @@
       </c>
       <c r="C358" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="359" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5226,7 +5217,7 @@
       </c>
       <c r="C359" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="360" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5236,12 +5227,12 @@
       </c>
       <c r="C360" t="str">
         <f>'Versioni EJB'!C9</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="361" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A361" s="4" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B361" s="4"/>
       <c r="C361" s="4"/>
@@ -5253,7 +5244,7 @@
       </c>
       <c r="C362" t="str">
         <f>'Versioni EJB'!C11</f>
-        <v>1.5.0-env-svis-SNAPSHOT</v>
+        <v>1.5.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="363" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5263,7 +5254,7 @@
       </c>
       <c r="C363" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="364" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5273,7 +5264,7 @@
       </c>
       <c r="C364" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.28.0-env-svis-SNAPSHOT</v>
+        <v>1.33.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="365" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5283,7 +5274,7 @@
       </c>
       <c r="C365" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="366" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5300,7 +5291,7 @@
       </c>
       <c r="C367" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="368" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5310,7 +5301,7 @@
       </c>
       <c r="C368" t="str">
         <f>'Versioni EJB'!C39</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="369" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5320,7 +5311,7 @@
       </c>
       <c r="C369" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="370" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5330,7 +5321,7 @@
       </c>
       <c r="C370" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="371" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5340,7 +5331,7 @@
       </c>
       <c r="C371" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="372" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5357,7 +5348,7 @@
       </c>
       <c r="C373" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="374" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5367,7 +5358,7 @@
       </c>
       <c r="C374" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="375" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5377,7 +5368,7 @@
       </c>
       <c r="C375" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="376" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5387,7 +5378,7 @@
       </c>
       <c r="C376" t="str">
         <f>'Versioni EJB'!C7</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="377" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5404,7 +5395,7 @@
       </c>
       <c r="C378" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="379" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5414,7 +5405,7 @@
       </c>
       <c r="C379" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="380" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5424,7 +5415,7 @@
       </c>
       <c r="C380" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="381" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5434,7 +5425,7 @@
       </c>
       <c r="C381" t="str">
         <f>'Versioni EJB'!C77</f>
-        <v>1.19.0-env-svis-SNAPSHOT</v>
+        <v>1.21.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="382" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5444,7 +5435,7 @@
       </c>
       <c r="C382" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="383" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5461,7 +5452,7 @@
       </c>
       <c r="C384" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="385" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5471,7 +5462,7 @@
       </c>
       <c r="C385" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="386" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5481,7 +5472,7 @@
       </c>
       <c r="C386" t="str">
         <f>'Versioni EJB'!C69</f>
-        <v>1.55.0-env-svis-SNAPSHOT</v>
+        <v>1.55.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="387" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5491,7 +5482,7 @@
       </c>
       <c r="C387" t="str">
         <f>'Versioni EJB'!C51</f>
-        <v>1.43.0-env-svis-SNAPSHOT</v>
+        <v>1.43.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="388" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5501,7 +5492,7 @@
       </c>
       <c r="C388" t="str">
         <f>'Versioni EJB'!C73</f>
-        <v>1.72.0-env-svis-SNAPSHOT</v>
+        <v>1.72.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="389" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5511,7 +5502,7 @@
       </c>
       <c r="C389" t="str">
         <f>'Versioni EJB'!C77</f>
-        <v>1.19.0-env-svis-SNAPSHOT</v>
+        <v>1.21.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="390" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5521,7 +5512,7 @@
       </c>
       <c r="C390" t="str">
         <f>'Versioni EJB'!C72</f>
-        <v>1.13.0-env-svis-SNAPSHOT</v>
+        <v>1.15.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="391" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5531,7 +5522,7 @@
       </c>
       <c r="C391" t="str">
         <f>'Versioni EJB'!C74</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="392" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5541,7 +5532,7 @@
       </c>
       <c r="C392" t="str">
         <f>'Versioni EJB'!C63</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="393" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5551,7 +5542,7 @@
       </c>
       <c r="C393" t="str">
         <f>'Versioni EJB'!C48</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="394" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5561,7 +5552,7 @@
       </c>
       <c r="C394" t="str">
         <f>'Versioni EJB'!C65</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="395" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5571,7 +5562,7 @@
       </c>
       <c r="C395" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="396" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5588,7 +5579,7 @@
       </c>
       <c r="C397" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="398" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5598,7 +5589,7 @@
       </c>
       <c r="C398" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="399" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5608,7 +5599,7 @@
       </c>
       <c r="C399" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="400" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5618,7 +5609,7 @@
       </c>
       <c r="C400" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="401" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5642,7 +5633,7 @@
       </c>
       <c r="C403" t="str">
         <f>'Versioni EJB'!C5</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="404" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5652,7 +5643,7 @@
       </c>
       <c r="C404" t="str">
         <f>'Versioni EJB'!C50</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="405" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5662,7 +5653,7 @@
       </c>
       <c r="C405" t="str">
         <f>'Versioni EJB'!C83</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="406" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5672,7 +5663,7 @@
       </c>
       <c r="C406" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="407" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5682,7 +5673,7 @@
       </c>
       <c r="C407" t="str">
         <f>'Versioni EJB'!C62</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="408" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5692,7 +5683,7 @@
       </c>
       <c r="C408" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="409" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5702,7 +5693,7 @@
       </c>
       <c r="C409" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="410" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5734,7 +5725,7 @@
       </c>
       <c r="C413" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="414" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5744,7 +5735,7 @@
       </c>
       <c r="C414" t="str">
         <f>'Versioni EJB'!C54</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="415" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5754,7 +5745,7 @@
       </c>
       <c r="C415" t="str">
         <f>'Versioni EJB'!C91</f>
-        <v>1.23.0-env-svis-SNAPSHOT</v>
+        <v>1.23.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="416" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5764,7 +5755,7 @@
       </c>
       <c r="C416" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="417" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5774,7 +5765,7 @@
       </c>
       <c r="C417" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.28.0-env-svis-SNAPSHOT</v>
+        <v>1.33.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="418" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5784,7 +5775,7 @@
       </c>
       <c r="C418" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="419" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5794,7 +5785,7 @@
       </c>
       <c r="C419" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="420" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5804,7 +5795,7 @@
       </c>
       <c r="C420" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="421" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5814,7 +5805,7 @@
       </c>
       <c r="C421" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="422" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5824,7 +5815,7 @@
       </c>
       <c r="C422" t="str">
         <f>'Versioni EJB'!C10</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="423" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5834,7 +5825,7 @@
       </c>
       <c r="C423" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="424" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5858,7 +5849,7 @@
       </c>
       <c r="C426" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="427" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5868,7 +5859,7 @@
       </c>
       <c r="C427" t="str">
         <f>'Versioni EJB'!C93</f>
-        <v>1.206.0-env-svis-SNAPSHOT</v>
+        <v>1.206.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="428" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5878,7 +5869,7 @@
       </c>
       <c r="C428" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="429" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5888,7 +5879,7 @@
       </c>
       <c r="C429" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="430" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5898,7 +5889,7 @@
       </c>
       <c r="C430" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="431" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5908,7 +5899,7 @@
       </c>
       <c r="C431" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="432" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5932,7 +5923,7 @@
       </c>
       <c r="C434" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="435" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5942,7 +5933,7 @@
       </c>
       <c r="C435" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="436" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5952,7 +5943,7 @@
       </c>
       <c r="C436" t="str">
         <f>'Versioni EJB'!C95</f>
-        <v>1.140.0-env-svis-SNAPSHOT</v>
+        <v>1.140.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="437" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5962,7 +5953,7 @@
       </c>
       <c r="C437" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="438" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5972,7 +5963,7 @@
       </c>
       <c r="C438" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="439" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5982,7 +5973,7 @@
       </c>
       <c r="C439" t="str">
         <f>'Versioni EJB'!C15</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="440" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -5999,7 +5990,7 @@
       </c>
       <c r="C441" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="442" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6009,7 +6000,7 @@
       </c>
       <c r="C442" t="str">
         <f>'Versioni EJB'!C93</f>
-        <v>1.206.0-env-svis-SNAPSHOT</v>
+        <v>1.206.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="443" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6019,7 +6010,7 @@
       </c>
       <c r="C443" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="444" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6029,7 +6020,7 @@
       </c>
       <c r="C444" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="445" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6039,7 +6030,7 @@
       </c>
       <c r="C445" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="446" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6049,7 +6040,7 @@
       </c>
       <c r="C446" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="447" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6059,7 +6050,7 @@
       </c>
       <c r="C447" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="448" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6076,7 +6067,7 @@
       </c>
       <c r="C449" t="str">
         <f>'Versioni EJB'!C95</f>
-        <v>1.140.0-env-svis-SNAPSHOT</v>
+        <v>1.140.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="450" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6086,7 +6077,7 @@
       </c>
       <c r="C450" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="451" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6096,7 +6087,7 @@
       </c>
       <c r="C451" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="452" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6106,7 +6097,7 @@
       </c>
       <c r="C452" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="453" spans="1:3" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -6116,7 +6107,7 @@
       </c>
       <c r="C453" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="454" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6133,7 +6124,7 @@
       </c>
       <c r="C455" t="str">
         <f>'Versioni EJB'!C93</f>
-        <v>1.206.0-env-svis-SNAPSHOT</v>
+        <v>1.206.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="456" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6143,7 +6134,7 @@
       </c>
       <c r="C456" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="457" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6153,7 +6144,7 @@
       </c>
       <c r="C457" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="458" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6163,7 +6154,7 @@
       </c>
       <c r="C458" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="459" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6173,7 +6164,7 @@
       </c>
       <c r="C459" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="460" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6183,7 +6174,7 @@
       </c>
       <c r="C460" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.28.0-env-svis-SNAPSHOT</v>
+        <v>1.33.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="461" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6193,7 +6184,7 @@
       </c>
       <c r="C461" t="str">
         <f>'Versioni EJB'!C21</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="462" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6203,7 +6194,7 @@
       </c>
       <c r="C462" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="463" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6213,7 +6204,7 @@
       </c>
       <c r="C463" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="464" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6223,7 +6214,7 @@
       </c>
       <c r="C464" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="465" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6233,7 +6224,7 @@
       </c>
       <c r="C465" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="466" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6243,7 +6234,7 @@
       </c>
       <c r="C466" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="467" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6253,7 +6244,7 @@
       </c>
       <c r="C467" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="468" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6263,7 +6254,7 @@
       </c>
       <c r="C468" t="str">
         <f>'Versioni EJB'!C58</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="469" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6273,7 +6264,7 @@
       </c>
       <c r="C469" t="str">
         <f>'Versioni EJB'!C13</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="470" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6290,7 +6281,7 @@
       </c>
       <c r="C471" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="472" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6300,7 +6291,7 @@
       </c>
       <c r="C472" t="str">
         <f>'Versioni EJB'!C47</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="473" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6310,7 +6301,7 @@
       </c>
       <c r="C473" t="str">
         <f>'Versioni EJB'!C27</f>
-        <v>1.28.0-env-svis-SNAPSHOT</v>
+        <v>1.33.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="474" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6320,7 +6311,7 @@
       </c>
       <c r="C474" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="475" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6330,7 +6321,7 @@
       </c>
       <c r="C475" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="476" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6340,7 +6331,7 @@
       </c>
       <c r="C476" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="477" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6350,7 +6341,7 @@
       </c>
       <c r="C477" t="str">
         <f>'Versioni EJB'!C95</f>
-        <v>1.140.0-env-svis-SNAPSHOT</v>
+        <v>1.140.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="478" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6367,7 +6358,7 @@
       </c>
       <c r="C479" t="str">
         <f>'Versioni EJB'!C95</f>
-        <v>1.140.0-env-svis-SNAPSHOT</v>
+        <v>1.140.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="480" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6377,7 +6368,7 @@
       </c>
       <c r="C480" t="str">
         <f>'Versioni EJB'!C14</f>
-        <v>1.52.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="481" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6387,7 +6378,7 @@
       </c>
       <c r="C481" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="482" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6397,7 +6388,7 @@
       </c>
       <c r="C482" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="483" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6407,7 +6398,7 @@
       </c>
       <c r="C483" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="484" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6431,7 +6422,7 @@
       </c>
       <c r="C486" t="str">
         <f>'Versioni EJB'!C86</f>
-        <v>1.43.0-env-svis-SNAPSHOT</v>
+        <v>1.43.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="487" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6441,7 +6432,7 @@
       </c>
       <c r="C487" t="str">
         <f>'Versioni EJB'!C85</f>
-        <v>1.30.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="488" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6451,7 +6442,7 @@
       </c>
       <c r="C488" t="str">
         <f>'Versioni EJB'!C32</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.16.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="489" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6461,7 +6452,7 @@
       </c>
       <c r="C489" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="490" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6471,7 +6462,7 @@
       </c>
       <c r="C490" t="str">
         <f>'Versioni EJB'!C82</f>
-        <v>1.11.0-env-svis-SNAPSHOT</v>
+        <v>1.11.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="491" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6481,7 +6472,7 @@
       </c>
       <c r="C491" t="str">
         <f>'Versioni EJB'!C29</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.12.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="492" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6491,7 +6482,7 @@
       </c>
       <c r="C492" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="493" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6501,7 +6492,7 @@
       </c>
       <c r="C493" t="str">
         <f>'Versioni EJB'!C102</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="494" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6511,7 +6502,7 @@
       </c>
       <c r="C494" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="495" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6521,7 +6512,7 @@
       </c>
       <c r="C495" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="496" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6531,7 +6522,7 @@
       </c>
       <c r="C496" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="497" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6541,7 +6532,7 @@
       </c>
       <c r="C497" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="498" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6551,7 +6542,7 @@
       </c>
       <c r="C498" t="str">
         <f>'Versioni EJB'!C2</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="499" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6568,7 +6559,7 @@
       </c>
       <c r="C500" t="str">
         <f>'Versioni EJB'!C100</f>
-        <v>1.123.0-env-svis-SNAPSHOT</v>
+        <v>1.124.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="501" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6578,7 +6569,7 @@
       </c>
       <c r="C501" t="str">
         <f>'Versioni EJB'!C93</f>
-        <v>1.206.0-env-svis-SNAPSHOT</v>
+        <v>1.206.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="502" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6588,7 +6579,7 @@
       </c>
       <c r="C502" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="503" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6598,7 +6589,7 @@
       </c>
       <c r="C503" t="str">
         <f>'Versioni EJB'!C60</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.17.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="504" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6608,7 +6599,7 @@
       </c>
       <c r="C504" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="505" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6618,7 +6609,7 @@
       </c>
       <c r="C505" t="str">
         <f>'Versioni EJB'!C46</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="506" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6628,7 +6619,7 @@
       </c>
       <c r="C506" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="507" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
@@ -6645,7 +6636,7 @@
       </c>
       <c r="C508" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="509" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6655,7 +6646,7 @@
       </c>
       <c r="C509" t="str">
         <f>'Versioni EJB'!C17</f>
-        <v>1.48.0-env-svis-SNAPSHOT</v>
+        <v>1.54.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="510" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6665,7 +6656,7 @@
       </c>
       <c r="C510" t="str">
         <f>'Versioni EJB'!C100</f>
-        <v>1.123.0-env-svis-SNAPSHOT</v>
+        <v>1.124.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="511" spans="1:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6675,12 +6666,12 @@
       </c>
       <c r="C511" t="str">
         <f>'Versioni EJB'!C34</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="512" spans="1:3" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A512" s="9" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="B512" s="9"/>
       <c r="C512" s="9"/>
@@ -6699,7 +6690,7 @@
       </c>
       <c r="C514" t="str">
         <f>'Versioni EJB'!C93</f>
-        <v>1.206.0-env-svis-SNAPSHOT</v>
+        <v>1.206.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="515" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6709,7 +6700,7 @@
       </c>
       <c r="C515" t="str">
         <f>'Versioni EJB'!C105</f>
-        <v>1.16.0-env-svis-SNAPSHOT</v>
+        <v>1.18.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="516" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6719,7 +6710,7 @@
       </c>
       <c r="C516" t="str">
         <f>'Versioni EJB'!C67</f>
-        <v>1.10.0-env-svis-SNAPSHOT</v>
+        <v>1.10.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="517" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6729,7 +6720,7 @@
       </c>
       <c r="C517" t="str">
         <f>'Versioni EJB'!C64</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="518" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6739,7 +6730,7 @@
       </c>
       <c r="C518" t="str">
         <f>'Versioni EJB'!C40</f>
-        <v>1.14.0-env-svis-SNAPSHOT</v>
+        <v>1.14.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="519" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6749,7 +6740,7 @@
       </c>
       <c r="C519" t="str">
         <f>'Versioni EJB'!C102</f>
-        <v>1.8.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="520" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6759,7 +6750,7 @@
       </c>
       <c r="C520" t="str">
         <f>'Versioni EJB'!C71</f>
-        <v>1.25.0-env-svis-SNAPSHOT</v>
+        <v>1.28.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="521" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6769,7 +6760,7 @@
       </c>
       <c r="C521" t="str">
         <f>'Versioni EJB'!C49</f>
-        <v>1.17.0-env-svis-SNAPSHOT</v>
+        <v>1.19.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="522" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6779,7 +6770,7 @@
       </c>
       <c r="C522" t="str">
         <f>'Versioni EJB'!C20</f>
-        <v>1.12.0-env-svis-SNAPSHOT</v>
+        <v>1.13.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="523" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6789,7 +6780,7 @@
       </c>
       <c r="C523" t="str">
         <f>'Versioni EJB'!C78</f>
-        <v>1.29.0-env-svis-SNAPSHOT</v>
+        <v>1.30.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="524" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6799,7 +6790,7 @@
       </c>
       <c r="C524" t="str">
         <f>'Versioni EJB'!C4</f>
-        <v>1.9.0-env-svis-SNAPSHOT</v>
+        <v>1.9.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
     <row r="525" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6809,7 +6800,7 @@
       </c>
       <c r="C525" t="str">
         <f>'Versioni EJB'!C41</f>
-        <v>1.21.0-env-svis-SNAPSHOT</v>
+        <v>1.22.0-env-svia-SNAPSHOT</v>
       </c>
     </row>
   </sheetData>
@@ -6817,12 +6808,6 @@
     <sortCondition ref="B20"/>
   </sortState>
   <mergeCells count="19">
-    <mergeCell ref="A133:C133"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A84:C84"/>
     <mergeCell ref="A512:C512"/>
     <mergeCell ref="A484:C484"/>
     <mergeCell ref="A172:C172"/>
@@ -6836,6 +6821,12 @@
     <mergeCell ref="A204:C204"/>
     <mergeCell ref="A197:C197"/>
     <mergeCell ref="A190:C190"/>
+    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A84:C84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunto appuntamento-ejb alla lista degli EJB di competenza di Alten
</commit_message>
<xml_diff>
--- a/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
+++ b/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Allineamenti\Software\SoftwareAllineamenti\src\main\resources\excelutils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openshift\SoftwareAllineamenti\src\main\resources\excelutils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{134A75AB-0A92-4841-9EBD-46B91DE4122F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EF3FF40-DEC0-4D98-9E17-4F6D66A971FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6F9E28-8696-4430-99AA-92A66BC09C93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4395" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versioni EJB" sheetId="1" r:id="rId1"/>
     <sheet name="Dipendenze" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Versioni EJB'!$B$1:$D$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Versioni EJB'!$B$1:$D$109</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="160">
   <si>
     <t>BLOCCO</t>
   </si>
@@ -509,6 +508,12 @@
   </si>
   <si>
     <t>Blocco 21</t>
+  </si>
+  <si>
+    <t>appuntamento-ejb</t>
+  </si>
+  <si>
+    <t>1.5.0</t>
   </si>
 </sst>
 </file>
@@ -590,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -615,6 +620,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -892,21 +913,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="92.25" customWidth="1"/>
-    <col min="7" max="7" width="51.875" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="92.21875" customWidth="1"/>
+    <col min="7" max="7" width="51.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1314,7 +1335,7 @@
         <v>antiriciclaggio --&gt; 1.17.0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.5">
+    <row r="22" spans="1:7">
       <c r="A22" s="10"/>
       <c r="B22" t="s">
         <v>33</v>
@@ -2206,7 +2227,7 @@
         <v>&lt;salvadanaio.version&gt;1.25.0&lt;/salvadanaio.version&gt;</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G108" si="7">CONCATENATE(E67," --&gt; ",C67)</f>
+        <f t="shared" ref="G67:G109" si="7">CONCATENATE(E67," --&gt; ",C67)</f>
         <v>salvadanaio --&gt; 1.25.0</v>
       </c>
     </row>
@@ -2251,7 +2272,7 @@
         <v>87</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" ref="E70:E108" si="8">LEFT(B70,LEN(B70)-4)</f>
+        <f t="shared" ref="E70:E109" si="8">LEFT(B70,LEN(B70)-4)</f>
         <v>bonifico</v>
       </c>
       <c r="F70" t="str">
@@ -2683,7 +2704,7 @@
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" spans="1:7" ht="13.5">
+    <row r="93" spans="1:7">
       <c r="A93" s="3">
         <v>16</v>
       </c>
@@ -2715,7 +2736,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
     </row>
-    <row r="95" spans="1:7" ht="13.5">
+    <row r="95" spans="1:7">
       <c r="A95" s="3">
         <v>17</v>
       </c>
@@ -2747,287 +2768,309 @@
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" ht="13.5">
+    <row r="97" spans="1:7" s="12" customFormat="1">
       <c r="A97" s="10">
         <v>18</v>
       </c>
-      <c r="B97" t="s">
-        <v>117</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="B97" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D97" s="13"/>
       <c r="E97" t="str">
         <f t="shared" si="8"/>
-        <v>bloccosblocco</v>
-      </c>
-      <c r="F97" t="str">
-        <f t="shared" ref="F97:F102" si="11">CONCATENATE("&lt;",E97,".version&gt;",C97,"&lt;/",E97,".version&gt;")</f>
-        <v>&lt;bloccosblocco.version&gt;1.21.0&lt;/bloccosblocco.version&gt;</v>
+        <v>appuntamento</v>
+      </c>
+      <c r="F97" s="14" t="str">
+        <f>CONCATENATE("&lt;",E97,".version&gt;",C97,"&lt;/",E97,".version&gt;")</f>
+        <v>&lt;appuntamento.version&gt;1.5.0&lt;/appuntamento.version&gt;</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="7"/>
-        <v>bloccosblocco --&gt; 1.21.0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="13.5">
+        <v>appuntamento --&gt; 1.5.0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="10"/>
       <c r="B98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="8"/>
+        <v>bloccosblocco</v>
+      </c>
+      <c r="F98" t="str">
+        <f t="shared" ref="F98:F103" si="11">CONCATENATE("&lt;",E98,".version&gt;",C98,"&lt;/",E98,".version&gt;")</f>
+        <v>&lt;bloccosblocco.version&gt;1.21.0&lt;/bloccosblocco.version&gt;</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="7"/>
+        <v>bloccosblocco --&gt; 1.21.0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="10"/>
+      <c r="B99" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="8"/>
         <v>condivisione</v>
       </c>
-      <c r="F98" t="str">
+      <c r="F99" t="str">
         <f t="shared" si="11"/>
         <v>&lt;condivisione.version&gt;1.19.0&lt;/condivisione.version&gt;</v>
       </c>
-      <c r="G98" t="str">
+      <c r="G99" t="str">
         <f t="shared" si="7"/>
         <v>condivisione --&gt; 1.19.0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="13.5">
-      <c r="A99" s="10"/>
-      <c r="B99" t="s">
+    <row r="100" spans="1:7">
+      <c r="A100" s="10"/>
+      <c r="B100" t="s">
         <v>119</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C100" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E99" t="str">
+      <c r="E100" t="str">
         <f t="shared" si="8"/>
         <v>conto</v>
       </c>
-      <c r="F99" t="str">
+      <c r="F100" t="str">
         <f t="shared" si="11"/>
         <v>&lt;conto.version&gt;1.39.0&lt;/conto.version&gt;</v>
       </c>
-      <c r="G99" t="str">
+      <c r="G100" t="str">
         <f t="shared" si="7"/>
         <v>conto --&gt; 1.39.0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="13.5">
-      <c r="A100" s="10"/>
-      <c r="B100" t="s">
+    <row r="101" spans="1:7">
+      <c r="A101" s="10"/>
+      <c r="B101" t="s">
         <v>120</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C101" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E100" t="str">
+      <c r="E101" t="str">
         <f t="shared" si="8"/>
         <v>globalposition</v>
       </c>
-      <c r="F100" t="str">
+      <c r="F101" t="str">
         <f t="shared" si="11"/>
         <v>&lt;globalposition.version&gt;1.133.0&lt;/globalposition.version&gt;</v>
       </c>
-      <c r="G100" t="str">
+      <c r="G101" t="str">
         <f t="shared" si="7"/>
         <v>globalposition --&gt; 1.133.0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="13.5">
-      <c r="A101" s="10"/>
-      <c r="B101" t="s">
+    <row r="102" spans="1:7">
+      <c r="A102" s="10"/>
+      <c r="B102" t="s">
         <v>122</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C102" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E101" t="str">
+      <c r="E102" t="str">
         <f t="shared" si="8"/>
         <v>identitadigitale</v>
       </c>
-      <c r="F101" t="str">
+      <c r="F102" t="str">
         <f t="shared" si="11"/>
         <v>&lt;identitadigitale.version&gt;1.45.0&lt;/identitadigitale.version&gt;</v>
       </c>
-      <c r="G101" t="str">
+      <c r="G102" t="str">
         <f t="shared" si="7"/>
         <v>identitadigitale --&gt; 1.45.0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="13.5">
-      <c r="A102" s="10"/>
-      <c r="B102" t="s">
+    <row r="103" spans="1:7">
+      <c r="A103" s="10"/>
+      <c r="B103" t="s">
         <v>124</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C103" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E102" t="str">
+      <c r="E103" t="str">
         <f t="shared" si="8"/>
         <v>proposte</v>
       </c>
-      <c r="F102" t="str">
+      <c r="F103" t="str">
         <f t="shared" si="11"/>
         <v>&lt;proposte.version&gt;1.13.0&lt;/proposte.version&gt;</v>
       </c>
-      <c r="G102" t="str">
+      <c r="G103" t="str">
         <f t="shared" si="7"/>
         <v>proposte --&gt; 1.13.0</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="4"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-    </row>
-    <row r="104" spans="1:7" ht="13.5">
-      <c r="A104" s="10">
+    <row r="104" spans="1:7">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="10">
         <v>19</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C105" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="E104" t="str">
+      <c r="E105" t="str">
         <f t="shared" si="8"/>
         <v>digitalwallet</v>
       </c>
-      <c r="F104" t="str">
-        <f>CONCATENATE("&lt;",E104,".version&gt;",C104,"&lt;/",E104,".version&gt;")</f>
+      <c r="F105" t="str">
+        <f>CONCATENATE("&lt;",E105,".version&gt;",C105,"&lt;/",E105,".version&gt;")</f>
         <v>&lt;digitalwallet.version&gt;1.64.0&lt;/digitalwallet.version&gt;</v>
       </c>
-      <c r="G104" t="str">
+      <c r="G105" t="str">
         <f t="shared" si="7"/>
         <v>digitalwallet --&gt; 1.64.0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="13.5">
-      <c r="A105" s="10"/>
-      <c r="B105" t="s">
+    <row r="106" spans="1:7">
+      <c r="A106" s="10"/>
+      <c r="B106" t="s">
         <v>128</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C106" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E105" t="str">
+      <c r="E106" t="str">
         <f t="shared" si="8"/>
         <v>pulsantiera</v>
       </c>
-      <c r="F105" t="str">
-        <f>CONCATENATE("&lt;",E105,".version&gt;",C105,"&lt;/",E105,".version&gt;")</f>
+      <c r="F106" t="str">
+        <f>CONCATENATE("&lt;",E106,".version&gt;",C106,"&lt;/",E106,".version&gt;")</f>
         <v>&lt;pulsantiera.version&gt;1.23.0&lt;/pulsantiera.version&gt;</v>
       </c>
-      <c r="G105" t="str">
+      <c r="G106" t="str">
         <f t="shared" si="7"/>
         <v>pulsantiera --&gt; 1.23.0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="13.5">
-      <c r="A106" s="10"/>
-      <c r="B106" t="s">
+    <row r="107" spans="1:7">
+      <c r="A107" s="10"/>
+      <c r="B107" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C107" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E106" t="str">
+      <c r="E107" t="str">
         <f t="shared" si="8"/>
         <v>trading</v>
       </c>
-      <c r="F106" t="str">
-        <f>CONCATENATE("&lt;",E106,".version&gt;",C106,"&lt;/",E106,".version&gt;")</f>
+      <c r="F107" t="str">
+        <f>CONCATENATE("&lt;",E107,".version&gt;",C107,"&lt;/",E107,".version&gt;")</f>
         <v>&lt;trading.version&gt;1.21.0&lt;/trading.version&gt;</v>
       </c>
-      <c r="G106" t="str">
+      <c r="G107" t="str">
         <f t="shared" si="7"/>
         <v>trading --&gt; 1.21.0</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="4"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-    </row>
-    <row r="108" spans="1:7" ht="13.5">
-      <c r="A108" s="3">
+    <row r="108" spans="1:7">
+      <c r="A108" s="4"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="3">
         <v>20</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>130</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C109" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E108" t="str">
+      <c r="E109" t="str">
         <f t="shared" si="8"/>
         <v>listaoperazioni</v>
       </c>
-      <c r="F108" t="str">
-        <f>CONCATENATE("&lt;",E108,".version&gt;",C108,"&lt;/",E108,".version&gt;")</f>
+      <c r="F109" t="str">
+        <f>CONCATENATE("&lt;",E109,".version&gt;",C109,"&lt;/",E109,".version&gt;")</f>
         <v>&lt;listaoperazioni.version&gt;1.77.0&lt;/listaoperazioni.version&gt;</v>
       </c>
-      <c r="G108" t="str">
+      <c r="G109" t="str">
         <f t="shared" si="7"/>
         <v>listaoperazioni --&gt; 1.77.0</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
-    </row>
-    <row r="110" spans="1:7" ht="13.5">
-      <c r="A110" s="3">
+    <row r="110" spans="1:7">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="3">
         <v>21</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>132</v>
       </c>
-      <c r="C110" s="8" t="s">
+      <c r="C111" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E110" t="str">
-        <f>LEFT(B110,LEN(B110)-4)</f>
+      <c r="E111" t="str">
+        <f>LEFT(B111,LEN(B111)-4)</f>
         <v>ricerca</v>
       </c>
-      <c r="F110" t="str">
-        <f>CONCATENATE("&lt;",E110,".version&gt;",C110,"&lt;/",E110,".version&gt;")</f>
+      <c r="F111" t="str">
+        <f>CONCATENATE("&lt;",E111,".version&gt;",C111,"&lt;/",E111,".version&gt;")</f>
         <v>&lt;ricerca.version&gt;1.9.0&lt;/ricerca.version&gt;</v>
       </c>
-      <c r="G110" t="str">
-        <f>CONCATENATE(E110," --&gt; ",C110)</f>
+      <c r="G111" t="str">
+        <f>CONCATENATE(E111," --&gt; ",C111)</f>
         <v>ricerca --&gt; 1.9.0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:D109" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="12">
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="A31:A41"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A105:A107"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A61:A68"/>
     <mergeCell ref="A70:A75"/>
     <mergeCell ref="A77:A80"/>
     <mergeCell ref="A82:A89"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="A31:A41"/>
-    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A97:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3036,18 +3079,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D531"/>
+  <dimension ref="A1:D539"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B418" sqref="B418"/>
+      <selection pane="bottomLeft" activeCell="A440" sqref="A440"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="29.875" customWidth="1"/>
-    <col min="2" max="2" width="25.375" customWidth="1"/>
-    <col min="3" max="3" width="29.75" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -7089,476 +7132,483 @@
       <c r="B433" s="11"/>
       <c r="C433" s="11"/>
     </row>
-    <row r="434" spans="1:3">
-      <c r="A434" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B434" s="2"/>
-      <c r="C434" s="2"/>
-    </row>
-    <row r="435" spans="1:3" outlineLevel="1">
-      <c r="B435" t="str">
+    <row r="434" spans="1:3" s="12" customFormat="1">
+      <c r="A434" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B434" s="17"/>
+      <c r="C434" s="17"/>
+    </row>
+    <row r="435" spans="1:3" s="12" customFormat="1" outlineLevel="1">
+      <c r="A435" s="15"/>
+      <c r="B435" s="14" t="str">
+        <f>'Versioni EJB'!B13</f>
+        <v>notification-ejb</v>
+      </c>
+      <c r="C435" s="14" t="str">
+        <f>'Versioni EJB'!C13</f>
+        <v>1.59.0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" s="12" customFormat="1" outlineLevel="1">
+      <c r="A436" s="15"/>
+      <c r="B436" s="14" t="str">
+        <f>'Versioni EJB'!B95</f>
+        <v>miogestore-ejb</v>
+      </c>
+      <c r="C436" s="14" t="str">
+        <f>'Versioni EJB'!C95</f>
+        <v>1.149.0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" s="12" customFormat="1" outlineLevel="1">
+      <c r="A437" s="15"/>
+      <c r="B437" s="14" t="str">
+        <f>'Versioni EJB'!B29</f>
+        <v>guestarea-ejb</v>
+      </c>
+      <c r="C437" s="14" t="str">
+        <f>'Versioni EJB'!C29</f>
+        <v>1.28.0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" s="12" customFormat="1" outlineLevel="1">
+      <c r="A438" s="15"/>
+      <c r="B438" s="14" t="str">
+        <f>'Versioni EJB'!B19</f>
+        <v>agenda-ejb</v>
+      </c>
+      <c r="C438" s="14" t="str">
+        <f>'Versioni EJB'!C19</f>
+        <v>1.19.0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" s="12" customFormat="1" outlineLevel="1">
+      <c r="A439" s="15"/>
+      <c r="B439" s="14" t="str">
+        <f>'Versioni EJB'!B4</f>
+        <v>banca-ejb</v>
+      </c>
+      <c r="C439" s="14" t="str">
+        <f>'Versioni EJB'!C4</f>
+        <v>1.15.0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" outlineLevel="1">
+      <c r="A440" s="15"/>
+      <c r="B440" s="14" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
       </c>
-      <c r="C435" t="str">
+      <c r="C440" s="14" t="str">
         <f>'Versioni EJB'!C2</f>
         <v>1.21.0</v>
       </c>
     </row>
-    <row r="436" spans="1:3" outlineLevel="1">
-      <c r="B436" t="str">
+    <row r="441" spans="1:3" outlineLevel="1">
+      <c r="A441" s="15"/>
+      <c r="B441" s="14" t="str">
+        <f>'Versioni EJB'!B16</f>
+        <v>profilocliente-ejb</v>
+      </c>
+      <c r="C441" s="14" t="str">
+        <f>'Versioni EJB'!C16</f>
+        <v>1.101.0</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3">
+      <c r="A442" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B442" s="2"/>
+      <c r="C442" s="2"/>
+    </row>
+    <row r="443" spans="1:3" outlineLevel="1">
+      <c r="B443" t="str">
+        <f>'Versioni EJB'!B2</f>
+        <v>isp-ib-om</v>
+      </c>
+      <c r="C443" t="str">
+        <f>'Versioni EJB'!C2</f>
+        <v>1.21.0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" outlineLevel="1">
+      <c r="B444" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
-      <c r="C436" t="str">
+      <c r="C444" t="str">
         <f>'Versioni EJB'!C4</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="437" spans="1:3" outlineLevel="1">
-      <c r="B437" t="str">
+    <row r="445" spans="1:3" outlineLevel="1">
+      <c r="B445" t="str">
         <f>'Versioni EJB'!B95</f>
         <v>miogestore-ejb</v>
       </c>
-      <c r="C437" t="str">
+      <c r="C445" t="str">
         <f>'Versioni EJB'!C95</f>
         <v>1.149.0</v>
       </c>
     </row>
-    <row r="438" spans="1:3" outlineLevel="1">
-      <c r="B438" t="str">
+    <row r="446" spans="1:3" outlineLevel="1">
+      <c r="B446" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C438" t="str">
+      <c r="C446" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="439" spans="1:3" outlineLevel="1">
-      <c r="B439" t="str">
+    <row r="447" spans="1:3" outlineLevel="1">
+      <c r="B447" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
       </c>
-      <c r="C439" t="str">
+      <c r="C447" t="str">
         <f>'Versioni EJB'!C13</f>
         <v>1.59.0</v>
       </c>
     </row>
-    <row r="440" spans="1:3" outlineLevel="1">
-      <c r="B440" t="str">
+    <row r="448" spans="1:3" outlineLevel="1">
+      <c r="B448" t="str">
         <f>'Versioni EJB'!B14</f>
         <v>postvendita-common-ejb</v>
       </c>
-      <c r="C440" t="str">
+      <c r="C448" t="str">
         <f>'Versioni EJB'!C14</f>
         <v>1.16.0</v>
       </c>
     </row>
-    <row r="441" spans="1:3">
-      <c r="A441" s="2" t="s">
+    <row r="449" spans="1:3">
+      <c r="A449" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B441" s="2"/>
-      <c r="C441" s="2"/>
-    </row>
-    <row r="442" spans="1:3" outlineLevel="2">
-      <c r="B442" t="str">
+      <c r="B449" s="2"/>
+      <c r="C449" s="2"/>
+    </row>
+    <row r="450" spans="1:3" outlineLevel="2">
+      <c r="B450" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
       </c>
-      <c r="C442" t="str">
+      <c r="C450" t="str">
         <f>'Versioni EJB'!C13</f>
         <v>1.59.0</v>
       </c>
     </row>
-    <row r="443" spans="1:3" outlineLevel="2">
-      <c r="B443" t="str">
+    <row r="451" spans="1:3" outlineLevel="2">
+      <c r="B451" t="str">
         <f>'Versioni EJB'!B93</f>
         <v>comunicazioni-ejb</v>
       </c>
-      <c r="C443" t="str">
+      <c r="C451" t="str">
         <f>'Versioni EJB'!C93</f>
         <v>1.239.0</v>
       </c>
     </row>
-    <row r="444" spans="1:3" outlineLevel="2">
-      <c r="B444" t="str">
+    <row r="452" spans="1:3" outlineLevel="2">
+      <c r="B452" t="str">
         <f>'Versioni EJB'!B78</f>
         <v>carte-ejb</v>
       </c>
-      <c r="C444" t="str">
+      <c r="C452" t="str">
         <f>'Versioni EJB'!C78</f>
         <v>1.39.0</v>
       </c>
     </row>
-    <row r="445" spans="1:3" outlineLevel="2">
-      <c r="B445" t="str">
+    <row r="453" spans="1:3" outlineLevel="2">
+      <c r="B453" t="str">
         <f>'Versioni EJB'!B55</f>
         <v>rubriche-ejb</v>
       </c>
-      <c r="C445" t="str">
+      <c r="C453" t="str">
         <f>'Versioni EJB'!C55</f>
         <v>1.31.0</v>
       </c>
     </row>
-    <row r="446" spans="1:3" outlineLevel="2">
-      <c r="B446" t="str">
+    <row r="454" spans="1:3" outlineLevel="2">
+      <c r="B454" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
-      <c r="C446" t="str">
+      <c r="C454" t="str">
         <f>'Versioni EJB'!C4</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="447" spans="1:3" outlineLevel="2">
-      <c r="B447" t="str">
+    <row r="455" spans="1:3" outlineLevel="2">
+      <c r="B455" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C447" t="str">
+      <c r="C455" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="448" spans="1:3" outlineLevel="2">
-      <c r="B448" t="str">
+    <row r="456" spans="1:3" outlineLevel="2">
+      <c r="B456" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
       </c>
-      <c r="C448" t="str">
+      <c r="C456" t="str">
         <f>'Versioni EJB'!C2</f>
         <v>1.21.0</v>
       </c>
     </row>
-    <row r="449" spans="1:3">
-      <c r="A449" s="2" t="s">
+    <row r="457" spans="1:3">
+      <c r="A457" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B449" s="2"/>
-      <c r="C449" s="2"/>
-    </row>
-    <row r="450" spans="1:3" outlineLevel="2">
-      <c r="B450" t="str">
+      <c r="B457" s="2"/>
+      <c r="C457" s="2"/>
+    </row>
+    <row r="458" spans="1:3" outlineLevel="2">
+      <c r="B458" t="str">
         <f>'Versioni EJB'!B95</f>
         <v>miogestore-ejb</v>
       </c>
-      <c r="C450" t="str">
+      <c r="C458" t="str">
         <f>'Versioni EJB'!C95</f>
         <v>1.149.0</v>
       </c>
     </row>
-    <row r="451" spans="1:3" outlineLevel="2">
-      <c r="B451" t="str">
+    <row r="459" spans="1:3" outlineLevel="2">
+      <c r="B459" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C451" t="str">
+      <c r="C459" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="452" spans="1:3" outlineLevel="2">
-      <c r="B452" t="str">
+    <row r="460" spans="1:3" outlineLevel="2">
+      <c r="B460" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
-      <c r="C452" t="str">
+      <c r="C460" t="str">
         <f>'Versioni EJB'!C4</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="453" spans="1:3" outlineLevel="2">
-      <c r="B453" t="str">
+    <row r="461" spans="1:3" outlineLevel="2">
+      <c r="B461" t="str">
         <f>'Versioni EJB'!B46</f>
         <v>pfm-ejb</v>
       </c>
-      <c r="C453" t="str">
+      <c r="C461" t="str">
         <f>'Versioni EJB'!C46</f>
         <v>1.29.0</v>
       </c>
     </row>
-    <row r="454" spans="1:3" outlineLevel="2">
-      <c r="B454" t="str">
+    <row r="462" spans="1:3" outlineLevel="2">
+      <c r="B462" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
       </c>
-      <c r="C454" t="str">
+      <c r="C462" t="str">
         <f>'Versioni EJB'!C2</f>
         <v>1.21.0</v>
       </c>
     </row>
-    <row r="455" spans="1:3">
-      <c r="A455" s="2" t="s">
+    <row r="463" spans="1:3">
+      <c r="A463" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B455" s="2"/>
-      <c r="C455" s="2"/>
-    </row>
-    <row r="456" spans="1:3" outlineLevel="1">
-      <c r="B456" t="str">
+      <c r="B463" s="2"/>
+      <c r="C463" s="2"/>
+    </row>
+    <row r="464" spans="1:3" outlineLevel="1">
+      <c r="B464" t="str">
         <f>'Versioni EJB'!B93</f>
         <v>comunicazioni-ejb</v>
       </c>
-      <c r="C456" t="str">
+      <c r="C464" t="str">
         <f>'Versioni EJB'!C93</f>
         <v>1.239.0</v>
       </c>
     </row>
-    <row r="457" spans="1:3" outlineLevel="1">
-      <c r="B457" t="str">
+    <row r="465" spans="1:3" outlineLevel="1">
+      <c r="B465" t="str">
         <f>'Versioni EJB'!B38</f>
         <v>prestiti-ejb</v>
       </c>
-      <c r="C457" t="str">
+      <c r="C465" t="str">
         <f>'Versioni EJB'!C38</f>
         <v>1.19.0</v>
       </c>
     </row>
-    <row r="458" spans="1:3" outlineLevel="1">
-      <c r="B458" t="str">
+    <row r="466" spans="1:3" outlineLevel="1">
+      <c r="B466" t="str">
         <f>'Versioni EJB'!B19</f>
         <v>agenda-ejb</v>
       </c>
-      <c r="C458" t="str">
+      <c r="C466" t="str">
         <f>'Versioni EJB'!C19</f>
         <v>1.19.0</v>
       </c>
     </row>
-    <row r="459" spans="1:3" outlineLevel="1">
-      <c r="B459" t="str">
+    <row r="467" spans="1:3" outlineLevel="1">
+      <c r="B467" t="str">
         <f>'Versioni EJB'!B33</f>
         <v>listiniinfofin-ejb</v>
       </c>
-      <c r="C459" t="str">
+      <c r="C467" t="str">
         <f>'Versioni EJB'!C33</f>
         <v>1.17.0</v>
       </c>
     </row>
-    <row r="460" spans="1:3" outlineLevel="1">
-      <c r="B460" t="str">
+    <row r="468" spans="1:3" outlineLevel="1">
+      <c r="B468" t="str">
         <f>'Versioni EJB'!B70</f>
         <v>bonifico-ejb</v>
       </c>
-      <c r="C460" t="str">
+      <c r="C468" t="str">
         <f>'Versioni EJB'!C70</f>
         <v>1.36.0</v>
       </c>
     </row>
-    <row r="461" spans="1:3" outlineLevel="1">
-      <c r="B461" t="str">
+    <row r="469" spans="1:3" outlineLevel="1">
+      <c r="B469" t="str">
         <f>'Versioni EJB'!B26</f>
         <v>filialevirtuale-ejb</v>
       </c>
-      <c r="C461" t="str">
+      <c r="C469" t="str">
         <f>'Versioni EJB'!C26</f>
         <v>1.75.0</v>
       </c>
     </row>
-    <row r="462" spans="1:3" outlineLevel="1">
-      <c r="B462" t="str">
+    <row r="470" spans="1:3" outlineLevel="1">
+      <c r="B470" t="str">
         <f>'Versioni EJB'!B20</f>
         <v>anagrafiche-ejb</v>
       </c>
-      <c r="C462" t="str">
+      <c r="C470" t="str">
         <f>'Versioni EJB'!C20</f>
         <v>1.17.0</v>
       </c>
     </row>
-    <row r="463" spans="1:3" outlineLevel="1">
-      <c r="B463" t="str">
+    <row r="471" spans="1:3" outlineLevel="1">
+      <c r="B471" t="str">
         <f>'Versioni EJB'!B57</f>
         <v>interactiondb-ejb</v>
       </c>
-      <c r="C463" t="str">
+      <c r="C471" t="str">
         <f>'Versioni EJB'!C57</f>
         <v>1.26.0</v>
       </c>
     </row>
-    <row r="464" spans="1:3" outlineLevel="1">
-      <c r="B464" t="str">
+    <row r="472" spans="1:3" outlineLevel="1">
+      <c r="B472" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C464" t="str">
+      <c r="C472" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="465" spans="1:3" outlineLevel="1">
-      <c r="B465" t="str">
+    <row r="473" spans="1:3" outlineLevel="1">
+      <c r="B473" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
       </c>
-      <c r="C465" t="str">
+      <c r="C473" t="str">
         <f>'Versioni EJB'!C39</f>
         <v>1.28.0</v>
       </c>
     </row>
-    <row r="466" spans="1:3" outlineLevel="1">
-      <c r="B466" t="str">
+    <row r="474" spans="1:3" outlineLevel="1">
+      <c r="B474" t="str">
         <f>'Versioni EJB'!B46</f>
         <v>pfm-ejb</v>
       </c>
-      <c r="C466" t="str">
+      <c r="C474" t="str">
         <f>'Versioni EJB'!C46</f>
         <v>1.29.0</v>
       </c>
     </row>
-    <row r="467" spans="1:3" outlineLevel="1">
-      <c r="B467" t="str">
+    <row r="475" spans="1:3" outlineLevel="1">
+      <c r="B475" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
-      <c r="C467" t="str">
+      <c r="C475" t="str">
         <f>'Versioni EJB'!C4</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="468" spans="1:3" outlineLevel="1">
-      <c r="B468" t="str">
+    <row r="476" spans="1:3" outlineLevel="1">
+      <c r="B476" t="str">
         <f>'Versioni EJB'!B78</f>
         <v>carte-ejb</v>
       </c>
-      <c r="C468" t="str">
+      <c r="C476" t="str">
         <f>'Versioni EJB'!C78</f>
         <v>1.39.0</v>
       </c>
     </row>
-    <row r="469" spans="1:3" outlineLevel="1">
-      <c r="B469" t="str">
+    <row r="477" spans="1:3" outlineLevel="1">
+      <c r="B477" t="str">
         <f>'Versioni EJB'!B55</f>
         <v>rubriche-ejb</v>
       </c>
-      <c r="C469" t="str">
+      <c r="C477" t="str">
         <f>'Versioni EJB'!C55</f>
         <v>1.31.0</v>
       </c>
     </row>
-    <row r="470" spans="1:3" outlineLevel="1">
-      <c r="B470" t="str">
+    <row r="478" spans="1:3" outlineLevel="1">
+      <c r="B478" t="str">
         <f>'Versioni EJB'!B12</f>
         <v>commons-ejb</v>
       </c>
-      <c r="C470" t="str">
+      <c r="C478" t="str">
         <f>'Versioni EJB'!C12</f>
         <v>1.18.0</v>
       </c>
     </row>
-    <row r="471" spans="1:3">
-      <c r="A471" s="2" t="s">
+    <row r="479" spans="1:3">
+      <c r="A479" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B471" s="2"/>
-      <c r="C471" s="2"/>
-    </row>
-    <row r="472" spans="1:3" outlineLevel="1">
-      <c r="B472" t="str">
+      <c r="B479" s="2"/>
+      <c r="C479" s="2"/>
+    </row>
+    <row r="480" spans="1:3" outlineLevel="1">
+      <c r="B480" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
       </c>
-      <c r="C472" t="str">
+      <c r="C480" t="str">
         <f>'Versioni EJB'!C13</f>
         <v>1.59.0</v>
       </c>
     </row>
-    <row r="473" spans="1:3" outlineLevel="1">
-      <c r="B473" t="str">
+    <row r="481" spans="1:3" outlineLevel="1">
+      <c r="B481" t="str">
         <f>'Versioni EJB'!B44</f>
         <v>condizioni-ejb</v>
       </c>
-      <c r="C473" t="str">
+      <c r="C481" t="str">
         <f>'Versioni EJB'!C44</f>
         <v>1.14.0</v>
       </c>
     </row>
-    <row r="474" spans="1:3" outlineLevel="1">
-      <c r="B474" t="str">
+    <row r="482" spans="1:3" outlineLevel="1">
+      <c r="B482" t="str">
         <f>'Versioni EJB'!B26</f>
         <v>filialevirtuale-ejb</v>
       </c>
-      <c r="C474" t="str">
+      <c r="C482" t="str">
         <f>'Versioni EJB'!C26</f>
         <v>1.75.0</v>
-      </c>
-    </row>
-    <row r="475" spans="1:3" outlineLevel="1">
-      <c r="B475" t="str">
-        <f>'Versioni EJB'!B16</f>
-        <v>profilocliente-ejb</v>
-      </c>
-      <c r="C475" t="str">
-        <f>'Versioni EJB'!C16</f>
-        <v>1.101.0</v>
-      </c>
-    </row>
-    <row r="476" spans="1:3" outlineLevel="1">
-      <c r="B476" t="str">
-        <f>'Versioni EJB'!B2</f>
-        <v>isp-ib-om</v>
-      </c>
-      <c r="C476" t="str">
-        <f>'Versioni EJB'!C2</f>
-        <v>1.21.0</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" outlineLevel="1">
-      <c r="B477" t="str">
-        <f>'Versioni EJB'!B4</f>
-        <v>banca-ejb</v>
-      </c>
-      <c r="C477" t="str">
-        <f>'Versioni EJB'!C4</f>
-        <v>1.15.0</v>
-      </c>
-    </row>
-    <row r="478" spans="1:3" outlineLevel="1">
-      <c r="B478" t="str">
-        <f>'Versioni EJB'!B95</f>
-        <v>miogestore-ejb</v>
-      </c>
-      <c r="C478" t="str">
-        <f>'Versioni EJB'!C95</f>
-        <v>1.149.0</v>
-      </c>
-    </row>
-    <row r="479" spans="1:3">
-      <c r="A479" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B479" s="2"/>
-      <c r="C479" s="2"/>
-    </row>
-    <row r="480" spans="1:3" outlineLevel="1">
-      <c r="B480" t="str">
-        <f>'Versioni EJB'!B95</f>
-        <v>miogestore-ejb</v>
-      </c>
-      <c r="C480" t="str">
-        <f>'Versioni EJB'!C95</f>
-        <v>1.149.0</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" outlineLevel="1">
-      <c r="B481" t="str">
-        <f>'Versioni EJB'!B13</f>
-        <v>notification-ejb</v>
-      </c>
-      <c r="C481" t="str">
-        <f>'Versioni EJB'!C13</f>
-        <v>1.59.0</v>
-      </c>
-    </row>
-    <row r="482" spans="1:3" outlineLevel="1">
-      <c r="B482" t="str">
-        <f>'Versioni EJB'!B39</f>
-        <v>saldo-ejb</v>
-      </c>
-      <c r="C482" t="str">
-        <f>'Versioni EJB'!C39</f>
-        <v>1.28.0</v>
       </c>
     </row>
     <row r="483" spans="1:3" outlineLevel="1">
@@ -7573,457 +7623,534 @@
     </row>
     <row r="484" spans="1:3" outlineLevel="1">
       <c r="B484" t="str">
+        <f>'Versioni EJB'!B2</f>
+        <v>isp-ib-om</v>
+      </c>
+      <c r="C484" t="str">
+        <f>'Versioni EJB'!C2</f>
+        <v>1.21.0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" outlineLevel="1">
+      <c r="B485" t="str">
+        <f>'Versioni EJB'!B4</f>
+        <v>banca-ejb</v>
+      </c>
+      <c r="C485" t="str">
+        <f>'Versioni EJB'!C4</f>
+        <v>1.15.0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" outlineLevel="1">
+      <c r="B486" t="str">
+        <f>'Versioni EJB'!B95</f>
+        <v>miogestore-ejb</v>
+      </c>
+      <c r="C486" t="str">
+        <f>'Versioni EJB'!C95</f>
+        <v>1.149.0</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3">
+      <c r="A487" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B487" s="2"/>
+      <c r="C487" s="2"/>
+    </row>
+    <row r="488" spans="1:3" outlineLevel="1">
+      <c r="B488" t="str">
+        <f>'Versioni EJB'!B95</f>
+        <v>miogestore-ejb</v>
+      </c>
+      <c r="C488" t="str">
+        <f>'Versioni EJB'!C95</f>
+        <v>1.149.0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" outlineLevel="1">
+      <c r="B489" t="str">
+        <f>'Versioni EJB'!B13</f>
+        <v>notification-ejb</v>
+      </c>
+      <c r="C489" t="str">
+        <f>'Versioni EJB'!C13</f>
+        <v>1.59.0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" outlineLevel="1">
+      <c r="B490" t="str">
+        <f>'Versioni EJB'!B39</f>
+        <v>saldo-ejb</v>
+      </c>
+      <c r="C490" t="str">
+        <f>'Versioni EJB'!C39</f>
+        <v>1.28.0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" outlineLevel="1">
+      <c r="B491" t="str">
+        <f>'Versioni EJB'!B16</f>
+        <v>profilocliente-ejb</v>
+      </c>
+      <c r="C491" t="str">
+        <f>'Versioni EJB'!C16</f>
+        <v>1.101.0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" outlineLevel="1">
+      <c r="B492" t="str">
         <f>'Versioni EJB'!B57</f>
         <v>interactiondb-ejb</v>
       </c>
-      <c r="C484" t="str">
+      <c r="C492" t="str">
         <f>'Versioni EJB'!C57</f>
         <v>1.26.0</v>
       </c>
     </row>
-    <row r="485" spans="1:3">
-      <c r="A485" s="11" t="s">
+    <row r="493" spans="1:3">
+      <c r="A493" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B485" s="11"/>
-      <c r="C485" s="11"/>
-    </row>
-    <row r="486" spans="1:3">
-      <c r="A486" s="2" t="s">
+      <c r="B493" s="11"/>
+      <c r="C493" s="11"/>
+    </row>
+    <row r="494" spans="1:3">
+      <c r="A494" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B486" s="2"/>
-      <c r="C486" s="2"/>
-    </row>
-    <row r="487" spans="1:3" outlineLevel="1">
-      <c r="B487" t="str">
+      <c r="B494" s="2"/>
+      <c r="C494" s="2"/>
+    </row>
+    <row r="495" spans="1:3" outlineLevel="1">
+      <c r="B495" t="str">
         <f>'Versioni EJB'!B86</f>
         <v>nfc-ejb</v>
       </c>
-      <c r="C487" t="str">
+      <c r="C495" t="str">
         <f>'Versioni EJB'!C86</f>
         <v>1.56.0</v>
       </c>
     </row>
-    <row r="488" spans="1:3" outlineLevel="1">
-      <c r="B488" t="str">
+    <row r="496" spans="1:3" outlineLevel="1">
+      <c r="B496" t="str">
         <f>'Versioni EJB'!B85</f>
         <v>masterpass-ejb</v>
       </c>
-      <c r="C488" t="str">
+      <c r="C496" t="str">
         <f>'Versioni EJB'!C85</f>
         <v>1.48.0</v>
       </c>
     </row>
-    <row r="489" spans="1:3" outlineLevel="1">
-      <c r="B489" t="str">
+    <row r="497" spans="1:3" outlineLevel="1">
+      <c r="B497" t="str">
         <f>'Versioni EJB'!B31</f>
         <v>jiffy-v2-ejb</v>
       </c>
-      <c r="C489" t="str">
+      <c r="C497" t="str">
         <f>'Versioni EJB'!C31</f>
         <v>1.22.0</v>
       </c>
     </row>
-    <row r="490" spans="1:3" outlineLevel="1">
-      <c r="B490" t="str">
+    <row r="498" spans="1:3" outlineLevel="1">
+      <c r="B498" t="str">
         <f>'Versioni EJB'!B66</f>
         <v>matchingidbpfm-ejb</v>
       </c>
-      <c r="C490" t="str">
+      <c r="C498" t="str">
         <f>'Versioni EJB'!C66</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="491" spans="1:3" outlineLevel="1">
-      <c r="B491" t="str">
+    <row r="499" spans="1:3" outlineLevel="1">
+      <c r="B499" t="str">
         <f>'Versioni EJB'!B82</f>
         <v>applepay-ejb</v>
       </c>
-      <c r="C491" t="str">
+      <c r="C499" t="str">
         <f>'Versioni EJB'!C82</f>
         <v>1.20.0</v>
       </c>
     </row>
-    <row r="492" spans="1:3" outlineLevel="1">
-      <c r="B492" t="str">
+    <row r="500" spans="1:3" outlineLevel="1">
+      <c r="B500" t="str">
         <f>'Versioni EJB'!B28</f>
         <v>gestorelimiti-ejb</v>
       </c>
-      <c r="C492" t="str">
+      <c r="C500" t="str">
         <f>'Versioni EJB'!C28</f>
         <v>1.17.0</v>
       </c>
     </row>
-    <row r="493" spans="1:3" outlineLevel="1">
-      <c r="B493" t="str">
+    <row r="501" spans="1:3" outlineLevel="1">
+      <c r="B501" t="str">
         <f>'Versioni EJB'!B63</f>
         <v>bustine-ejb</v>
       </c>
-      <c r="C493" t="str">
+      <c r="C501" t="str">
         <f>'Versioni EJB'!C63</f>
         <v>1.14.0</v>
       </c>
     </row>
-    <row r="494" spans="1:3" outlineLevel="1">
-      <c r="B494" t="str">
-        <f>'Versioni EJB'!B102</f>
+    <row r="502" spans="1:3" outlineLevel="1">
+      <c r="B502" t="str">
+        <f>'Versioni EJB'!B103</f>
         <v>proposte-ejb</v>
       </c>
-      <c r="C494" t="str">
-        <f>'Versioni EJB'!C102</f>
+      <c r="C502" t="str">
+        <f>'Versioni EJB'!C103</f>
         <v>1.13.0</v>
       </c>
     </row>
-    <row r="495" spans="1:3" outlineLevel="1">
-      <c r="B495" t="str">
+    <row r="503" spans="1:3" outlineLevel="1">
+      <c r="B503" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
       </c>
-      <c r="C495" t="str">
+      <c r="C503" t="str">
         <f>'Versioni EJB'!C39</f>
         <v>1.28.0</v>
       </c>
     </row>
-    <row r="496" spans="1:3" outlineLevel="1">
-      <c r="B496" t="str">
+    <row r="504" spans="1:3" outlineLevel="1">
+      <c r="B504" t="str">
         <f>'Versioni EJB'!B46</f>
         <v>pfm-ejb</v>
       </c>
-      <c r="C496" t="str">
+      <c r="C504" t="str">
         <f>'Versioni EJB'!C46</f>
         <v>1.29.0</v>
       </c>
     </row>
-    <row r="497" spans="1:3" outlineLevel="1">
-      <c r="B497" t="str">
+    <row r="505" spans="1:3" outlineLevel="1">
+      <c r="B505" t="str">
         <f>'Versioni EJB'!B78</f>
         <v>carte-ejb</v>
       </c>
-      <c r="C497" t="str">
+      <c r="C505" t="str">
         <f>'Versioni EJB'!C78</f>
         <v>1.39.0</v>
       </c>
     </row>
-    <row r="498" spans="1:3" outlineLevel="1">
-      <c r="B498" t="str">
+    <row r="506" spans="1:3" outlineLevel="1">
+      <c r="B506" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C498" t="str">
+      <c r="C506" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="499" spans="1:3" outlineLevel="1">
-      <c r="B499" t="str">
+    <row r="507" spans="1:3" outlineLevel="1">
+      <c r="B507" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
       </c>
-      <c r="C499" t="str">
+      <c r="C507" t="str">
         <f>'Versioni EJB'!C2</f>
         <v>1.21.0</v>
       </c>
     </row>
-    <row r="500" spans="1:3">
-      <c r="A500" s="2" t="s">
+    <row r="508" spans="1:3">
+      <c r="A508" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B500" s="2"/>
-      <c r="C500" s="2"/>
-    </row>
-    <row r="501" spans="1:3" outlineLevel="1">
-      <c r="B501" t="str">
-        <f>'Versioni EJB'!B100</f>
+      <c r="B508" s="2"/>
+      <c r="C508" s="2"/>
+    </row>
+    <row r="509" spans="1:3" outlineLevel="1">
+      <c r="B509" t="str">
+        <f>'Versioni EJB'!B101</f>
         <v>globalposition-ejb</v>
       </c>
-      <c r="C501" t="str">
-        <f>'Versioni EJB'!C100</f>
+      <c r="C509" t="str">
+        <f>'Versioni EJB'!C101</f>
         <v>1.133.0</v>
       </c>
     </row>
-    <row r="502" spans="1:3" outlineLevel="1">
-      <c r="B502" t="str">
+    <row r="510" spans="1:3" outlineLevel="1">
+      <c r="B510" t="str">
         <f>'Versioni EJB'!B93</f>
         <v>comunicazioni-ejb</v>
       </c>
-      <c r="C502" t="str">
+      <c r="C510" t="str">
         <f>'Versioni EJB'!C93</f>
         <v>1.239.0</v>
       </c>
     </row>
-    <row r="503" spans="1:3" outlineLevel="1">
-      <c r="B503" t="str">
+    <row r="511" spans="1:3" outlineLevel="1">
+      <c r="B511" t="str">
         <f>'Versioni EJB'!B70</f>
         <v>bonifico-ejb</v>
       </c>
-      <c r="C503" t="str">
+      <c r="C511" t="str">
         <f>'Versioni EJB'!C70</f>
         <v>1.36.0</v>
       </c>
     </row>
-    <row r="504" spans="1:3" outlineLevel="1">
-      <c r="B504" t="str">
+    <row r="512" spans="1:3" outlineLevel="1">
+      <c r="B512" t="str">
         <f>'Versioni EJB'!B57</f>
         <v>interactiondb-ejb</v>
       </c>
-      <c r="C504" t="str">
+      <c r="C512" t="str">
         <f>'Versioni EJB'!C57</f>
         <v>1.26.0</v>
       </c>
     </row>
-    <row r="505" spans="1:3" outlineLevel="1">
-      <c r="B505" t="str">
+    <row r="513" spans="1:3" outlineLevel="1">
+      <c r="B513" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C505" t="str">
+      <c r="C513" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="506" spans="1:3" outlineLevel="1">
-      <c r="B506" t="str">
+    <row r="514" spans="1:3" outlineLevel="1">
+      <c r="B514" t="str">
         <f>'Versioni EJB'!B43</f>
         <v>commonssmallbusiness-ejb</v>
       </c>
-      <c r="C506" t="str">
+      <c r="C514" t="str">
         <f>'Versioni EJB'!C43</f>
         <v>1.16.0</v>
       </c>
     </row>
-    <row r="507" spans="1:3" outlineLevel="1">
-      <c r="B507" t="str">
+    <row r="515" spans="1:3" outlineLevel="1">
+      <c r="B515" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
       </c>
-      <c r="C507" t="str">
+      <c r="C515" t="str">
         <f>'Versioni EJB'!C39</f>
         <v>1.28.0</v>
       </c>
     </row>
-    <row r="508" spans="1:3">
-      <c r="A508" s="2" t="s">
+    <row r="516" spans="1:3">
+      <c r="A516" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B508" s="2"/>
-      <c r="C508" s="2"/>
-    </row>
-    <row r="509" spans="1:3" outlineLevel="1">
-      <c r="B509" t="str">
+      <c r="B516" s="2"/>
+      <c r="C516" s="2"/>
+    </row>
+    <row r="517" spans="1:3" outlineLevel="1">
+      <c r="B517" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
-      <c r="C509" t="str">
+      <c r="C517" t="str">
         <f>'Versioni EJB'!C4</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="510" spans="1:3" outlineLevel="1">
-      <c r="B510" t="str">
+    <row r="518" spans="1:3" outlineLevel="1">
+      <c r="B518" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
       </c>
-      <c r="C510" t="str">
+      <c r="C518" t="str">
         <f>'Versioni EJB'!C16</f>
         <v>1.101.0</v>
       </c>
     </row>
-    <row r="511" spans="1:3" outlineLevel="1">
-      <c r="B511" t="str">
-        <f>'Versioni EJB'!B100</f>
+    <row r="519" spans="1:3" outlineLevel="1">
+      <c r="B519" t="str">
+        <f>'Versioni EJB'!B101</f>
         <v>globalposition-ejb</v>
       </c>
-      <c r="C511" t="str">
-        <f>'Versioni EJB'!C100</f>
+      <c r="C519" t="str">
+        <f>'Versioni EJB'!C101</f>
         <v>1.133.0</v>
       </c>
     </row>
-    <row r="512" spans="1:3" outlineLevel="1">
-      <c r="B512" t="str">
+    <row r="520" spans="1:3" outlineLevel="1">
+      <c r="B520" t="str">
         <f>'Versioni EJB'!B33</f>
         <v>listiniinfofin-ejb</v>
       </c>
-      <c r="C512" t="str">
+      <c r="C520" t="str">
         <f>'Versioni EJB'!C33</f>
         <v>1.17.0</v>
       </c>
     </row>
-    <row r="513" spans="1:3">
-      <c r="A513" s="11" t="s">
+    <row r="521" spans="1:3">
+      <c r="A521" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B513" s="11"/>
-      <c r="C513" s="11"/>
-    </row>
-    <row r="514" spans="1:3">
-      <c r="A514" s="2" t="s">
+      <c r="B521" s="11"/>
+      <c r="C521" s="11"/>
+    </row>
+    <row r="522" spans="1:3">
+      <c r="A522" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B514" s="2"/>
-      <c r="C514" s="2"/>
-    </row>
-    <row r="515" spans="1:3" outlineLevel="1">
-      <c r="B515" t="str">
+      <c r="B522" s="2"/>
+      <c r="C522" s="2"/>
+    </row>
+    <row r="523" spans="1:3" outlineLevel="1">
+      <c r="B523" t="str">
         <f>'Versioni EJB'!B93</f>
         <v>comunicazioni-ejb</v>
       </c>
-      <c r="C515" t="str">
+      <c r="C523" t="str">
         <f>'Versioni EJB'!C93</f>
         <v>1.239.0</v>
       </c>
     </row>
-    <row r="516" spans="1:3" outlineLevel="1">
-      <c r="B516" t="str">
-        <f>'Versioni EJB'!B105</f>
+    <row r="524" spans="1:3" outlineLevel="1">
+      <c r="B524" t="str">
+        <f>'Versioni EJB'!B106</f>
         <v>pulsantiera-ejb</v>
       </c>
-      <c r="C516" t="str">
-        <f>'Versioni EJB'!C105</f>
+      <c r="C524" t="str">
+        <f>'Versioni EJB'!C106</f>
         <v>1.23.0</v>
       </c>
     </row>
-    <row r="517" spans="1:3" outlineLevel="1">
-      <c r="B517" t="str">
+    <row r="525" spans="1:3" outlineLevel="1">
+      <c r="B525" t="str">
         <f>'Versioni EJB'!B66</f>
         <v>matchingidbpfm-ejb</v>
       </c>
-      <c r="C517" t="str">
+      <c r="C525" t="str">
         <f>'Versioni EJB'!C66</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="518" spans="1:3" outlineLevel="1">
-      <c r="B518" t="str">
+    <row r="526" spans="1:3" outlineLevel="1">
+      <c r="B526" t="str">
         <f>'Versioni EJB'!B63</f>
         <v>bustine-ejb</v>
       </c>
-      <c r="C518" t="str">
+      <c r="C526" t="str">
         <f>'Versioni EJB'!C63</f>
         <v>1.14.0</v>
       </c>
     </row>
-    <row r="519" spans="1:3" outlineLevel="1">
-      <c r="B519" t="str">
+    <row r="527" spans="1:3" outlineLevel="1">
+      <c r="B527" t="str">
         <f>'Versioni EJB'!B38</f>
         <v>prestiti-ejb</v>
       </c>
-      <c r="C519" t="str">
+      <c r="C527" t="str">
         <f>'Versioni EJB'!C38</f>
         <v>1.19.0</v>
       </c>
     </row>
-    <row r="520" spans="1:3" outlineLevel="1">
-      <c r="B520" t="str">
-        <f>'Versioni EJB'!B102</f>
+    <row r="528" spans="1:3" outlineLevel="1">
+      <c r="B528" t="str">
+        <f>'Versioni EJB'!B103</f>
         <v>proposte-ejb</v>
       </c>
-      <c r="C520" t="str">
-        <f>'Versioni EJB'!C102</f>
+      <c r="C528" t="str">
+        <f>'Versioni EJB'!C103</f>
         <v>1.13.0</v>
       </c>
     </row>
-    <row r="521" spans="1:3" outlineLevel="1">
-      <c r="B521" t="str">
+    <row r="529" spans="1:3" outlineLevel="1">
+      <c r="B529" t="str">
         <f>'Versioni EJB'!B70</f>
         <v>bonifico-ejb</v>
       </c>
-      <c r="C521" t="str">
+      <c r="C529" t="str">
         <f>'Versioni EJB'!C70</f>
         <v>1.36.0</v>
       </c>
     </row>
-    <row r="522" spans="1:3" outlineLevel="1">
-      <c r="B522" t="str">
+    <row r="530" spans="1:3" outlineLevel="1">
+      <c r="B530" t="str">
         <f>'Versioni EJB'!B46</f>
         <v>pfm-ejb</v>
       </c>
-      <c r="C522" t="str">
+      <c r="C530" t="str">
         <f>'Versioni EJB'!C46</f>
         <v>1.29.0</v>
       </c>
     </row>
-    <row r="523" spans="1:3" outlineLevel="1">
-      <c r="B523" t="str">
+    <row r="531" spans="1:3" outlineLevel="1">
+      <c r="B531" t="str">
         <f>'Versioni EJB'!B19</f>
         <v>agenda-ejb</v>
       </c>
-      <c r="C523" t="str">
+      <c r="C531" t="str">
         <f>'Versioni EJB'!C19</f>
         <v>1.19.0</v>
       </c>
     </row>
-    <row r="524" spans="1:3" outlineLevel="1">
-      <c r="B524" t="str">
+    <row r="532" spans="1:3" outlineLevel="1">
+      <c r="B532" t="str">
         <f>'Versioni EJB'!B78</f>
         <v>carte-ejb</v>
       </c>
-      <c r="C524" t="str">
+      <c r="C532" t="str">
         <f>'Versioni EJB'!C78</f>
         <v>1.39.0</v>
       </c>
     </row>
-    <row r="525" spans="1:3" outlineLevel="1">
-      <c r="B525" t="str">
+    <row r="533" spans="1:3" outlineLevel="1">
+      <c r="B533" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
       </c>
-      <c r="C525" t="str">
+      <c r="C533" t="str">
         <f>'Versioni EJB'!C4</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="526" spans="1:3" outlineLevel="1">
-      <c r="B526" t="str">
+    <row r="534" spans="1:3" outlineLevel="1">
+      <c r="B534" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
       </c>
-      <c r="C526" t="str">
+      <c r="C534" t="str">
         <f>'Versioni EJB'!C39</f>
         <v>1.28.0</v>
       </c>
     </row>
-    <row r="527" spans="1:3">
-      <c r="A527" s="11" t="s">
+    <row r="535" spans="1:3">
+      <c r="A535" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B527" s="11"/>
-      <c r="C527" s="11"/>
-    </row>
-    <row r="528" spans="1:3">
-      <c r="A528" s="2" t="s">
+      <c r="B535" s="11"/>
+      <c r="C535" s="11"/>
+    </row>
+    <row r="536" spans="1:3">
+      <c r="A536" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B528" s="2"/>
-      <c r="C528" s="2"/>
-    </row>
-    <row r="529" spans="2:3" outlineLevel="1">
-      <c r="B529" t="str">
+      <c r="B536" s="2"/>
+      <c r="C536" s="2"/>
+    </row>
+    <row r="537" spans="1:3" outlineLevel="1">
+      <c r="B537" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
       </c>
-      <c r="C529" t="str">
+      <c r="C537" t="str">
         <f>'Versioni EJB'!C2</f>
         <v>1.21.0</v>
       </c>
     </row>
-    <row r="530" spans="2:3" outlineLevel="1">
-      <c r="B530" t="str">
+    <row r="538" spans="1:3" outlineLevel="1">
+      <c r="B538" t="str">
         <f>'Versioni EJB'!B66</f>
         <v>matchingidbpfm-ejb</v>
       </c>
-      <c r="C530" t="str">
+      <c r="C538" t="str">
         <f>'Versioni EJB'!C66</f>
         <v>1.15.0</v>
       </c>
     </row>
-    <row r="531" spans="2:3" outlineLevel="1">
-      <c r="B531" t="str">
-        <f>'Versioni EJB'!B108</f>
+    <row r="539" spans="1:3" outlineLevel="1">
+      <c r="B539" t="str">
+        <f>'Versioni EJB'!B109</f>
         <v>listaoperazioni-ejb</v>
       </c>
-      <c r="C531" t="str">
-        <f>'Versioni EJB'!C108</f>
+      <c r="C539" t="str">
+        <f>'Versioni EJB'!C109</f>
         <v>1.77.0</v>
       </c>
     </row>
@@ -8032,12 +8159,7 @@
     <sortCondition ref="B18"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="A260:C260"/>
-    <mergeCell ref="A312:C312"/>
-    <mergeCell ref="A351:C351"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A411:C411"/>
-    <mergeCell ref="A527:C527"/>
+    <mergeCell ref="A535:C535"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A26:C26"/>
@@ -8051,8 +8173,13 @@
     <mergeCell ref="A192:C192"/>
     <mergeCell ref="A425:C425"/>
     <mergeCell ref="A433:C433"/>
-    <mergeCell ref="A485:C485"/>
-    <mergeCell ref="A513:C513"/>
+    <mergeCell ref="A493:C493"/>
+    <mergeCell ref="A521:C521"/>
+    <mergeCell ref="A260:C260"/>
+    <mergeCell ref="A312:C312"/>
+    <mergeCell ref="A351:C351"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A411:C411"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Sviluppo della nuova funzionalità per la verifica automatica delle versioni per le dipendenze nei POM degli EJB
</commit_message>
<xml_diff>
--- a/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
+++ b/src/main/resources/excelutils/Allineamento EJB in ambienti paralleli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Openshift\SoftwareAllineamenti\src\main\resources\excelutils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4827C26-3DF1-448D-84E6-B4F5D7041670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A63445-E44E-4FAB-9CF7-17D954B2A5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versioni EJB" sheetId="1" r:id="rId1"/>
@@ -894,9 +894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F111"/>
+      <selection pane="bottomLeft" activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3058,10 +3058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D539"/>
+  <dimension ref="A1:D540"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A521" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A440" sqref="A440"/>
     </sheetView>
   </sheetViews>
@@ -3681,7 +3681,7 @@
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
-    <row r="69" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="69" spans="1:3" outlineLevel="1">
       <c r="B69" t="s">
         <v>83</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="70" spans="1:3" outlineLevel="1">
       <c r="B70" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
@@ -3699,7 +3699,7 @@
         <v>1.61.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="71" spans="1:3" outlineLevel="1">
       <c r="B71" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
@@ -3709,7 +3709,7 @@
         <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="72" spans="1:3" outlineLevel="1">
       <c r="B72" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
@@ -3719,7 +3719,7 @@
         <v>1.105.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="73" spans="1:3" collapsed="1">
+    <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
         <v>28</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
     </row>
-    <row r="129" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="129" spans="1:3" outlineLevel="1">
       <c r="B129" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
@@ -4238,7 +4238,7 @@
         <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="130" spans="1:3" outlineLevel="1">
       <c r="B130" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
@@ -4248,7 +4248,7 @@
         <v>1.61.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="131" spans="1:3" outlineLevel="1">
       <c r="B131" t="s">
         <v>71</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="132" spans="1:3" outlineLevel="1">
       <c r="B132" t="str">
         <f>'Versioni EJB'!B12</f>
         <v>commons-ejb</v>
@@ -4266,7 +4266,7 @@
         <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="133" spans="1:3" outlineLevel="1">
       <c r="B133" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
@@ -4276,14 +4276,14 @@
         <v>1.105.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="134" spans="1:3" collapsed="1">
+    <row r="134" spans="1:3">
       <c r="A134" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="135" spans="1:3" outlineLevel="1">
       <c r="B135" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
@@ -4293,7 +4293,7 @@
         <v>1.105.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="136" spans="1:3" outlineLevel="1">
       <c r="B136" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
@@ -4303,7 +4303,7 @@
         <v>1.30.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="137" spans="1:3" collapsed="1">
+    <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
         <v>44</v>
       </c>
@@ -4377,7 +4377,7 @@
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
     </row>
-    <row r="145" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="145" spans="1:3" outlineLevel="1">
       <c r="B145" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
@@ -4387,7 +4387,7 @@
         <v>1.105.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="146" spans="1:3" outlineLevel="1">
       <c r="B146" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
@@ -4397,7 +4397,7 @@
         <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="147" spans="1:3" outlineLevel="1">
       <c r="B147" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
@@ -4407,7 +4407,7 @@
         <v>1.30.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="148" spans="1:3" outlineLevel="1">
       <c r="B148" t="s">
         <v>87</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="149" spans="1:3" outlineLevel="1">
       <c r="B149" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
@@ -4425,7 +4425,7 @@
         <v>1.61.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="150" spans="1:3" outlineLevel="1">
       <c r="B150" t="s">
         <v>61</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:3" collapsed="1">
+    <row r="151" spans="1:3">
       <c r="A151" s="2" t="s">
         <v>46</v>
       </c>
@@ -6912,7 +6912,7 @@
       <c r="B412" s="2"/>
       <c r="C412" s="2"/>
     </row>
-    <row r="413" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="413" spans="1:3" outlineLevel="1">
       <c r="B413" t="s">
         <v>83</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="414" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="414" spans="1:3" outlineLevel="1">
       <c r="B414" t="str">
         <f>'Versioni EJB'!B13</f>
         <v>notification-ejb</v>
@@ -6930,7 +6930,7 @@
         <v>1.61.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="415" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="415" spans="1:3" outlineLevel="1">
       <c r="B415" t="str">
         <f>'Versioni EJB'!B51</f>
         <v>etichette-ejb</v>
@@ -6940,7 +6940,7 @@
         <v>1.25.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="416" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="416" spans="1:3" outlineLevel="1">
       <c r="B416" t="str">
         <f>'Versioni EJB'!B91</f>
         <v>ricordamidi-ejb</v>
@@ -6950,7 +6950,7 @@
         <v>1.30.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="417" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="417" spans="1:3" outlineLevel="1">
       <c r="B417" t="str">
         <f>'Versioni EJB'!B46</f>
         <v>pfm-ejb</v>
@@ -6960,7 +6960,7 @@
         <v>1.31.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="418" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="418" spans="1:3" outlineLevel="1">
       <c r="B418" t="str">
         <f>'Versioni EJB'!B26</f>
         <v>filialevirtuale-ejb</v>
@@ -6970,7 +6970,7 @@
         <v>1.83.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="419" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="419" spans="1:3" outlineLevel="1">
       <c r="B419" t="str">
         <f>'Versioni EJB'!B39</f>
         <v>saldo-ejb</v>
@@ -6980,7 +6980,7 @@
         <v>1.30.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="420" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="420" spans="1:3" outlineLevel="1">
       <c r="B420" t="str">
         <f>'Versioni EJB'!B12</f>
         <v>commons-ejb</v>
@@ -6990,7 +6990,7 @@
         <v>1.20.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="421" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="421" spans="1:3" outlineLevel="1">
       <c r="B421" t="str">
         <f>'Versioni EJB'!B4</f>
         <v>banca-ejb</v>
@@ -7000,7 +7000,7 @@
         <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="422" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="422" spans="1:3" outlineLevel="1">
       <c r="B422" t="str">
         <f>'Versioni EJB'!B16</f>
         <v>profilocliente-ejb</v>
@@ -7010,7 +7010,7 @@
         <v>1.105.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="423" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="423" spans="1:3" outlineLevel="1">
       <c r="B423" t="str">
         <f>'Versioni EJB'!B9</f>
         <v>userpreferences-ejb</v>
@@ -7020,7 +7020,7 @@
         <v>1.18.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="424" spans="1:3" hidden="1" outlineLevel="1">
+    <row r="424" spans="1:3" outlineLevel="1">
       <c r="B424" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
@@ -7030,7 +7030,7 @@
         <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="425" spans="1:3" collapsed="1">
+    <row r="425" spans="1:3">
       <c r="A425" s="15" t="s">
         <v>115</v>
       </c>
@@ -8103,7 +8103,7 @@
       <c r="B536" s="2"/>
       <c r="C536" s="2"/>
     </row>
-    <row r="537" spans="1:3" outlineLevel="1">
+    <row r="537" spans="1:3" hidden="1" outlineLevel="1">
       <c r="B537" t="str">
         <f>'Versioni EJB'!B2</f>
         <v>isp-ib-om</v>
@@ -8113,7 +8113,7 @@
         <v>1.23.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="538" spans="1:3" outlineLevel="1">
+    <row r="538" spans="1:3" hidden="1" outlineLevel="1">
       <c r="B538" t="str">
         <f>'Versioni EJB'!B66</f>
         <v>matchingidbpfm-ejb</v>
@@ -8123,7 +8123,7 @@
         <v>1.17.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
-    <row r="539" spans="1:3" outlineLevel="1">
+    <row r="539" spans="1:3" hidden="1" outlineLevel="1">
       <c r="B539" t="str">
         <f>'Versioni EJB'!B109</f>
         <v>listaoperazioni-ejb</v>
@@ -8133,6 +8133,7 @@
         <v>1.81.0-env-svis-SNAPSHOT</v>
       </c>
     </row>
+    <row r="540" spans="1:3" collapsed="1"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B18:C19">
     <sortCondition ref="B18"/>

</xml_diff>